<commit_message>
Se cambió la vista de Factura 3.0
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\OneDrive\Documentos\Trabajos Universidad\ModuloFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3281EB34-1D12-4FBC-BF05-4516B54DA19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443FC926-3E01-4FDB-A5E1-E09A35E80E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="1" xr2:uid="{D6C15466-4649-4A22-BCE7-3BF8AFBFC14E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{D6C15466-4649-4A22-BCE7-3BF8AFBFC14E}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="206">
   <si>
     <t>Telefono Casa</t>
   </si>
@@ -630,7 +630,31 @@
     <t>Semi-Modular</t>
   </si>
   <si>
-    <t>inventario</t>
+    <t>factura</t>
+  </si>
+  <si>
+    <t>nfac</t>
+  </si>
+  <si>
+    <t>idpago</t>
+  </si>
+  <si>
+    <t>idtipofac</t>
+  </si>
+  <si>
+    <t>idpersona</t>
+  </si>
+  <si>
+    <t>idTipopersona</t>
+  </si>
+  <si>
+    <t>codemple</t>
+  </si>
+  <si>
+    <t>fecha fac</t>
+  </si>
+  <si>
+    <t>valorfac</t>
   </si>
 </sst>
 </file>
@@ -695,13 +719,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3572,10 +3594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530204FE-A160-4075-98A7-610FC6631479}">
-  <dimension ref="B2:T111"/>
+  <dimension ref="B2:V112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="V99" sqref="V99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,13 +3659,13 @@
       <c r="N2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>97</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -3694,13 +3716,13 @@
       <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>99</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>117</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -3752,13 +3774,13 @@
       <c r="N4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="3" t="s">
         <v>101</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="3" t="s">
         <v>109</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -3809,13 +3831,13 @@
       <c r="N5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="3" t="s">
         <v>98</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -3861,19 +3883,19 @@
         <v>6</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M12" si="1">M5+1</f>
+        <f t="shared" ref="M6" si="1">M5+1</f>
         <v>1234567901</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="3" t="s">
         <v>100</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="3" t="s">
         <v>110</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -3924,13 +3946,13 @@
       <c r="N7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3" t="s">
         <v>107</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="3" t="s">
         <v>111</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -3976,19 +3998,19 @@
         <v>6</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M12" si="2">M7+1</f>
+        <f t="shared" ref="M8" si="2">M7+1</f>
         <v>1234567902</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>106</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>112</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -4039,13 +4061,13 @@
       <c r="N9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>105</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="3" t="s">
         <v>113</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -4091,19 +4113,19 @@
         <v>6</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M12" si="3">M9+1</f>
+        <f t="shared" ref="M10" si="3">M9+1</f>
         <v>1234567903</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="3" t="s">
         <v>104</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="3" t="s">
         <v>114</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -4154,13 +4176,13 @@
       <c r="N11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="3" t="s">
         <v>103</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="Q11" s="3" t="s">
         <v>115</v>
       </c>
       <c r="R11" s="1" t="s">
@@ -4212,13 +4234,13 @@
       <c r="N12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="3" t="s">
         <v>102</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="3" t="s">
         <v>116</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -4262,13 +4284,13 @@
       <c r="J14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>97</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="3" t="s">
         <v>119</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -4306,7 +4328,7 @@
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>99</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -4351,7 +4373,7 @@
       <c r="J16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>101</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -4396,7 +4418,7 @@
       <c r="J17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>98</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -4441,7 +4463,7 @@
       <c r="J18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3" t="s">
         <v>100</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -4486,7 +4508,7 @@
       <c r="J19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="3" t="s">
         <v>107</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -4531,7 +4553,7 @@
       <c r="J20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="3" t="s">
         <v>106</v>
       </c>
       <c r="L20" s="1" t="s">
@@ -4576,7 +4598,7 @@
       <c r="J21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="3" t="s">
         <v>105</v>
       </c>
       <c r="L21" s="1" t="s">
@@ -4621,7 +4643,7 @@
       <c r="J22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="3" t="s">
         <v>104</v>
       </c>
       <c r="L22" s="1" t="s">
@@ -4666,7 +4688,7 @@
       <c r="J23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="3" t="s">
         <v>103</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -4711,7 +4733,7 @@
       <c r="J24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="3" t="s">
         <v>102</v>
       </c>
       <c r="L24" s="1" t="s">
@@ -4768,13 +4790,13 @@
       <c r="N26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O26" s="4" t="s">
+      <c r="O26" s="3" t="s">
         <v>99</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q26" s="1">
         <v>60000001</v>
       </c>
       <c r="R26" s="1" t="s">
@@ -4813,7 +4835,7 @@
       <c r="J27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="3" t="s">
         <v>134</v>
       </c>
       <c r="L27" s="1" t="s">
@@ -4825,13 +4847,13 @@
       <c r="N27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="O27" s="3" t="s">
         <v>101</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27">
         <f>Q26+1</f>
         <v>60000002</v>
       </c>
@@ -4871,7 +4893,7 @@
       <c r="J28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="3" t="s">
         <v>135</v>
       </c>
       <c r="L28" s="1" t="s">
@@ -4883,13 +4905,13 @@
       <c r="N28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O28" s="4" t="s">
+      <c r="O28" s="3" t="s">
         <v>98</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28">
         <f t="shared" ref="Q28:Q29" si="7">Q27+1</f>
         <v>60000003</v>
       </c>
@@ -4929,7 +4951,7 @@
       <c r="J29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="3" t="s">
         <v>136</v>
       </c>
       <c r="L29" s="1" t="s">
@@ -4941,13 +4963,13 @@
       <c r="N29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O29" s="4" t="s">
+      <c r="O29" s="3" t="s">
         <v>100</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="Q29">
         <f t="shared" si="7"/>
         <v>60000004</v>
       </c>
@@ -4963,7 +4985,7 @@
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="1"/>
       <c r="M30" s="2"/>
       <c r="N30" s="1"/>
@@ -6424,7 +6446,7 @@
       <c r="L66" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M66" s="6" t="s">
+      <c r="M66" s="4" t="s">
         <v>172</v>
       </c>
       <c r="N66" s="1" t="s">
@@ -6469,7 +6491,7 @@
       <c r="L67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M67" s="6" t="s">
+      <c r="M67" s="4" t="s">
         <v>171</v>
       </c>
       <c r="N67" s="1" t="s">
@@ -6559,7 +6581,7 @@
       <c r="L69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M69" s="6">
+      <c r="M69" s="4">
         <v>3200</v>
       </c>
       <c r="N69" s="1" t="s">
@@ -6604,7 +6626,7 @@
       <c r="L70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M70" s="7" t="s">
+      <c r="M70" s="5" t="s">
         <v>173</v>
       </c>
       <c r="N70" s="1" t="s">
@@ -6694,7 +6716,7 @@
       <c r="L72" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M72" s="6" t="s">
+      <c r="M72" s="4" t="s">
         <v>175</v>
       </c>
       <c r="N72" s="1" t="s">
@@ -6739,7 +6761,7 @@
       <c r="L73" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M73" s="6" t="s">
+      <c r="M73" s="4" t="s">
         <v>171</v>
       </c>
       <c r="N73" s="1" t="s">
@@ -6829,7 +6851,7 @@
       <c r="L75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M75" s="6">
+      <c r="M75" s="4">
         <v>3600</v>
       </c>
       <c r="N75" s="1" t="s">
@@ -6874,7 +6896,7 @@
       <c r="L76" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M76" s="7" t="s">
+      <c r="M76" s="5" t="s">
         <v>176</v>
       </c>
       <c r="N76" s="1" t="s">
@@ -6964,7 +6986,7 @@
       <c r="L78" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M78" s="6" t="s">
+      <c r="M78" s="4" t="s">
         <v>182</v>
       </c>
       <c r="N78" s="1" t="s">
@@ -7016,7 +7038,7 @@
         <v>7</v>
       </c>
       <c r="P79" t="str">
-        <f t="shared" ref="P79:P111" si="14">_xlfn.CONCAT(B79:N79)</f>
+        <f t="shared" ref="P79:P93" si="14">_xlfn.CONCAT(B79:N79)</f>
         <v>insert into refcarac values ('35','9',NULL,'1','HDD');</v>
       </c>
     </row>
@@ -7065,7 +7087,7 @@
         <v>insert into refcarac values ('36','9','19','3','7200');</v>
       </c>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>29</v>
       </c>
@@ -7110,7 +7132,7 @@
         <v>insert into refcarac values ('37','9','6','4','3');</v>
       </c>
     </row>
-    <row r="82" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>29</v>
       </c>
@@ -7144,7 +7166,7 @@
       <c r="L82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M82" s="6" t="s">
+      <c r="M82" s="4" t="s">
         <v>186</v>
       </c>
       <c r="N82" s="1" t="s">
@@ -7155,7 +7177,7 @@
         <v>insert into refcarac values ('38','9',NULL,'11','SATA 6 Gb/s');</v>
       </c>
     </row>
-    <row r="83" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>29</v>
       </c>
@@ -7189,7 +7211,7 @@
       <c r="L83" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M83" s="6" t="s">
+      <c r="M83" s="4" t="s">
         <v>187</v>
       </c>
       <c r="N83" s="1" t="s">
@@ -7200,7 +7222,7 @@
         <v>insert into refcarac values ('39','10',NULL,'2','Samsung ');</v>
       </c>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>29</v>
       </c>
@@ -7245,7 +7267,7 @@
         <v>insert into refcarac values ('40','10',NULL,'1','SDD');</v>
       </c>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>29</v>
       </c>
@@ -7290,7 +7312,7 @@
         <v>insert into refcarac values ('41','10','21','3','2500');</v>
       </c>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>29</v>
       </c>
@@ -7335,7 +7357,7 @@
         <v>insert into refcarac values ('42','10','5','4','250');</v>
       </c>
     </row>
-    <row r="87" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>29</v>
       </c>
@@ -7369,7 +7391,7 @@
       <c r="L87" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M87" s="6" t="s">
+      <c r="M87" s="4" t="s">
         <v>190</v>
       </c>
       <c r="N87" s="1" t="s">
@@ -7380,7 +7402,7 @@
         <v>insert into refcarac values ('43','10',NULL,'11','PCIe 3.0 x4');</v>
       </c>
     </row>
-    <row r="88" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>29</v>
       </c>
@@ -7414,7 +7436,7 @@
       <c r="L88" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M88" s="6" t="s">
+      <c r="M88" s="4" t="s">
         <v>191</v>
       </c>
       <c r="N88" s="1" t="s">
@@ -7425,7 +7447,7 @@
         <v>insert into refcarac values ('44','11',NULL,'2','EVGA ');</v>
       </c>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>29</v>
       </c>
@@ -7470,7 +7492,7 @@
         <v>insert into refcarac values ('45','11',NULL,'1','Modular');</v>
       </c>
     </row>
-    <row r="90" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>29</v>
       </c>
@@ -7504,7 +7526,7 @@
       <c r="L90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M90" s="6" t="s">
+      <c r="M90" s="4" t="s">
         <v>193</v>
       </c>
       <c r="N90" s="1" t="s">
@@ -7515,7 +7537,7 @@
         <v>insert into refcarac values ('46','11',NULL,'5','1x 24-pin, 1x 8-pin (CPU)');</v>
       </c>
     </row>
-    <row r="91" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>29</v>
       </c>
@@ -7549,7 +7571,7 @@
       <c r="L91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M91" s="6" t="s">
+      <c r="M91" s="4" t="s">
         <v>195</v>
       </c>
       <c r="N91" s="1" t="s">
@@ -7560,7 +7582,7 @@
         <v>insert into refcarac values ('47','12',NULL,'2','Seasonic  ');</v>
       </c>
     </row>
-    <row r="92" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>29</v>
       </c>
@@ -7594,7 +7616,7 @@
       <c r="L92" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M92" s="6" t="s">
+      <c r="M92" s="4" t="s">
         <v>196</v>
       </c>
       <c r="N92" s="1" t="s">
@@ -7605,7 +7627,7 @@
         <v>insert into refcarac values ('48','12',NULL,'1','Semi-Modular');</v>
       </c>
     </row>
-    <row r="93" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>29</v>
       </c>
@@ -7639,7 +7661,7 @@
       <c r="L93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M93" s="6" t="s">
+      <c r="M93" s="4" t="s">
         <v>194</v>
       </c>
       <c r="N93" s="1" t="s">
@@ -7650,35 +7672,88 @@
         <v>insert into refcarac values ('49','12',NULL,'5','4x PCIe 8-pin');</v>
       </c>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
       <c r="F94" s="1"/>
       <c r="H94" s="1"/>
       <c r="J94" s="1"/>
       <c r="L94" s="1"/>
+      <c r="M94" s="4"/>
       <c r="N94" s="1"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>29</v>
-      </c>
-      <c r="C95" t="s">
+    <row r="95" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E95" t="s">
+        <v>198</v>
+      </c>
+      <c r="F95" s="1"/>
+      <c r="G95" t="s">
+        <v>199</v>
+      </c>
+      <c r="H95" s="1"/>
+      <c r="I95" t="s">
+        <v>200</v>
+      </c>
+      <c r="J95" s="1"/>
+      <c r="K95" t="s">
+        <v>201</v>
+      </c>
+      <c r="L95" s="1"/>
+      <c r="M95" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="N95" s="1"/>
+      <c r="O95" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S95" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="96" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
         <v>197</v>
       </c>
-      <c r="D95" t="s">
-        <v>9</v>
-      </c>
-      <c r="F95" s="1"/>
-      <c r="H95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="L95" s="1"/>
-      <c r="N95" s="1"/>
-    </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F96" s="1"/>
-      <c r="H96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="L96" s="1"/>
-      <c r="N96" s="1"/>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96">
+        <v>51</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G96">
+        <v>14</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V96" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="97" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
@@ -7785,6 +7860,13 @@
       <c r="L111" s="1"/>
       <c r="N111" s="1"/>
     </row>
+    <row r="112" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="N112" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se actualizo estructura  y datos de la BD
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\OneDrive\Documentos\Trabajos Universidad\ModuloFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443FC926-3E01-4FDB-A5E1-E09A35E80E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9F806B-E936-4CB3-8519-DF795E2316C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{D6C15466-4649-4A22-BCE7-3BF8AFBFC14E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="224">
   <si>
     <t>Telefono Casa</t>
   </si>
@@ -655,6 +655,60 @@
   </si>
   <si>
     <t>valorfac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert into  </t>
+  </si>
+  <si>
+    <t>20/10/2023</t>
+  </si>
+  <si>
+    <t>inventario</t>
+  </si>
+  <si>
+    <t>noinven</t>
+  </si>
+  <si>
+    <t>IDEVENTO</t>
+  </si>
+  <si>
+    <t>FCHEVE</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>IDREF</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>ensamble</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>detalleensamble</t>
+  </si>
+  <si>
+    <t>ITEMEMS</t>
+  </si>
+  <si>
+    <t>CONSE</t>
+  </si>
+  <si>
+    <t>NO INVEN</t>
   </si>
 </sst>
 </file>
@@ -719,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -728,6 +782,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190975C7-0781-412E-A518-D2C14B20E49F}">
   <dimension ref="B2:K105"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
@@ -3594,10 +3650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530204FE-A160-4075-98A7-610FC6631479}">
-  <dimension ref="B2:V112"/>
+  <dimension ref="B2:Y172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="V99" sqref="V99"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="U158" sqref="U158:U172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,7 +3661,7 @@
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
     <col min="6" max="6" width="3.140625" customWidth="1"/>
     <col min="7" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
@@ -3614,9 +3670,10 @@
     <col min="13" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="2.85546875" customWidth="1"/>
     <col min="16" max="16" width="4" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
     <col min="18" max="18" width="2.85546875" customWidth="1"/>
     <col min="19" max="19" width="3.140625" customWidth="1"/>
+    <col min="23" max="23" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
@@ -7087,7 +7144,7 @@
         <v>insert into refcarac values ('36','9','19','3','7200');</v>
       </c>
     </row>
-    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>29</v>
       </c>
@@ -7132,7 +7189,7 @@
         <v>insert into refcarac values ('37','9','6','4','3');</v>
       </c>
     </row>
-    <row r="82" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>29</v>
       </c>
@@ -7177,7 +7234,7 @@
         <v>insert into refcarac values ('38','9',NULL,'11','SATA 6 Gb/s');</v>
       </c>
     </row>
-    <row r="83" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>29</v>
       </c>
@@ -7222,7 +7279,7 @@
         <v>insert into refcarac values ('39','10',NULL,'2','Samsung ');</v>
       </c>
     </row>
-    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>29</v>
       </c>
@@ -7267,7 +7324,7 @@
         <v>insert into refcarac values ('40','10',NULL,'1','SDD');</v>
       </c>
     </row>
-    <row r="85" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>29</v>
       </c>
@@ -7312,7 +7369,7 @@
         <v>insert into refcarac values ('41','10','21','3','2500');</v>
       </c>
     </row>
-    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>29</v>
       </c>
@@ -7357,7 +7414,7 @@
         <v>insert into refcarac values ('42','10','5','4','250');</v>
       </c>
     </row>
-    <row r="87" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>29</v>
       </c>
@@ -7402,7 +7459,7 @@
         <v>insert into refcarac values ('43','10',NULL,'11','PCIe 3.0 x4');</v>
       </c>
     </row>
-    <row r="88" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>29</v>
       </c>
@@ -7447,7 +7504,7 @@
         <v>insert into refcarac values ('44','11',NULL,'2','EVGA ');</v>
       </c>
     </row>
-    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>29</v>
       </c>
@@ -7492,7 +7549,7 @@
         <v>insert into refcarac values ('45','11',NULL,'1','Modular');</v>
       </c>
     </row>
-    <row r="90" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>29</v>
       </c>
@@ -7537,7 +7594,7 @@
         <v>insert into refcarac values ('46','11',NULL,'5','1x 24-pin, 1x 8-pin (CPU)');</v>
       </c>
     </row>
-    <row r="91" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>29</v>
       </c>
@@ -7582,7 +7639,7 @@
         <v>insert into refcarac values ('47','12',NULL,'2','Seasonic  ');</v>
       </c>
     </row>
-    <row r="92" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>29</v>
       </c>
@@ -7627,7 +7684,7 @@
         <v>insert into refcarac values ('48','12',NULL,'1','Semi-Modular');</v>
       </c>
     </row>
-    <row r="93" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>29</v>
       </c>
@@ -7672,7 +7729,7 @@
         <v>insert into refcarac values ('49','12',NULL,'5','4x PCIe 8-pin');</v>
       </c>
     </row>
-    <row r="94" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="F94" s="1"/>
       <c r="H94" s="1"/>
       <c r="J94" s="1"/>
@@ -7680,7 +7737,7 @@
       <c r="M94" s="4"/>
       <c r="N94" s="1"/>
     </row>
-    <row r="95" spans="2:22" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:23" ht="17.25" x14ac:dyDescent="0.3">
       <c r="E95" t="s">
         <v>198</v>
       </c>
@@ -7711,9 +7768,9 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>8</v>
+        <v>206</v>
       </c>
       <c r="C96" t="s">
         <v>197</v>
@@ -7722,150 +7779,4084 @@
         <v>9</v>
       </c>
       <c r="E96">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G96">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="I96">
+        <v>2</v>
+      </c>
       <c r="J96" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="K96">
+        <v>601</v>
+      </c>
       <c r="L96" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
       <c r="N96" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="O96">
+        <v>301</v>
+      </c>
       <c r="P96" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="Q96" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="R96" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T96" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V96" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="U96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W96" t="str">
+        <f>_xlfn.CONCAT(B96:U96)</f>
+        <v>insert into  factura values ('1','4',2,'601','1','301','20/10/2023','','');</v>
+      </c>
+    </row>
+    <row r="97" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
       <c r="H97" s="1"/>
       <c r="J97" s="1"/>
       <c r="L97" s="1"/>
       <c r="N97" s="1"/>
     </row>
-    <row r="98" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F98" s="1"/>
       <c r="H98" s="1"/>
       <c r="J98" s="1"/>
       <c r="L98" s="1"/>
       <c r="N98" s="1"/>
     </row>
-    <row r="99" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F99" s="1"/>
       <c r="H99" s="1"/>
       <c r="J99" s="1"/>
       <c r="L99" s="1"/>
       <c r="N99" s="1"/>
     </row>
-    <row r="100" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>209</v>
+      </c>
       <c r="F100" s="1"/>
+      <c r="G100" t="s">
+        <v>198</v>
+      </c>
       <c r="H100" s="1"/>
+      <c r="I100" t="s">
+        <v>210</v>
+      </c>
       <c r="J100" s="1"/>
-      <c r="L100" s="1"/>
-      <c r="N100" s="1"/>
-    </row>
-    <row r="101" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F101" s="1"/>
-      <c r="H101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="N101" s="1"/>
-    </row>
-    <row r="102" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="N102" s="1"/>
-    </row>
-    <row r="103" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F103" s="1"/>
-      <c r="H103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="L103" s="1"/>
-      <c r="N103" s="1"/>
-    </row>
-    <row r="104" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="L104" s="1"/>
-      <c r="N104" s="1"/>
-    </row>
-    <row r="105" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F105" s="1"/>
-      <c r="H105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="L105" s="1"/>
-      <c r="N105" s="1"/>
-    </row>
-    <row r="106" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F106" s="1"/>
-      <c r="H106" s="1"/>
-      <c r="J106" s="1"/>
-      <c r="L106" s="1"/>
-      <c r="N106" s="1"/>
-    </row>
-    <row r="107" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F107" s="1"/>
-      <c r="H107" s="1"/>
-      <c r="J107" s="1"/>
-      <c r="L107" s="1"/>
-      <c r="N107" s="1"/>
-    </row>
-    <row r="108" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F108" s="1"/>
-      <c r="H108" s="1"/>
-      <c r="J108" s="1"/>
-      <c r="L108" s="1"/>
-      <c r="N108" s="1"/>
-    </row>
-    <row r="109" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="J109" s="1"/>
-      <c r="L109" s="1"/>
-      <c r="N109" s="1"/>
-    </row>
-    <row r="110" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="L110" s="1"/>
-      <c r="N110" s="1"/>
-    </row>
-    <row r="111" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F111" s="1"/>
-      <c r="H111" s="1"/>
-      <c r="J111" s="1"/>
-      <c r="L111" s="1"/>
-      <c r="N111" s="1"/>
-    </row>
-    <row r="112" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="L112" s="1"/>
-      <c r="N112" s="1"/>
+      <c r="K100" t="s">
+        <v>211</v>
+      </c>
+      <c r="P100" s="1"/>
+      <c r="Q100" t="s">
+        <v>212</v>
+      </c>
+      <c r="R100" s="1"/>
+      <c r="S100" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>206</v>
+      </c>
+      <c r="C101" t="s">
+        <v>208</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G101" t="s">
+        <v>163</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K101" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L101" t="s">
+        <v>215</v>
+      </c>
+      <c r="M101" s="6">
+        <v>10</v>
+      </c>
+      <c r="N101" t="s">
+        <v>215</v>
+      </c>
+      <c r="O101">
+        <v>2023</v>
+      </c>
+      <c r="P101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q101">
+        <v>40</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S101">
+        <v>1</v>
+      </c>
+      <c r="T101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U101" t="str">
+        <f>_xlfn.CONCAT(B101:T101)</f>
+        <v>insert into  inventario values ('1',NULL,'1','06/10/2023','40','1');</v>
+      </c>
+      <c r="Y101">
+        <f>Q101/10</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>206</v>
+      </c>
+      <c r="C102" t="s">
+        <v>208</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G102" t="s">
+        <v>163</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I102">
+        <v>2</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K102" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L102" t="s">
+        <v>215</v>
+      </c>
+      <c r="M102">
+        <v>11</v>
+      </c>
+      <c r="N102" t="s">
+        <v>215</v>
+      </c>
+      <c r="O102">
+        <v>2023</v>
+      </c>
+      <c r="P102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q102">
+        <v>42</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S102">
+        <v>1</v>
+      </c>
+      <c r="T102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U102" t="str">
+        <f t="shared" ref="U102:U148" si="15">_xlfn.CONCAT(B102:T102)</f>
+        <v>insert into  inventario values ('2',NULL,'2','06/11/2023','42','1');</v>
+      </c>
+      <c r="Y102">
+        <f t="shared" ref="Y102:Y148" si="16">Q102/10</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="103" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>206</v>
+      </c>
+      <c r="C103" t="s">
+        <v>208</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103">
+        <v>3</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G103" t="s">
+        <v>163</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I103">
+        <v>4</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K103" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L103" t="s">
+        <v>215</v>
+      </c>
+      <c r="M103" s="6">
+        <v>12</v>
+      </c>
+      <c r="N103" t="s">
+        <v>215</v>
+      </c>
+      <c r="O103">
+        <v>2023</v>
+      </c>
+      <c r="P103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q103">
+        <v>41</v>
+      </c>
+      <c r="R103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S103">
+        <v>1</v>
+      </c>
+      <c r="T103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U103" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('3',NULL,'4','06/12/2023','41','1');</v>
+      </c>
+      <c r="Y103">
+        <f t="shared" si="16"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" t="s">
+        <v>208</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104">
+        <v>4</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G104" t="s">
+        <v>163</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I104">
+        <v>5</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K104" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L104" t="s">
+        <v>215</v>
+      </c>
+      <c r="M104">
+        <v>13</v>
+      </c>
+      <c r="N104" t="s">
+        <v>215</v>
+      </c>
+      <c r="O104">
+        <v>2023</v>
+      </c>
+      <c r="P104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q104">
+        <v>40</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S104">
+        <v>1</v>
+      </c>
+      <c r="T104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U104" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('4',NULL,'5','06/13/2023','40','1');</v>
+      </c>
+      <c r="Y104">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>206</v>
+      </c>
+      <c r="C105" t="s">
+        <v>208</v>
+      </c>
+      <c r="D105" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105">
+        <v>5</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G105" t="s">
+        <v>163</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I105">
+        <v>6</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K105" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L105" t="s">
+        <v>215</v>
+      </c>
+      <c r="M105" s="6">
+        <v>14</v>
+      </c>
+      <c r="N105" t="s">
+        <v>215</v>
+      </c>
+      <c r="O105">
+        <v>2023</v>
+      </c>
+      <c r="P105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q105">
+        <v>35</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S105">
+        <v>2</v>
+      </c>
+      <c r="T105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U105" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('5',NULL,'6','06/14/2023','35','2');</v>
+      </c>
+      <c r="Y105">
+        <f t="shared" si="16"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="106" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>206</v>
+      </c>
+      <c r="C106" t="s">
+        <v>208</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106">
+        <v>6</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G106" t="s">
+        <v>163</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I106">
+        <v>1</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K106" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L106" t="s">
+        <v>215</v>
+      </c>
+      <c r="M106">
+        <v>15</v>
+      </c>
+      <c r="N106" t="s">
+        <v>215</v>
+      </c>
+      <c r="O106">
+        <v>2023</v>
+      </c>
+      <c r="P106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q106">
+        <v>37</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S106">
+        <v>2</v>
+      </c>
+      <c r="T106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U106" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('6',NULL,'1','06/15/2023','37','2');</v>
+      </c>
+      <c r="Y106">
+        <f t="shared" si="16"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="107" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>206</v>
+      </c>
+      <c r="C107" t="s">
+        <v>208</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107">
+        <v>7</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G107" t="s">
+        <v>163</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I107">
+        <v>2</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K107" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L107" t="s">
+        <v>215</v>
+      </c>
+      <c r="M107" s="6">
+        <v>16</v>
+      </c>
+      <c r="N107" t="s">
+        <v>215</v>
+      </c>
+      <c r="O107">
+        <v>2023</v>
+      </c>
+      <c r="P107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q107">
+        <v>36</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S107">
+        <v>2</v>
+      </c>
+      <c r="T107" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U107" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('7',NULL,'2','06/16/2023','36','2');</v>
+      </c>
+      <c r="Y107">
+        <f t="shared" si="16"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="108" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>206</v>
+      </c>
+      <c r="C108" t="s">
+        <v>208</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108">
+        <v>8</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G108" t="s">
+        <v>163</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I108">
+        <v>4</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K108" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L108" t="s">
+        <v>215</v>
+      </c>
+      <c r="M108">
+        <v>17</v>
+      </c>
+      <c r="N108" t="s">
+        <v>215</v>
+      </c>
+      <c r="O108">
+        <v>2023</v>
+      </c>
+      <c r="P108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q108">
+        <v>35</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S108">
+        <v>2</v>
+      </c>
+      <c r="T108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U108" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('8',NULL,'4','06/17/2023','35','2');</v>
+      </c>
+      <c r="Y108">
+        <f t="shared" si="16"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="109" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" t="s">
+        <v>208</v>
+      </c>
+      <c r="D109" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109">
+        <v>9</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G109" t="s">
+        <v>163</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I109">
+        <v>5</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L109" t="s">
+        <v>215</v>
+      </c>
+      <c r="M109" s="6">
+        <v>18</v>
+      </c>
+      <c r="N109" t="s">
+        <v>215</v>
+      </c>
+      <c r="O109">
+        <v>2023</v>
+      </c>
+      <c r="P109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q109">
+        <v>55</v>
+      </c>
+      <c r="R109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S109">
+        <v>3</v>
+      </c>
+      <c r="T109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U109" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('9',NULL,'5','06/18/2023','55','3');</v>
+      </c>
+      <c r="Y109">
+        <f t="shared" si="16"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="110" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>206</v>
+      </c>
+      <c r="C110" t="s">
+        <v>208</v>
+      </c>
+      <c r="D110" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110">
+        <v>10</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G110" t="s">
+        <v>163</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I110">
+        <v>6</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K110" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L110" t="s">
+        <v>215</v>
+      </c>
+      <c r="M110">
+        <v>19</v>
+      </c>
+      <c r="N110" t="s">
+        <v>215</v>
+      </c>
+      <c r="O110">
+        <v>2023</v>
+      </c>
+      <c r="P110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q110">
+        <v>57</v>
+      </c>
+      <c r="R110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S110">
+        <v>3</v>
+      </c>
+      <c r="T110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U110" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('10',NULL,'6','06/19/2023','57','3');</v>
+      </c>
+      <c r="Y110">
+        <f t="shared" si="16"/>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="111" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>206</v>
+      </c>
+      <c r="C111" t="s">
+        <v>208</v>
+      </c>
+      <c r="D111" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111">
+        <v>11</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G111" t="s">
+        <v>163</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I111">
+        <v>1</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L111" t="s">
+        <v>215</v>
+      </c>
+      <c r="M111" s="6">
+        <v>20</v>
+      </c>
+      <c r="N111" t="s">
+        <v>215</v>
+      </c>
+      <c r="O111">
+        <v>2023</v>
+      </c>
+      <c r="P111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q111">
+        <v>56</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S111">
+        <v>3</v>
+      </c>
+      <c r="T111" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U111" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('11',NULL,'1','06/20/2023','56','3');</v>
+      </c>
+      <c r="Y111">
+        <f t="shared" si="16"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>206</v>
+      </c>
+      <c r="C112" t="s">
+        <v>208</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112">
+        <v>12</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G112" t="s">
+        <v>163</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K112">
+        <f>K101+1</f>
+        <v>7</v>
+      </c>
+      <c r="L112" t="s">
+        <v>215</v>
+      </c>
+      <c r="M112" s="6">
+        <v>10</v>
+      </c>
+      <c r="N112" t="s">
+        <v>215</v>
+      </c>
+      <c r="O112">
+        <v>2023</v>
+      </c>
+      <c r="P112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q112">
+        <v>55</v>
+      </c>
+      <c r="R112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S112">
+        <v>3</v>
+      </c>
+      <c r="T112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U112" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('12',NULL,'1','7/10/2023','55','3');</v>
+      </c>
+      <c r="Y112">
+        <f t="shared" si="16"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="113" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>206</v>
+      </c>
+      <c r="C113" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113">
+        <v>13</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G113" t="s">
+        <v>163</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I113">
+        <v>2</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K113">
+        <f t="shared" ref="K113:K148" si="17">K102+1</f>
+        <v>7</v>
+      </c>
+      <c r="L113" t="s">
+        <v>215</v>
+      </c>
+      <c r="M113">
+        <v>11</v>
+      </c>
+      <c r="N113" t="s">
+        <v>215</v>
+      </c>
+      <c r="O113">
+        <v>2023</v>
+      </c>
+      <c r="P113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q113">
+        <v>80</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S113">
+        <f>S109+1</f>
+        <v>4</v>
+      </c>
+      <c r="T113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U113" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('13',NULL,'2','7/11/2023','80','4');</v>
+      </c>
+      <c r="Y113">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>206</v>
+      </c>
+      <c r="C114" t="s">
+        <v>208</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114">
+        <v>14</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G114" t="s">
+        <v>163</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I114">
+        <v>4</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L114" t="s">
+        <v>215</v>
+      </c>
+      <c r="M114" s="6">
+        <v>12</v>
+      </c>
+      <c r="N114" t="s">
+        <v>215</v>
+      </c>
+      <c r="O114">
+        <v>2023</v>
+      </c>
+      <c r="P114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q114">
+        <v>84</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S114">
+        <f>S110+1</f>
+        <v>4</v>
+      </c>
+      <c r="T114" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U114" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('14',NULL,'4','7/12/2023','84','4');</v>
+      </c>
+      <c r="Y114">
+        <f t="shared" si="16"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="115" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>206</v>
+      </c>
+      <c r="C115" t="s">
+        <v>208</v>
+      </c>
+      <c r="D115" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115">
+        <v>15</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G115" t="s">
+        <v>163</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I115">
+        <v>5</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K115">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L115" t="s">
+        <v>215</v>
+      </c>
+      <c r="M115">
+        <v>13</v>
+      </c>
+      <c r="N115" t="s">
+        <v>215</v>
+      </c>
+      <c r="O115">
+        <v>2023</v>
+      </c>
+      <c r="P115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q115">
+        <v>82</v>
+      </c>
+      <c r="R115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S115">
+        <f>S111+1</f>
+        <v>4</v>
+      </c>
+      <c r="T115" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U115" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('15',NULL,'5','7/13/2023','82','4');</v>
+      </c>
+      <c r="Y115">
+        <f t="shared" si="16"/>
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="116" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>206</v>
+      </c>
+      <c r="C116" t="s">
+        <v>208</v>
+      </c>
+      <c r="D116" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116">
+        <v>16</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G116" t="s">
+        <v>163</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I116">
+        <v>6</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K116">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L116" t="s">
+        <v>215</v>
+      </c>
+      <c r="M116" s="6">
+        <v>14</v>
+      </c>
+      <c r="N116" t="s">
+        <v>215</v>
+      </c>
+      <c r="O116">
+        <v>2023</v>
+      </c>
+      <c r="P116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q116">
+        <v>80</v>
+      </c>
+      <c r="R116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S116">
+        <f>S112+1</f>
+        <v>4</v>
+      </c>
+      <c r="T116" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U116" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('16',NULL,'6','7/14/2023','80','4');</v>
+      </c>
+      <c r="Y116">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>206</v>
+      </c>
+      <c r="C117" t="s">
+        <v>208</v>
+      </c>
+      <c r="D117" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117">
+        <v>17</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G117" t="s">
+        <v>163</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K117">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L117" t="s">
+        <v>215</v>
+      </c>
+      <c r="M117">
+        <v>15</v>
+      </c>
+      <c r="N117" t="s">
+        <v>215</v>
+      </c>
+      <c r="O117">
+        <v>2023</v>
+      </c>
+      <c r="P117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q117">
+        <v>70</v>
+      </c>
+      <c r="R117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S117">
+        <f>S113+1</f>
+        <v>5</v>
+      </c>
+      <c r="T117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U117" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('17',NULL,'1','7/15/2023','70','5');</v>
+      </c>
+      <c r="Y117">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>206</v>
+      </c>
+      <c r="C118" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118">
+        <v>18</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G118" t="s">
+        <v>163</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I118">
+        <v>2</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K118">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L118" t="s">
+        <v>215</v>
+      </c>
+      <c r="M118" s="6">
+        <v>16</v>
+      </c>
+      <c r="N118" t="s">
+        <v>215</v>
+      </c>
+      <c r="O118">
+        <v>2023</v>
+      </c>
+      <c r="P118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q118">
+        <v>74</v>
+      </c>
+      <c r="R118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S118">
+        <f>S114+1</f>
+        <v>5</v>
+      </c>
+      <c r="T118" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U118" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('18',NULL,'2','7/16/2023','74','5');</v>
+      </c>
+      <c r="Y118">
+        <f t="shared" si="16"/>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="119" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>206</v>
+      </c>
+      <c r="C119" t="s">
+        <v>208</v>
+      </c>
+      <c r="D119" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119">
+        <v>19</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G119" t="s">
+        <v>163</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I119">
+        <v>4</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L119" t="s">
+        <v>215</v>
+      </c>
+      <c r="M119">
+        <v>17</v>
+      </c>
+      <c r="N119" t="s">
+        <v>215</v>
+      </c>
+      <c r="O119">
+        <v>2023</v>
+      </c>
+      <c r="P119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q119">
+        <v>72</v>
+      </c>
+      <c r="R119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S119">
+        <f>S115+1</f>
+        <v>5</v>
+      </c>
+      <c r="T119" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U119" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('19',NULL,'4','7/17/2023','72','5');</v>
+      </c>
+      <c r="Y119">
+        <f t="shared" si="16"/>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="120" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>206</v>
+      </c>
+      <c r="C120" t="s">
+        <v>208</v>
+      </c>
+      <c r="D120" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120">
+        <v>20</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G120" t="s">
+        <v>163</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I120">
+        <v>5</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L120" t="s">
+        <v>215</v>
+      </c>
+      <c r="M120" s="6">
+        <v>18</v>
+      </c>
+      <c r="N120" t="s">
+        <v>215</v>
+      </c>
+      <c r="O120">
+        <v>2023</v>
+      </c>
+      <c r="P120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q120">
+        <v>70</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S120">
+        <f>S116+1</f>
+        <v>5</v>
+      </c>
+      <c r="T120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U120" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('20',NULL,'5','7/18/2023','70','5');</v>
+      </c>
+      <c r="Y120">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>206</v>
+      </c>
+      <c r="C121" t="s">
+        <v>208</v>
+      </c>
+      <c r="D121" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121">
+        <v>21</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G121" t="s">
+        <v>163</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I121">
+        <v>6</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L121" t="s">
+        <v>215</v>
+      </c>
+      <c r="M121">
+        <v>19</v>
+      </c>
+      <c r="N121" t="s">
+        <v>215</v>
+      </c>
+      <c r="O121">
+        <v>2023</v>
+      </c>
+      <c r="P121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q121">
+        <v>11</v>
+      </c>
+      <c r="R121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S121">
+        <f>S117+1</f>
+        <v>6</v>
+      </c>
+      <c r="T121" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U121" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('21',NULL,'6','7/19/2023','11','6');</v>
+      </c>
+      <c r="Y121">
+        <f>Q121/100</f>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="122" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>206</v>
+      </c>
+      <c r="C122" t="s">
+        <v>208</v>
+      </c>
+      <c r="D122" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122">
+        <v>22</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G122" t="s">
+        <v>163</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K122">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="L122" t="s">
+        <v>215</v>
+      </c>
+      <c r="M122" s="6">
+        <v>20</v>
+      </c>
+      <c r="N122" t="s">
+        <v>215</v>
+      </c>
+      <c r="O122">
+        <v>2023</v>
+      </c>
+      <c r="P122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q122">
+        <v>11</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S122">
+        <f>S118+1</f>
+        <v>6</v>
+      </c>
+      <c r="T122" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U122" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('22',NULL,'1','7/20/2023','11','6');</v>
+      </c>
+      <c r="Y122">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>206</v>
+      </c>
+      <c r="C123" t="s">
+        <v>208</v>
+      </c>
+      <c r="D123" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123">
+        <v>23</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G123" t="s">
+        <v>163</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I123">
+        <v>1</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K123">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L123" t="s">
+        <v>215</v>
+      </c>
+      <c r="M123" s="6">
+        <v>10</v>
+      </c>
+      <c r="N123" t="s">
+        <v>215</v>
+      </c>
+      <c r="O123">
+        <v>2023</v>
+      </c>
+      <c r="P123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q123">
+        <v>11</v>
+      </c>
+      <c r="R123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S123">
+        <f>S119+1</f>
+        <v>6</v>
+      </c>
+      <c r="T123" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U123" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('23',NULL,'1','8/10/2023','11','6');</v>
+      </c>
+      <c r="Y123">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>206</v>
+      </c>
+      <c r="C124" t="s">
+        <v>208</v>
+      </c>
+      <c r="D124" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124">
+        <v>24</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G124" t="s">
+        <v>163</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I124">
+        <v>2</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L124" t="s">
+        <v>215</v>
+      </c>
+      <c r="M124">
+        <v>11</v>
+      </c>
+      <c r="N124" t="s">
+        <v>215</v>
+      </c>
+      <c r="O124">
+        <v>2023</v>
+      </c>
+      <c r="P124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q124">
+        <v>11</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S124">
+        <f>S120+1</f>
+        <v>6</v>
+      </c>
+      <c r="T124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U124" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('24',NULL,'2','8/11/2023','11','6');</v>
+      </c>
+      <c r="Y124">
+        <f t="shared" ref="Y122:Y124" si="18">Q124/100</f>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="125" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>206</v>
+      </c>
+      <c r="C125" t="s">
+        <v>208</v>
+      </c>
+      <c r="D125" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125">
+        <v>25</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G125" t="s">
+        <v>163</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I125">
+        <v>4</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L125" t="s">
+        <v>215</v>
+      </c>
+      <c r="M125" s="6">
+        <v>12</v>
+      </c>
+      <c r="N125" t="s">
+        <v>215</v>
+      </c>
+      <c r="O125">
+        <v>2023</v>
+      </c>
+      <c r="P125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q125">
+        <v>20</v>
+      </c>
+      <c r="R125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S125">
+        <f>S121+1</f>
+        <v>7</v>
+      </c>
+      <c r="T125" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U125" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('25',NULL,'4','8/12/2023','20','7');</v>
+      </c>
+      <c r="Y125">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>206</v>
+      </c>
+      <c r="C126" t="s">
+        <v>208</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126">
+        <v>26</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G126" t="s">
+        <v>163</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I126">
+        <v>5</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L126" t="s">
+        <v>215</v>
+      </c>
+      <c r="M126">
+        <v>13</v>
+      </c>
+      <c r="N126" t="s">
+        <v>215</v>
+      </c>
+      <c r="O126">
+        <v>2023</v>
+      </c>
+      <c r="P126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q126">
+        <v>21</v>
+      </c>
+      <c r="R126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S126">
+        <f>S122+1</f>
+        <v>7</v>
+      </c>
+      <c r="T126" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U126" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('26',NULL,'5','8/13/2023','21','7');</v>
+      </c>
+      <c r="Y126">
+        <f t="shared" si="16"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>206</v>
+      </c>
+      <c r="C127" t="s">
+        <v>208</v>
+      </c>
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127">
+        <v>27</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G127" t="s">
+        <v>163</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I127">
+        <v>6</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L127" t="s">
+        <v>215</v>
+      </c>
+      <c r="M127" s="6">
+        <v>14</v>
+      </c>
+      <c r="N127" t="s">
+        <v>215</v>
+      </c>
+      <c r="O127">
+        <v>2023</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q127">
+        <v>20</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S127">
+        <f>S123+1</f>
+        <v>7</v>
+      </c>
+      <c r="T127" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U127" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('27',NULL,'6','8/14/2023','20','7');</v>
+      </c>
+      <c r="Y127">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>206</v>
+      </c>
+      <c r="C128" t="s">
+        <v>208</v>
+      </c>
+      <c r="D128" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128">
+        <v>28</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G128" t="s">
+        <v>163</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L128" t="s">
+        <v>215</v>
+      </c>
+      <c r="M128">
+        <v>15</v>
+      </c>
+      <c r="N128" t="s">
+        <v>215</v>
+      </c>
+      <c r="O128">
+        <v>2023</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q128">
+        <v>20</v>
+      </c>
+      <c r="R128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S128">
+        <f>S124+1</f>
+        <v>7</v>
+      </c>
+      <c r="T128" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U128" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('28',NULL,'1','8/15/2023','20','7');</v>
+      </c>
+      <c r="Y128">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>206</v>
+      </c>
+      <c r="C129" t="s">
+        <v>208</v>
+      </c>
+      <c r="D129" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129">
+        <v>29</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G129" t="s">
+        <v>163</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I129">
+        <v>2</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L129" t="s">
+        <v>215</v>
+      </c>
+      <c r="M129" s="6">
+        <v>16</v>
+      </c>
+      <c r="N129" t="s">
+        <v>215</v>
+      </c>
+      <c r="O129">
+        <v>2023</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q129">
+        <v>17</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S129">
+        <f>S125+1</f>
+        <v>8</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U129" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('29',NULL,'2','8/16/2023','17','8');</v>
+      </c>
+      <c r="Y129">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>206</v>
+      </c>
+      <c r="C130" t="s">
+        <v>208</v>
+      </c>
+      <c r="D130" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130">
+        <v>30</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G130" t="s">
+        <v>163</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I130">
+        <v>4</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K130">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L130" t="s">
+        <v>215</v>
+      </c>
+      <c r="M130">
+        <v>17</v>
+      </c>
+      <c r="N130" t="s">
+        <v>215</v>
+      </c>
+      <c r="O130">
+        <v>2023</v>
+      </c>
+      <c r="P130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q130">
+        <v>18</v>
+      </c>
+      <c r="R130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S130">
+        <f>S126+1</f>
+        <v>8</v>
+      </c>
+      <c r="T130" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U130" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('30',NULL,'4','8/17/2023','18','8');</v>
+      </c>
+      <c r="Y130">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>206</v>
+      </c>
+      <c r="C131" t="s">
+        <v>208</v>
+      </c>
+      <c r="D131" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131">
+        <v>31</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G131" t="s">
+        <v>163</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I131">
+        <v>5</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K131">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L131" t="s">
+        <v>215</v>
+      </c>
+      <c r="M131" s="6">
+        <v>18</v>
+      </c>
+      <c r="N131" t="s">
+        <v>215</v>
+      </c>
+      <c r="O131">
+        <v>2023</v>
+      </c>
+      <c r="P131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q131">
+        <v>18</v>
+      </c>
+      <c r="R131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S131">
+        <f>S127+1</f>
+        <v>8</v>
+      </c>
+      <c r="T131" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U131" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('31',NULL,'5','8/18/2023','18','8');</v>
+      </c>
+      <c r="Y131">
+        <f t="shared" si="16"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="132" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>206</v>
+      </c>
+      <c r="C132" t="s">
+        <v>208</v>
+      </c>
+      <c r="D132" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132">
+        <v>32</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G132" t="s">
+        <v>163</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I132">
+        <v>6</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L132" t="s">
+        <v>215</v>
+      </c>
+      <c r="M132">
+        <v>19</v>
+      </c>
+      <c r="N132" t="s">
+        <v>215</v>
+      </c>
+      <c r="O132">
+        <v>2023</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q132">
+        <v>17</v>
+      </c>
+      <c r="R132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S132">
+        <f>S128+1</f>
+        <v>8</v>
+      </c>
+      <c r="T132" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U132" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('32',NULL,'6','8/19/2023','17','8');</v>
+      </c>
+      <c r="Y132">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="133" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>206</v>
+      </c>
+      <c r="C133" t="s">
+        <v>208</v>
+      </c>
+      <c r="D133" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133">
+        <v>33</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G133" t="s">
+        <v>163</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="J133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="L133" t="s">
+        <v>215</v>
+      </c>
+      <c r="M133" s="6">
+        <v>20</v>
+      </c>
+      <c r="N133" t="s">
+        <v>215</v>
+      </c>
+      <c r="O133">
+        <v>2023</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q133">
+        <v>20</v>
+      </c>
+      <c r="R133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S133">
+        <f>S129+1</f>
+        <v>9</v>
+      </c>
+      <c r="T133" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U133" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('33',NULL,'1','8/20/2023','20','9');</v>
+      </c>
+      <c r="Y133">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>206</v>
+      </c>
+      <c r="C134" t="s">
+        <v>208</v>
+      </c>
+      <c r="D134" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134">
+        <v>34</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G134" t="s">
+        <v>163</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L134" t="s">
+        <v>215</v>
+      </c>
+      <c r="M134" s="6">
+        <v>10</v>
+      </c>
+      <c r="N134" t="s">
+        <v>215</v>
+      </c>
+      <c r="O134">
+        <v>2023</v>
+      </c>
+      <c r="P134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q134">
+        <v>21</v>
+      </c>
+      <c r="R134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S134">
+        <f>S130+1</f>
+        <v>9</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U134" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('34',NULL,'1','9/10/2023','21','9');</v>
+      </c>
+      <c r="Y134">
+        <f t="shared" si="16"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>206</v>
+      </c>
+      <c r="C135" t="s">
+        <v>208</v>
+      </c>
+      <c r="D135" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135">
+        <v>35</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G135" t="s">
+        <v>163</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I135">
+        <v>2</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L135" t="s">
+        <v>215</v>
+      </c>
+      <c r="M135">
+        <v>11</v>
+      </c>
+      <c r="N135" t="s">
+        <v>215</v>
+      </c>
+      <c r="O135">
+        <v>2023</v>
+      </c>
+      <c r="P135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q135">
+        <v>20</v>
+      </c>
+      <c r="R135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S135">
+        <f>S131+1</f>
+        <v>9</v>
+      </c>
+      <c r="T135" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U135" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('35',NULL,'2','9/11/2023','20','9');</v>
+      </c>
+      <c r="Y135">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>206</v>
+      </c>
+      <c r="C136" t="s">
+        <v>208</v>
+      </c>
+      <c r="D136" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136">
+        <v>36</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G136" t="s">
+        <v>163</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I136">
+        <v>4</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K136">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L136" t="s">
+        <v>215</v>
+      </c>
+      <c r="M136" s="6">
+        <v>12</v>
+      </c>
+      <c r="N136" t="s">
+        <v>215</v>
+      </c>
+      <c r="O136">
+        <v>2023</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q136">
+        <v>20</v>
+      </c>
+      <c r="R136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S136">
+        <f>S132+1</f>
+        <v>9</v>
+      </c>
+      <c r="T136" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U136" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('36',NULL,'4','9/12/2023','20','9');</v>
+      </c>
+      <c r="Y136">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>206</v>
+      </c>
+      <c r="C137" t="s">
+        <v>208</v>
+      </c>
+      <c r="D137" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137">
+        <v>37</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G137" t="s">
+        <v>163</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I137">
+        <v>5</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L137" t="s">
+        <v>215</v>
+      </c>
+      <c r="M137">
+        <v>13</v>
+      </c>
+      <c r="N137" t="s">
+        <v>215</v>
+      </c>
+      <c r="O137">
+        <v>2023</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q137">
+        <v>17</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S137">
+        <f>S133+1</f>
+        <v>10</v>
+      </c>
+      <c r="T137" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U137" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('37',NULL,'5','9/13/2023','17','10');</v>
+      </c>
+      <c r="Y137">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>206</v>
+      </c>
+      <c r="C138" t="s">
+        <v>208</v>
+      </c>
+      <c r="D138" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138">
+        <v>38</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G138" t="s">
+        <v>163</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I138">
+        <v>6</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L138" t="s">
+        <v>215</v>
+      </c>
+      <c r="M138" s="6">
+        <v>14</v>
+      </c>
+      <c r="N138" t="s">
+        <v>215</v>
+      </c>
+      <c r="O138">
+        <v>2023</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q138">
+        <v>18</v>
+      </c>
+      <c r="R138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S138">
+        <f>S134+1</f>
+        <v>10</v>
+      </c>
+      <c r="T138" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U138" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('38',NULL,'6','9/14/2023','18','10');</v>
+      </c>
+      <c r="Y138">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>206</v>
+      </c>
+      <c r="C139" t="s">
+        <v>208</v>
+      </c>
+      <c r="D139" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139">
+        <v>39</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G139" t="s">
+        <v>163</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K139">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L139" t="s">
+        <v>215</v>
+      </c>
+      <c r="M139">
+        <v>15</v>
+      </c>
+      <c r="N139" t="s">
+        <v>215</v>
+      </c>
+      <c r="O139">
+        <v>2023</v>
+      </c>
+      <c r="P139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q139">
+        <v>18</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S139">
+        <f>S135+1</f>
+        <v>10</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U139" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('39',NULL,'1','9/15/2023','18','10');</v>
+      </c>
+      <c r="Y139">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="140" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>206</v>
+      </c>
+      <c r="C140" t="s">
+        <v>208</v>
+      </c>
+      <c r="D140" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140">
+        <v>40</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G140" t="s">
+        <v>163</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I140">
+        <v>2</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K140">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L140" t="s">
+        <v>215</v>
+      </c>
+      <c r="M140" s="6">
+        <v>16</v>
+      </c>
+      <c r="N140" t="s">
+        <v>215</v>
+      </c>
+      <c r="O140">
+        <v>2023</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q140">
+        <v>17</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S140">
+        <f>S136+1</f>
+        <v>10</v>
+      </c>
+      <c r="T140" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U140" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('40',NULL,'2','9/16/2023','17','10');</v>
+      </c>
+      <c r="Y140">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>206</v>
+      </c>
+      <c r="C141" t="s">
+        <v>208</v>
+      </c>
+      <c r="D141" t="s">
+        <v>9</v>
+      </c>
+      <c r="E141">
+        <v>41</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G141" t="s">
+        <v>163</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I141">
+        <v>4</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K141">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L141" t="s">
+        <v>215</v>
+      </c>
+      <c r="M141">
+        <v>17</v>
+      </c>
+      <c r="N141" t="s">
+        <v>215</v>
+      </c>
+      <c r="O141">
+        <v>2023</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q141">
+        <v>18</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S141">
+        <f>S137+1</f>
+        <v>11</v>
+      </c>
+      <c r="T141" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U141" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('41',NULL,'4','9/17/2023','18','11');</v>
+      </c>
+      <c r="Y141">
+        <f t="shared" si="16"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="142" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>206</v>
+      </c>
+      <c r="C142" t="s">
+        <v>208</v>
+      </c>
+      <c r="D142" t="s">
+        <v>9</v>
+      </c>
+      <c r="E142">
+        <v>42</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G142" t="s">
+        <v>163</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I142">
+        <v>5</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K142">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L142" t="s">
+        <v>215</v>
+      </c>
+      <c r="M142" s="6">
+        <v>18</v>
+      </c>
+      <c r="N142" t="s">
+        <v>215</v>
+      </c>
+      <c r="O142">
+        <v>2023</v>
+      </c>
+      <c r="P142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q142">
+        <v>23</v>
+      </c>
+      <c r="R142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S142">
+        <f>S138+1</f>
+        <v>11</v>
+      </c>
+      <c r="T142" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U142" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('42',NULL,'5','9/18/2023','23','11');</v>
+      </c>
+      <c r="Y142">
+        <f t="shared" si="16"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="143" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>206</v>
+      </c>
+      <c r="C143" t="s">
+        <v>208</v>
+      </c>
+      <c r="D143" t="s">
+        <v>9</v>
+      </c>
+      <c r="E143">
+        <v>43</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G143" t="s">
+        <v>163</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I143">
+        <v>6</v>
+      </c>
+      <c r="J143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K143">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L143" t="s">
+        <v>215</v>
+      </c>
+      <c r="M143">
+        <v>19</v>
+      </c>
+      <c r="N143" t="s">
+        <v>215</v>
+      </c>
+      <c r="O143">
+        <v>2023</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q143">
+        <v>18</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S143">
+        <f>S139+1</f>
+        <v>11</v>
+      </c>
+      <c r="T143" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U143" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('43',NULL,'6','9/19/2023','18','11');</v>
+      </c>
+      <c r="Y143">
+        <f t="shared" si="16"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="144" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>206</v>
+      </c>
+      <c r="C144" t="s">
+        <v>208</v>
+      </c>
+      <c r="D144" t="s">
+        <v>9</v>
+      </c>
+      <c r="E144">
+        <v>44</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G144" t="s">
+        <v>163</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K144">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="L144" t="s">
+        <v>215</v>
+      </c>
+      <c r="M144" s="6">
+        <v>20</v>
+      </c>
+      <c r="N144" t="s">
+        <v>215</v>
+      </c>
+      <c r="O144">
+        <v>2023</v>
+      </c>
+      <c r="P144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q144">
+        <v>17</v>
+      </c>
+      <c r="R144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S144">
+        <f>S140+1</f>
+        <v>11</v>
+      </c>
+      <c r="T144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U144" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('44',NULL,'1','9/20/2023','17','11');</v>
+      </c>
+      <c r="Y144">
+        <f t="shared" si="16"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="145" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>206</v>
+      </c>
+      <c r="C145" t="s">
+        <v>208</v>
+      </c>
+      <c r="D145" t="s">
+        <v>9</v>
+      </c>
+      <c r="E145">
+        <v>45</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G145" t="s">
+        <v>163</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I145">
+        <v>1</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K145">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L145" t="s">
+        <v>215</v>
+      </c>
+      <c r="M145" s="6">
+        <v>10</v>
+      </c>
+      <c r="N145" t="s">
+        <v>215</v>
+      </c>
+      <c r="O145">
+        <v>2023</v>
+      </c>
+      <c r="P145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q145">
+        <v>25</v>
+      </c>
+      <c r="R145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S145">
+        <f>S141+1</f>
+        <v>12</v>
+      </c>
+      <c r="T145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U145" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('45',NULL,'1','10/10/2023','25','12');</v>
+      </c>
+      <c r="Y145">
+        <f t="shared" si="16"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="146" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>206</v>
+      </c>
+      <c r="C146" t="s">
+        <v>208</v>
+      </c>
+      <c r="D146" t="s">
+        <v>9</v>
+      </c>
+      <c r="E146">
+        <v>46</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G146" t="s">
+        <v>163</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I146">
+        <v>2</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K146">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L146" t="s">
+        <v>215</v>
+      </c>
+      <c r="M146">
+        <v>11</v>
+      </c>
+      <c r="N146" t="s">
+        <v>215</v>
+      </c>
+      <c r="O146">
+        <v>2023</v>
+      </c>
+      <c r="P146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q146">
+        <v>18</v>
+      </c>
+      <c r="R146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S146">
+        <f>S142+1</f>
+        <v>12</v>
+      </c>
+      <c r="T146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U146" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('46',NULL,'2','10/11/2023','18','12');</v>
+      </c>
+      <c r="Y146">
+        <f t="shared" si="16"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="147" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>206</v>
+      </c>
+      <c r="C147" t="s">
+        <v>208</v>
+      </c>
+      <c r="D147" t="s">
+        <v>9</v>
+      </c>
+      <c r="E147">
+        <v>47</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G147" t="s">
+        <v>163</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I147">
+        <v>4</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K147">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L147" t="s">
+        <v>215</v>
+      </c>
+      <c r="M147" s="6">
+        <v>12</v>
+      </c>
+      <c r="N147" t="s">
+        <v>215</v>
+      </c>
+      <c r="O147">
+        <v>2023</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q147">
+        <v>15</v>
+      </c>
+      <c r="R147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S147">
+        <f>S143+1</f>
+        <v>12</v>
+      </c>
+      <c r="T147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U147" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('47',NULL,'4','10/12/2023','15','12');</v>
+      </c>
+      <c r="Y147">
+        <f t="shared" si="16"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="148" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>206</v>
+      </c>
+      <c r="C148" t="s">
+        <v>208</v>
+      </c>
+      <c r="D148" t="s">
+        <v>9</v>
+      </c>
+      <c r="E148">
+        <v>48</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G148" t="s">
+        <v>163</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I148">
+        <v>5</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K148">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="L148" t="s">
+        <v>215</v>
+      </c>
+      <c r="M148">
+        <v>13</v>
+      </c>
+      <c r="N148" t="s">
+        <v>215</v>
+      </c>
+      <c r="O148">
+        <v>2023</v>
+      </c>
+      <c r="P148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q148">
+        <v>30</v>
+      </c>
+      <c r="R148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S148">
+        <f>S144+1</f>
+        <v>12</v>
+      </c>
+      <c r="T148" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U148" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into  inventario values ('48',NULL,'5','10/13/2023','30','12');</v>
+      </c>
+      <c r="Y148">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="E150" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="151" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>206</v>
+      </c>
+      <c r="C151" t="s">
+        <v>217</v>
+      </c>
+      <c r="D151" t="s">
+        <v>9</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G151">
+        <f>K140+1</f>
+        <v>10</v>
+      </c>
+      <c r="H151" t="s">
+        <v>215</v>
+      </c>
+      <c r="I151">
+        <v>13</v>
+      </c>
+      <c r="J151" t="s">
+        <v>215</v>
+      </c>
+      <c r="K151">
+        <v>2023</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M151" t="s">
+        <v>219</v>
+      </c>
+      <c r="N151" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="O151">
+        <v>301</v>
+      </c>
+      <c r="P151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="T151" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U151" t="str">
+        <f t="shared" ref="U151:U153" si="19">_xlfn.CONCAT(B151:T151)</f>
+        <v>insert into  ensamble values ('1','10/13/2023',true,'301');</v>
+      </c>
+    </row>
+    <row r="152" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>206</v>
+      </c>
+      <c r="C152" t="s">
+        <v>217</v>
+      </c>
+      <c r="D152" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152">
+        <v>2</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G152">
+        <f t="shared" ref="G152:G153" si="20">K141+1</f>
+        <v>10</v>
+      </c>
+      <c r="H152" t="s">
+        <v>215</v>
+      </c>
+      <c r="I152">
+        <v>14</v>
+      </c>
+      <c r="J152" t="s">
+        <v>215</v>
+      </c>
+      <c r="K152">
+        <v>2023</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M152" t="s">
+        <v>218</v>
+      </c>
+      <c r="N152" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="O152" t="s">
+        <v>163</v>
+      </c>
+      <c r="P152" s="1"/>
+      <c r="R152" s="1"/>
+      <c r="T152" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U152" t="str">
+        <f t="shared" si="19"/>
+        <v>insert into  ensamble values ('2','10/14/2023',false,NULL);</v>
+      </c>
+    </row>
+    <row r="153" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>206</v>
+      </c>
+      <c r="C153" t="s">
+        <v>217</v>
+      </c>
+      <c r="D153" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153">
+        <v>3</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="H153" t="s">
+        <v>215</v>
+      </c>
+      <c r="I153">
+        <v>15</v>
+      </c>
+      <c r="J153" t="s">
+        <v>215</v>
+      </c>
+      <c r="K153">
+        <v>2023</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M153" t="s">
+        <v>218</v>
+      </c>
+      <c r="N153" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="O153" t="s">
+        <v>163</v>
+      </c>
+      <c r="P153" s="1"/>
+      <c r="R153" s="1"/>
+      <c r="T153" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U153" t="str">
+        <f t="shared" si="19"/>
+        <v>insert into  ensamble values ('3','10/15/2023',false,NULL);</v>
+      </c>
+    </row>
+    <row r="154" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="F154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="N154" s="1"/>
+      <c r="P154" s="1"/>
+      <c r="R154" s="1"/>
+      <c r="T154" s="1"/>
+    </row>
+    <row r="155" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="F155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="N155" s="1"/>
+      <c r="P155" s="1"/>
+      <c r="R155" s="1"/>
+      <c r="T155" s="1"/>
+    </row>
+    <row r="156" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="T156" s="1"/>
+    </row>
+    <row r="157" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="E157" t="s">
+        <v>221</v>
+      </c>
+      <c r="G157" t="s">
+        <v>222</v>
+      </c>
+      <c r="I157" t="s">
+        <v>223</v>
+      </c>
+      <c r="T157" s="1"/>
+    </row>
+    <row r="158" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>206</v>
+      </c>
+      <c r="C158" t="s">
+        <v>220</v>
+      </c>
+      <c r="D158" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G158">
+        <v>1</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I158">
+        <v>1</v>
+      </c>
+      <c r="T158" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U158" t="str">
+        <f t="shared" ref="U158:U163" si="21">_xlfn.CONCAT(B158:T158)</f>
+        <v>insert into  detalleensamble values ('1','1','1');</v>
+      </c>
+    </row>
+    <row r="159" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>206</v>
+      </c>
+      <c r="C159" t="s">
+        <v>220</v>
+      </c>
+      <c r="D159" t="s">
+        <v>9</v>
+      </c>
+      <c r="E159">
+        <v>2</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I159">
+        <v>5</v>
+      </c>
+      <c r="T159" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U159" t="str">
+        <f t="shared" si="21"/>
+        <v>insert into  detalleensamble values ('2','1','5');</v>
+      </c>
+    </row>
+    <row r="160" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>206</v>
+      </c>
+      <c r="C160" t="s">
+        <v>220</v>
+      </c>
+      <c r="D160" t="s">
+        <v>9</v>
+      </c>
+      <c r="E160">
+        <v>3</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I160">
+        <v>9</v>
+      </c>
+      <c r="T160" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U160" t="str">
+        <f t="shared" si="21"/>
+        <v>insert into  detalleensamble values ('3','1','9');</v>
+      </c>
+    </row>
+    <row r="161" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>206</v>
+      </c>
+      <c r="C161" t="s">
+        <v>220</v>
+      </c>
+      <c r="D161" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161">
+        <v>4</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G161">
+        <v>1</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I161">
+        <v>13</v>
+      </c>
+      <c r="T161" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U161" t="str">
+        <f t="shared" si="21"/>
+        <v>insert into  detalleensamble values ('4','1','13');</v>
+      </c>
+    </row>
+    <row r="162" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>206</v>
+      </c>
+      <c r="C162" t="s">
+        <v>220</v>
+      </c>
+      <c r="D162" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162">
+        <v>5</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I162">
+        <v>17</v>
+      </c>
+      <c r="T162" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U162" t="str">
+        <f t="shared" si="21"/>
+        <v>insert into  detalleensamble values ('5','1','17');</v>
+      </c>
+    </row>
+    <row r="163" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>206</v>
+      </c>
+      <c r="C163" t="s">
+        <v>220</v>
+      </c>
+      <c r="D163" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163">
+        <v>6</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G163">
+        <f>G158+1</f>
+        <v>2</v>
+      </c>
+      <c r="H163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I163">
+        <v>21</v>
+      </c>
+      <c r="T163" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U163" t="str">
+        <f t="shared" si="21"/>
+        <v>insert into  detalleensamble values ('6','2','21');</v>
+      </c>
+    </row>
+    <row r="164" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>206</v>
+      </c>
+      <c r="C164" t="s">
+        <v>220</v>
+      </c>
+      <c r="D164" t="s">
+        <v>9</v>
+      </c>
+      <c r="E164">
+        <v>7</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G164">
+        <f t="shared" ref="G164:G172" si="22">G159+1</f>
+        <v>2</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I164">
+        <v>25</v>
+      </c>
+      <c r="T164" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U164" t="str">
+        <f t="shared" ref="U164:U171" si="23">_xlfn.CONCAT(B164:T164)</f>
+        <v>insert into  detalleensamble values ('7','2','25');</v>
+      </c>
+    </row>
+    <row r="165" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>206</v>
+      </c>
+      <c r="C165" t="s">
+        <v>220</v>
+      </c>
+      <c r="D165" t="s">
+        <v>9</v>
+      </c>
+      <c r="E165">
+        <v>8</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I165">
+        <v>29</v>
+      </c>
+      <c r="T165" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U165" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('8','2','29');</v>
+      </c>
+    </row>
+    <row r="166" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>206</v>
+      </c>
+      <c r="C166" t="s">
+        <v>220</v>
+      </c>
+      <c r="D166" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166">
+        <v>9</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I166">
+        <v>33</v>
+      </c>
+      <c r="T166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U166" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('9','2','33');</v>
+      </c>
+    </row>
+    <row r="167" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>206</v>
+      </c>
+      <c r="C167" t="s">
+        <v>220</v>
+      </c>
+      <c r="D167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167">
+        <v>10</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I167">
+        <v>37</v>
+      </c>
+      <c r="T167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U167" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('10','2','37');</v>
+      </c>
+    </row>
+    <row r="168" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>206</v>
+      </c>
+      <c r="C168" t="s">
+        <v>220</v>
+      </c>
+      <c r="D168" t="s">
+        <v>9</v>
+      </c>
+      <c r="E168">
+        <v>11</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I168">
+        <v>41</v>
+      </c>
+      <c r="T168" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U168" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('11','3','41');</v>
+      </c>
+    </row>
+    <row r="169" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>206</v>
+      </c>
+      <c r="C169" t="s">
+        <v>220</v>
+      </c>
+      <c r="D169" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169">
+        <v>12</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I169">
+        <v>45</v>
+      </c>
+      <c r="T169" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U169" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('12','3','45');</v>
+      </c>
+    </row>
+    <row r="170" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>206</v>
+      </c>
+      <c r="C170" t="s">
+        <v>220</v>
+      </c>
+      <c r="D170" t="s">
+        <v>9</v>
+      </c>
+      <c r="E170">
+        <v>13</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I170">
+        <v>2</v>
+      </c>
+      <c r="T170" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U170" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('13','3','2');</v>
+      </c>
+    </row>
+    <row r="171" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>206</v>
+      </c>
+      <c r="C171" t="s">
+        <v>220</v>
+      </c>
+      <c r="D171" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171">
+        <v>14</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I171">
+        <v>6</v>
+      </c>
+      <c r="T171" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U171" t="str">
+        <f t="shared" si="23"/>
+        <v>insert into  detalleensamble values ('14','3','6');</v>
+      </c>
+    </row>
+    <row r="172" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>206</v>
+      </c>
+      <c r="C172" t="s">
+        <v>220</v>
+      </c>
+      <c r="D172" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172">
+        <v>15</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I172">
+        <v>10</v>
+      </c>
+      <c r="T172" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U172" t="str">
+        <f t="shared" ref="U172" si="24">_xlfn.CONCAT(B172:T172)</f>
+        <v>insert into  detalleensamble values ('15','3','10');</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Se actualizo estructura  y datos de la BD 2.0
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\OneDrive\Documentos\Trabajos Universidad\ModuloFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9F806B-E936-4CB3-8519-DF795E2316C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957CEBAA-CE03-4922-A8E0-FE9D88452452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{D6C15466-4649-4A22-BCE7-3BF8AFBFC14E}"/>
   </bookViews>
@@ -773,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -782,8 +782,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3652,8 +3650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530204FE-A160-4075-98A7-610FC6631479}">
   <dimension ref="B2:Y172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="U158" sqref="U158:U172"/>
+    <sheetView tabSelected="1" topLeftCell="K114" workbookViewId="0">
+      <selection activeCell="U101" sqref="U101:U148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3786,7 +3784,7 @@
         <v>7</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T12" si="0">_xlfn.CONCAT(B3:R3)</f>
+        <f>_xlfn.CONCAT(B3:R3)</f>
         <v>insert into empleado values ('102','1','Anuel','Ara','1234567899','2/06/2022','3/10/1984');</v>
       </c>
     </row>
@@ -3844,7 +3842,7 @@
         <v>7</v>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B4:R4)</f>
         <v>insert into empleado values ('103','4','Ana','Aguila','1234567900','3/06/2023','4/08/1985');</v>
       </c>
     </row>
@@ -3901,7 +3899,7 @@
         <v>7</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B5:R5)</f>
         <v>insert into empleado values ('201','1','Bruno','Baldomero','1234567900','1/06/2023','2/09/2000');</v>
       </c>
     </row>
@@ -3940,7 +3938,7 @@
         <v>6</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6" si="1">M5+1</f>
+        <f t="shared" ref="M6" si="0">M5+1</f>
         <v>1234567901</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -3959,7 +3957,7 @@
         <v>7</v>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B6:R6)</f>
         <v>insert into empleado values ('202','1','Benito','Baez','1234567901','2/06/2023','3/10/1995');</v>
       </c>
     </row>
@@ -4016,7 +4014,7 @@
         <v>7</v>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B7:R7)</f>
         <v>insert into empleado values ('203','1','Brenda','Basilio','1234567901','4/06/2022','3/10/1996');</v>
       </c>
     </row>
@@ -4055,7 +4053,7 @@
         <v>6</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8" si="2">M7+1</f>
+        <f t="shared" ref="M8" si="1">M7+1</f>
         <v>1234567902</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -4074,7 +4072,7 @@
         <v>7</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B8:R8)</f>
         <v>insert into empleado values ('301','4','Carla','Casto','1234567902','5/06/2022','3/10/1997');</v>
       </c>
     </row>
@@ -4131,7 +4129,7 @@
         <v>7</v>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B9:R9)</f>
         <v>insert into empleado values ('302','4','Carlo','Castro','1234567902','6/06/2022','3/10/1998');</v>
       </c>
     </row>
@@ -4170,7 +4168,7 @@
         <v>6</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10" si="3">M9+1</f>
+        <f t="shared" ref="M10" si="2">M9+1</f>
         <v>1234567903</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -4189,7 +4187,7 @@
         <v>7</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B10:R10)</f>
         <v>insert into empleado values ('303','1','Camilo','Ciel','1234567903','7/06/2022','3/10/1999');</v>
       </c>
     </row>
@@ -4246,7 +4244,7 @@
         <v>7</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B11:R11)</f>
         <v>insert into empleado values ('304','1','Caleb','Carmelo','1234567903','8/06/2022','3/10/2000');</v>
       </c>
     </row>
@@ -4285,7 +4283,7 @@
         <v>6</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12" si="4">M11+1</f>
+        <f t="shared" ref="M12" si="3">M11+1</f>
         <v>1234567904</v>
       </c>
       <c r="N12" s="1" t="s">
@@ -4304,7 +4302,7 @@
         <v>7</v>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(B12:R12)</f>
         <v>insert into empleado values ('305','4','Camilo','Ciro','1234567904','9/06/2022','3/10/2001');</v>
       </c>
     </row>
@@ -4398,7 +4396,7 @@
         <v>121</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" ref="P15:P24" si="5">_xlfn.CONCAT(B15:N15)</f>
+        <f>_xlfn.CONCAT(B15:N15)</f>
         <v>insert into historiacargo values ('2','1','102','2/06/2022','1/06/2024');</v>
       </c>
     </row>
@@ -4443,7 +4441,7 @@
         <v>121</v>
       </c>
       <c r="P16" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B16:N16)</f>
         <v>insert into historiacargo values ('3','1','103','3/06/2023','2/06/2025');</v>
       </c>
     </row>
@@ -4488,7 +4486,7 @@
         <v>121</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B17:N17)</f>
         <v>insert into historiacargo values ('4','2','201','1/06/2023','31/05/2025');</v>
       </c>
     </row>
@@ -4533,7 +4531,7 @@
         <v>121</v>
       </c>
       <c r="P18" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B18:N18)</f>
         <v>insert into historiacargo values ('5','2','202','2/06/2023','1/06/2025');</v>
       </c>
     </row>
@@ -4578,7 +4576,7 @@
         <v>121</v>
       </c>
       <c r="P19" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B19:N19)</f>
         <v>insert into historiacargo values ('6','2','203','4/06/2022','3/06/2024');</v>
       </c>
     </row>
@@ -4623,7 +4621,7 @@
         <v>121</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B20:N20)</f>
         <v>insert into historiacargo values ('7','3','301','5/06/2022','4/06/2024');</v>
       </c>
     </row>
@@ -4668,7 +4666,7 @@
         <v>121</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B21:N21)</f>
         <v>insert into historiacargo values ('8','3','302','6/06/2022','5/06/2024');</v>
       </c>
     </row>
@@ -4713,7 +4711,7 @@
         <v>121</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B22:N22)</f>
         <v>insert into historiacargo values ('9','3','303','7/06/2022','6/06/2024');</v>
       </c>
     </row>
@@ -4758,7 +4756,7 @@
         <v>121</v>
       </c>
       <c r="P23" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B23:N23)</f>
         <v>insert into historiacargo values ('10','3','304','8/06/2022','7/06/2024');</v>
       </c>
     </row>
@@ -4803,7 +4801,7 @@
         <v>121</v>
       </c>
       <c r="P24" t="str">
-        <f t="shared" si="5"/>
+        <f>_xlfn.CONCAT(B24:N24)</f>
         <v>insert into historiacargo values ('11','3','305','9/06/2022','8/06/2024');</v>
       </c>
     </row>
@@ -4918,7 +4916,7 @@
         <v>7</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" ref="T27:T29" si="6">_xlfn.CONCAT(B27:R27)</f>
+        <f>_xlfn.CONCAT(B27:R27)</f>
         <v>insert into persona values ('602','1','1','Pablo','Ciel','3/06/2023','60000002');</v>
       </c>
     </row>
@@ -4969,14 +4967,14 @@
         <v>6</v>
       </c>
       <c r="Q28">
-        <f t="shared" ref="Q28:Q29" si="7">Q27+1</f>
+        <f t="shared" ref="Q28:Q29" si="4">Q27+1</f>
         <v>60000003</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(B28:R28)</f>
         <v>insert into persona values ('603','3','1','Paola','Carmelo','1/06/2023','60000003');</v>
       </c>
     </row>
@@ -5027,14 +5025,14 @@
         <v>6</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>60000004</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="6"/>
+        <f>_xlfn.CONCAT(B29:R29)</f>
         <v>insert into persona values ('604','4','1','Pancho','Ciro','2/06/2023','60000004');</v>
       </c>
     </row>
@@ -5117,7 +5115,7 @@
         <v>7</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" ref="N32:N42" si="8">_xlfn.CONCAT(B32:L32)</f>
+        <f>_xlfn.CONCAT(B32:L32)</f>
         <v>insert into referenciaelemento values ('2','1','Obs: Board B');</v>
       </c>
       <c r="O32" s="2"/>
@@ -5155,7 +5153,7 @@
         <v>7</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B33:L33)</f>
         <v>insert into referenciaelemento values ('3','1','Obs: Board C');</v>
       </c>
       <c r="O33" s="2"/>
@@ -5193,7 +5191,7 @@
         <v>7</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B34:L34)</f>
         <v>insert into referenciaelemento values ('4','2','Obs: Procesador A');</v>
       </c>
       <c r="O34" s="2"/>
@@ -5231,7 +5229,7 @@
         <v>7</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B35:L35)</f>
         <v>insert into referenciaelemento values ('5','2','Obs: Procesador B');</v>
       </c>
       <c r="O35" s="2"/>
@@ -5269,7 +5267,7 @@
         <v>7</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B36:L36)</f>
         <v>insert into referenciaelemento values ('6','2','Obs: Procesador C');</v>
       </c>
       <c r="O36" s="2"/>
@@ -5307,7 +5305,7 @@
         <v>7</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B37:L37)</f>
         <v>insert into referenciaelemento values ('7','3','Obs: Ram A');</v>
       </c>
       <c r="O37" s="2"/>
@@ -5345,7 +5343,7 @@
         <v>7</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B38:L38)</f>
         <v>insert into referenciaelemento values ('8','3','Obs: Ram B');</v>
       </c>
       <c r="O38" s="2"/>
@@ -5383,7 +5381,7 @@
         <v>7</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B39:L39)</f>
         <v>insert into referenciaelemento values ('9','4','Obs: Disco Duro A');</v>
       </c>
     </row>
@@ -5419,7 +5417,7 @@
         <v>7</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B40:L40)</f>
         <v>insert into referenciaelemento values ('10','4','Obs: Disco Duro B');</v>
       </c>
     </row>
@@ -5455,7 +5453,7 @@
         <v>7</v>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B41:L41)</f>
         <v>insert into referenciaelemento values ('11','5','Obs: Fuente de alimentación A');</v>
       </c>
     </row>
@@ -5491,7 +5489,7 @@
         <v>7</v>
       </c>
       <c r="N42" t="str">
-        <f t="shared" si="8"/>
+        <f>_xlfn.CONCAT(B42:L42)</f>
         <v>insert into referenciaelemento values ('12','5','Obs: Fuente de alimentación B');</v>
       </c>
     </row>
@@ -5835,7 +5833,7 @@
         <v>7</v>
       </c>
       <c r="P51" t="str">
-        <f t="shared" ref="P51" si="9">_xlfn.CONCAT(B51:N51)</f>
+        <f>_xlfn.CONCAT(B51:N51)</f>
         <v>insert into refcarac values ('7','4',NULL,'2','INTEL');</v>
       </c>
     </row>
@@ -5880,7 +5878,7 @@
         <v>7</v>
       </c>
       <c r="P52" t="str">
-        <f t="shared" ref="P52:P60" si="10">_xlfn.CONCAT(B52:N52)</f>
+        <f>_xlfn.CONCAT(B52:N52)</f>
         <v>insert into refcarac values ('8','4','4','4','20');</v>
       </c>
     </row>
@@ -5925,7 +5923,7 @@
         <v>7</v>
       </c>
       <c r="P53" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B53:N53)</f>
         <v>insert into refcarac values ('9','4','2','6','5,3');</v>
       </c>
     </row>
@@ -5970,7 +5968,7 @@
         <v>7</v>
       </c>
       <c r="P54" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B54:N54)</f>
         <v>insert into refcarac values ('10','4','14','9','2');</v>
       </c>
     </row>
@@ -6015,7 +6013,7 @@
         <v>7</v>
       </c>
       <c r="P55" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B55:N55)</f>
         <v>insert into refcarac values ('11','4','8','8','125');</v>
       </c>
     </row>
@@ -6060,7 +6058,7 @@
         <v>7</v>
       </c>
       <c r="P56" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B56:N56)</f>
         <v>insert into refcarac values ('12','5',NULL,'2','AMD');</v>
       </c>
     </row>
@@ -6105,7 +6103,7 @@
         <v>7</v>
       </c>
       <c r="P57" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B57:N57)</f>
         <v>insert into refcarac values ('13','5','4','4','32');</v>
       </c>
     </row>
@@ -6150,7 +6148,7 @@
         <v>7</v>
       </c>
       <c r="P58" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B58:N58)</f>
         <v>insert into refcarac values ('14','5','2','6','3,8');</v>
       </c>
     </row>
@@ -6195,7 +6193,7 @@
         <v>7</v>
       </c>
       <c r="P59" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B59:N59)</f>
         <v>insert into refcarac values ('15','5','14','9','3');</v>
       </c>
     </row>
@@ -6240,7 +6238,7 @@
         <v>7</v>
       </c>
       <c r="P60" t="str">
-        <f t="shared" si="10"/>
+        <f>_xlfn.CONCAT(B60:N60)</f>
         <v>insert into refcarac values ('16','5','8','8','105');</v>
       </c>
     </row>
@@ -6285,7 +6283,7 @@
         <v>7</v>
       </c>
       <c r="P61" t="str">
-        <f t="shared" ref="P61:P74" si="11">_xlfn.CONCAT(B61:N61)</f>
+        <f>_xlfn.CONCAT(B61:N61)</f>
         <v>insert into refcarac values ('17','6',NULL,'2','APPLE');</v>
       </c>
     </row>
@@ -6330,7 +6328,7 @@
         <v>7</v>
       </c>
       <c r="P62" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B62:N62)</f>
         <v>insert into refcarac values ('18','6','4','4','12');</v>
       </c>
     </row>
@@ -6375,7 +6373,7 @@
         <v>7</v>
       </c>
       <c r="P63" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B63:N63)</f>
         <v>insert into refcarac values ('19','6','2','6','4,5');</v>
       </c>
     </row>
@@ -6420,7 +6418,7 @@
         <v>7</v>
       </c>
       <c r="P64" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B64:N64)</f>
         <v>insert into refcarac values ('20','6','14','9','4');</v>
       </c>
     </row>
@@ -6465,7 +6463,7 @@
         <v>7</v>
       </c>
       <c r="P65" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B65:N65)</f>
         <v>insert into refcarac values ('21','6','8','8','110');</v>
       </c>
     </row>
@@ -6510,7 +6508,7 @@
         <v>7</v>
       </c>
       <c r="P66" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B66:N66)</f>
         <v>insert into refcarac values ('22','7',NULL,'2','Corsair ');</v>
       </c>
     </row>
@@ -6555,7 +6553,7 @@
         <v>7</v>
       </c>
       <c r="P67" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B67:N67)</f>
         <v>insert into refcarac values ('23','7',NULL,'1','DDR4');</v>
       </c>
     </row>
@@ -6600,7 +6598,7 @@
         <v>7</v>
       </c>
       <c r="P68" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B68:N68)</f>
         <v>insert into refcarac values ('24','7','5','4','16');</v>
       </c>
     </row>
@@ -6645,7 +6643,7 @@
         <v>7</v>
       </c>
       <c r="P69" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B69:N69)</f>
         <v>insert into refcarac values ('25','7','1','6','3200');</v>
       </c>
     </row>
@@ -6690,7 +6688,7 @@
         <v>7</v>
       </c>
       <c r="P70" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B70:N70)</f>
         <v>insert into refcarac values ('26','7',NULL,'7','16-18-18-36');</v>
       </c>
     </row>
@@ -6735,7 +6733,7 @@
         <v>7</v>
       </c>
       <c r="P71" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B71:N71)</f>
         <v>insert into refcarac values ('27','7','7','8','1,35');</v>
       </c>
     </row>
@@ -6780,7 +6778,7 @@
         <v>7</v>
       </c>
       <c r="P72" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B72:N72)</f>
         <v>insert into refcarac values ('28','8',NULL,'2','Kingston ');</v>
       </c>
     </row>
@@ -6825,7 +6823,7 @@
         <v>7</v>
       </c>
       <c r="P73" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B73:N73)</f>
         <v>insert into refcarac values ('29','8',NULL,'1','DDR4');</v>
       </c>
     </row>
@@ -6870,7 +6868,7 @@
         <v>7</v>
       </c>
       <c r="P74" t="str">
-        <f t="shared" si="11"/>
+        <f>_xlfn.CONCAT(B74:N74)</f>
         <v>insert into refcarac values ('30','8','5','4','32');</v>
       </c>
     </row>
@@ -6915,7 +6913,7 @@
         <v>7</v>
       </c>
       <c r="P75" t="str">
-        <f t="shared" ref="P75:P77" si="12">_xlfn.CONCAT(B75:N75)</f>
+        <f>_xlfn.CONCAT(B75:N75)</f>
         <v>insert into refcarac values ('31','8','1','6','3600');</v>
       </c>
     </row>
@@ -6960,7 +6958,7 @@
         <v>7</v>
       </c>
       <c r="P76" t="str">
-        <f t="shared" si="12"/>
+        <f>_xlfn.CONCAT(B76:N76)</f>
         <v>insert into refcarac values ('32','8',NULL,'7','16-17-17-35');</v>
       </c>
     </row>
@@ -7005,7 +7003,7 @@
         <v>7</v>
       </c>
       <c r="P77" t="str">
-        <f t="shared" si="12"/>
+        <f>_xlfn.CONCAT(B77:N77)</f>
         <v>insert into refcarac values ('33','8','7','8','1,2');</v>
       </c>
     </row>
@@ -7050,7 +7048,7 @@
         <v>7</v>
       </c>
       <c r="P78" t="str">
-        <f t="shared" ref="P78" si="13">_xlfn.CONCAT(B78:N78)</f>
+        <f>_xlfn.CONCAT(B78:N78)</f>
         <v>insert into refcarac values ('34','9',NULL,'2','Toshiba ');</v>
       </c>
     </row>
@@ -7095,7 +7093,7 @@
         <v>7</v>
       </c>
       <c r="P79" t="str">
-        <f t="shared" ref="P79:P93" si="14">_xlfn.CONCAT(B79:N79)</f>
+        <f>_xlfn.CONCAT(B79:N79)</f>
         <v>insert into refcarac values ('35','9',NULL,'1','HDD');</v>
       </c>
     </row>
@@ -7140,7 +7138,7 @@
         <v>7</v>
       </c>
       <c r="P80" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B80:N80)</f>
         <v>insert into refcarac values ('36','9','19','3','7200');</v>
       </c>
     </row>
@@ -7185,7 +7183,7 @@
         <v>7</v>
       </c>
       <c r="P81" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B81:N81)</f>
         <v>insert into refcarac values ('37','9','6','4','3');</v>
       </c>
     </row>
@@ -7230,7 +7228,7 @@
         <v>7</v>
       </c>
       <c r="P82" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B82:N82)</f>
         <v>insert into refcarac values ('38','9',NULL,'11','SATA 6 Gb/s');</v>
       </c>
     </row>
@@ -7275,7 +7273,7 @@
         <v>7</v>
       </c>
       <c r="P83" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B83:N83)</f>
         <v>insert into refcarac values ('39','10',NULL,'2','Samsung ');</v>
       </c>
     </row>
@@ -7320,7 +7318,7 @@
         <v>7</v>
       </c>
       <c r="P84" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B84:N84)</f>
         <v>insert into refcarac values ('40','10',NULL,'1','SDD');</v>
       </c>
     </row>
@@ -7365,7 +7363,7 @@
         <v>7</v>
       </c>
       <c r="P85" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B85:N85)</f>
         <v>insert into refcarac values ('41','10','21','3','2500');</v>
       </c>
     </row>
@@ -7410,7 +7408,7 @@
         <v>7</v>
       </c>
       <c r="P86" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B86:N86)</f>
         <v>insert into refcarac values ('42','10','5','4','250');</v>
       </c>
     </row>
@@ -7455,7 +7453,7 @@
         <v>7</v>
       </c>
       <c r="P87" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B87:N87)</f>
         <v>insert into refcarac values ('43','10',NULL,'11','PCIe 3.0 x4');</v>
       </c>
     </row>
@@ -7500,7 +7498,7 @@
         <v>7</v>
       </c>
       <c r="P88" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B88:N88)</f>
         <v>insert into refcarac values ('44','11',NULL,'2','EVGA ');</v>
       </c>
     </row>
@@ -7545,7 +7543,7 @@
         <v>7</v>
       </c>
       <c r="P89" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B89:N89)</f>
         <v>insert into refcarac values ('45','11',NULL,'1','Modular');</v>
       </c>
     </row>
@@ -7590,7 +7588,7 @@
         <v>7</v>
       </c>
       <c r="P90" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B90:N90)</f>
         <v>insert into refcarac values ('46','11',NULL,'5','1x 24-pin, 1x 8-pin (CPU)');</v>
       </c>
     </row>
@@ -7635,7 +7633,7 @@
         <v>7</v>
       </c>
       <c r="P91" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B91:N91)</f>
         <v>insert into refcarac values ('47','12',NULL,'2','Seasonic  ');</v>
       </c>
     </row>
@@ -7680,7 +7678,7 @@
         <v>7</v>
       </c>
       <c r="P92" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B92:N92)</f>
         <v>insert into refcarac values ('48','12',NULL,'1','Semi-Modular');</v>
       </c>
     </row>
@@ -7725,7 +7723,7 @@
         <v>7</v>
       </c>
       <c r="P93" t="str">
-        <f t="shared" si="14"/>
+        <f>_xlfn.CONCAT(B93:N93)</f>
         <v>insert into refcarac values ('49','12',NULL,'5','4x PCIe 8-pin');</v>
       </c>
     </row>
@@ -7905,42 +7903,42 @@
       <c r="J101" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K101" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L101" t="s">
-        <v>215</v>
-      </c>
-      <c r="M101" s="6">
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M101" s="1">
         <v>10</v>
       </c>
       <c r="N101" t="s">
         <v>215</v>
       </c>
-      <c r="O101">
+      <c r="O101" t="s">
+        <v>216</v>
+      </c>
+      <c r="P101" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q101">
         <v>2023</v>
       </c>
-      <c r="P101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q101">
+      <c r="R101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S101">
         <v>40</v>
-      </c>
-      <c r="R101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S101">
-        <v>1</v>
       </c>
       <c r="T101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U101" t="str">
         <f>_xlfn.CONCAT(B101:T101)</f>
-        <v>insert into  inventario values ('1',NULL,'1','06/10/2023','40','1');</v>
+        <v>insert into  inventario values ('1',NULL,'1','1','10/06/2023','40');</v>
       </c>
       <c r="Y101">
-        <f>Q101/10</f>
+        <f>S101/10</f>
         <v>4</v>
       </c>
     </row>
@@ -7972,11 +7970,11 @@
       <c r="J102" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K102" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L102" t="s">
-        <v>215</v>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M102">
         <v>11</v>
@@ -7984,30 +7982,30 @@
       <c r="N102" t="s">
         <v>215</v>
       </c>
-      <c r="O102">
+      <c r="O102" t="s">
+        <v>216</v>
+      </c>
+      <c r="P102" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q102">
         <v>2023</v>
       </c>
-      <c r="P102" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q102">
+      <c r="R102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S102">
         <v>42</v>
       </c>
-      <c r="R102" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S102">
-        <v>1</v>
-      </c>
       <c r="T102" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U102" t="str">
-        <f t="shared" ref="U102:U148" si="15">_xlfn.CONCAT(B102:T102)</f>
-        <v>insert into  inventario values ('2',NULL,'2','06/11/2023','42','1');</v>
+        <f>_xlfn.CONCAT(B102:T102)</f>
+        <v>insert into  inventario values ('2',NULL,'2','1','11/06/2023','42');</v>
       </c>
       <c r="Y102">
-        <f t="shared" ref="Y102:Y148" si="16">Q102/10</f>
+        <f>S102/10</f>
         <v>4.2</v>
       </c>
     </row>
@@ -8039,42 +8037,42 @@
       <c r="J103" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K103" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L103" t="s">
-        <v>215</v>
-      </c>
-      <c r="M103" s="6">
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M103" s="1">
         <v>12</v>
       </c>
       <c r="N103" t="s">
         <v>215</v>
       </c>
-      <c r="O103">
+      <c r="O103" t="s">
+        <v>216</v>
+      </c>
+      <c r="P103" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q103">
         <v>2023</v>
       </c>
-      <c r="P103" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q103">
+      <c r="R103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S103">
         <v>41</v>
       </c>
-      <c r="R103" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S103">
-        <v>1</v>
-      </c>
       <c r="T103" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U103" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('3',NULL,'4','06/12/2023','41','1');</v>
+        <f>_xlfn.CONCAT(B103:T103)</f>
+        <v>insert into  inventario values ('3',NULL,'4','1','12/06/2023','41');</v>
       </c>
       <c r="Y103">
-        <f t="shared" si="16"/>
+        <f>S103/10</f>
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -8106,11 +8104,11 @@
       <c r="J104" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K104" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L104" t="s">
-        <v>215</v>
+      <c r="K104">
+        <v>1</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M104">
         <v>13</v>
@@ -8118,30 +8116,30 @@
       <c r="N104" t="s">
         <v>215</v>
       </c>
-      <c r="O104">
+      <c r="O104" t="s">
+        <v>216</v>
+      </c>
+      <c r="P104" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q104">
         <v>2023</v>
       </c>
-      <c r="P104" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q104">
+      <c r="R104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S104">
         <v>40</v>
       </c>
-      <c r="R104" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S104">
-        <v>1</v>
-      </c>
       <c r="T104" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U104" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('4',NULL,'5','06/13/2023','40','1');</v>
+        <f>_xlfn.CONCAT(B104:T104)</f>
+        <v>insert into  inventario values ('4',NULL,'5','1','13/06/2023','40');</v>
       </c>
       <c r="Y104">
-        <f t="shared" si="16"/>
+        <f>S104/10</f>
         <v>4</v>
       </c>
     </row>
@@ -8173,42 +8171,42 @@
       <c r="J105" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K105" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L105" t="s">
-        <v>215</v>
-      </c>
-      <c r="M105" s="6">
+      <c r="K105">
+        <v>2</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M105" s="1">
         <v>14</v>
       </c>
       <c r="N105" t="s">
         <v>215</v>
       </c>
-      <c r="O105">
+      <c r="O105" t="s">
+        <v>216</v>
+      </c>
+      <c r="P105" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q105">
         <v>2023</v>
       </c>
-      <c r="P105" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q105">
+      <c r="R105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S105">
         <v>35</v>
       </c>
-      <c r="R105" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S105">
-        <v>2</v>
-      </c>
       <c r="T105" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U105" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('5',NULL,'6','06/14/2023','35','2');</v>
+        <f>_xlfn.CONCAT(B105:T105)</f>
+        <v>insert into  inventario values ('5',NULL,'6','2','14/06/2023','35');</v>
       </c>
       <c r="Y105">
-        <f t="shared" si="16"/>
+        <f>S105/10</f>
         <v>3.5</v>
       </c>
     </row>
@@ -8240,11 +8238,11 @@
       <c r="J106" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K106" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L106" t="s">
-        <v>215</v>
+      <c r="K106">
+        <v>2</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M106">
         <v>15</v>
@@ -8252,30 +8250,30 @@
       <c r="N106" t="s">
         <v>215</v>
       </c>
-      <c r="O106">
+      <c r="O106" t="s">
+        <v>216</v>
+      </c>
+      <c r="P106" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q106">
         <v>2023</v>
       </c>
-      <c r="P106" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q106">
+      <c r="R106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S106">
         <v>37</v>
       </c>
-      <c r="R106" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S106">
-        <v>2</v>
-      </c>
       <c r="T106" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U106" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('6',NULL,'1','06/15/2023','37','2');</v>
+        <f>_xlfn.CONCAT(B106:T106)</f>
+        <v>insert into  inventario values ('6',NULL,'1','2','15/06/2023','37');</v>
       </c>
       <c r="Y106">
-        <f t="shared" si="16"/>
+        <f>S106/10</f>
         <v>3.7</v>
       </c>
     </row>
@@ -8307,42 +8305,42 @@
       <c r="J107" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K107" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L107" t="s">
-        <v>215</v>
-      </c>
-      <c r="M107" s="6">
+      <c r="K107">
+        <v>2</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M107" s="1">
         <v>16</v>
       </c>
       <c r="N107" t="s">
         <v>215</v>
       </c>
-      <c r="O107">
+      <c r="O107" t="s">
+        <v>216</v>
+      </c>
+      <c r="P107" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q107">
         <v>2023</v>
       </c>
-      <c r="P107" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q107">
+      <c r="R107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S107">
         <v>36</v>
       </c>
-      <c r="R107" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S107">
-        <v>2</v>
-      </c>
       <c r="T107" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U107" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('7',NULL,'2','06/16/2023','36','2');</v>
+        <f>_xlfn.CONCAT(B107:T107)</f>
+        <v>insert into  inventario values ('7',NULL,'2','2','16/06/2023','36');</v>
       </c>
       <c r="Y107">
-        <f t="shared" si="16"/>
+        <f>S107/10</f>
         <v>3.6</v>
       </c>
     </row>
@@ -8374,11 +8372,11 @@
       <c r="J108" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K108" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L108" t="s">
-        <v>215</v>
+      <c r="K108">
+        <v>2</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M108">
         <v>17</v>
@@ -8386,30 +8384,30 @@
       <c r="N108" t="s">
         <v>215</v>
       </c>
-      <c r="O108">
+      <c r="O108" t="s">
+        <v>216</v>
+      </c>
+      <c r="P108" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q108">
         <v>2023</v>
       </c>
-      <c r="P108" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q108">
+      <c r="R108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S108">
         <v>35</v>
       </c>
-      <c r="R108" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S108">
-        <v>2</v>
-      </c>
       <c r="T108" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U108" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('8',NULL,'4','06/17/2023','35','2');</v>
+        <f>_xlfn.CONCAT(B108:T108)</f>
+        <v>insert into  inventario values ('8',NULL,'4','2','17/06/2023','35');</v>
       </c>
       <c r="Y108">
-        <f t="shared" si="16"/>
+        <f>S108/10</f>
         <v>3.5</v>
       </c>
     </row>
@@ -8441,42 +8439,42 @@
       <c r="J109" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K109" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L109" t="s">
-        <v>215</v>
-      </c>
-      <c r="M109" s="6">
+      <c r="K109">
+        <v>3</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M109" s="1">
         <v>18</v>
       </c>
       <c r="N109" t="s">
         <v>215</v>
       </c>
-      <c r="O109">
+      <c r="O109" t="s">
+        <v>216</v>
+      </c>
+      <c r="P109" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q109">
         <v>2023</v>
       </c>
-      <c r="P109" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q109">
+      <c r="R109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S109">
         <v>55</v>
       </c>
-      <c r="R109" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S109">
-        <v>3</v>
-      </c>
       <c r="T109" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U109" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('9',NULL,'5','06/18/2023','55','3');</v>
+        <f>_xlfn.CONCAT(B109:T109)</f>
+        <v>insert into  inventario values ('9',NULL,'5','3','18/06/2023','55');</v>
       </c>
       <c r="Y109">
-        <f t="shared" si="16"/>
+        <f>S109/10</f>
         <v>5.5</v>
       </c>
     </row>
@@ -8508,11 +8506,11 @@
       <c r="J110" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K110" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L110" t="s">
-        <v>215</v>
+      <c r="K110">
+        <v>3</v>
+      </c>
+      <c r="L110" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M110">
         <v>19</v>
@@ -8520,30 +8518,30 @@
       <c r="N110" t="s">
         <v>215</v>
       </c>
-      <c r="O110">
+      <c r="O110" t="s">
+        <v>216</v>
+      </c>
+      <c r="P110" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q110">
         <v>2023</v>
       </c>
-      <c r="P110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q110">
+      <c r="R110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S110">
         <v>57</v>
       </c>
-      <c r="R110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S110">
-        <v>3</v>
-      </c>
       <c r="T110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U110" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('10',NULL,'6','06/19/2023','57','3');</v>
+        <f>_xlfn.CONCAT(B110:T110)</f>
+        <v>insert into  inventario values ('10',NULL,'6','3','19/06/2023','57');</v>
       </c>
       <c r="Y110">
-        <f t="shared" si="16"/>
+        <f>S110/10</f>
         <v>5.7</v>
       </c>
     </row>
@@ -8575,42 +8573,42 @@
       <c r="J111" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K111" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="L111" t="s">
-        <v>215</v>
-      </c>
-      <c r="M111" s="6">
+      <c r="K111">
+        <v>3</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M111" s="1">
         <v>20</v>
       </c>
       <c r="N111" t="s">
         <v>215</v>
       </c>
-      <c r="O111">
+      <c r="O111" t="s">
+        <v>216</v>
+      </c>
+      <c r="P111" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q111">
         <v>2023</v>
       </c>
-      <c r="P111" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q111">
+      <c r="R111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S111">
         <v>56</v>
       </c>
-      <c r="R111" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S111">
-        <v>3</v>
-      </c>
       <c r="T111" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U111" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('11',NULL,'1','06/20/2023','56','3');</v>
+        <f>_xlfn.CONCAT(B111:T111)</f>
+        <v>insert into  inventario values ('11',NULL,'1','3','20/06/2023','56');</v>
       </c>
       <c r="Y111">
-        <f t="shared" si="16"/>
+        <f>S111/10</f>
         <v>5.6</v>
       </c>
     </row>
@@ -8643,42 +8641,42 @@
         <v>6</v>
       </c>
       <c r="K112">
-        <f>K101+1</f>
-        <v>7</v>
-      </c>
-      <c r="L112" t="s">
-        <v>215</v>
-      </c>
-      <c r="M112" s="6">
+        <v>3</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M112" s="1">
         <v>10</v>
       </c>
       <c r="N112" t="s">
         <v>215</v>
       </c>
       <c r="O112">
+        <f>O101+1</f>
+        <v>7</v>
+      </c>
+      <c r="P112" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q112">
         <v>2023</v>
       </c>
-      <c r="P112" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q112">
+      <c r="R112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S112">
         <v>55</v>
       </c>
-      <c r="R112" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S112">
-        <v>3</v>
-      </c>
       <c r="T112" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U112" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('12',NULL,'1','7/10/2023','55','3');</v>
+        <f>_xlfn.CONCAT(B112:T112)</f>
+        <v>insert into  inventario values ('12',NULL,'1','3','10/7/2023','55');</v>
       </c>
       <c r="Y112">
-        <f t="shared" si="16"/>
+        <f>S112/10</f>
         <v>5.5</v>
       </c>
     </row>
@@ -8711,11 +8709,11 @@
         <v>6</v>
       </c>
       <c r="K113">
-        <f t="shared" ref="K113:K148" si="17">K102+1</f>
-        <v>7</v>
-      </c>
-      <c r="L113" t="s">
-        <v>215</v>
+        <f t="shared" ref="K113:K148" si="5">K109+1</f>
+        <v>4</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M113">
         <v>11</v>
@@ -8724,30 +8722,30 @@
         <v>215</v>
       </c>
       <c r="O113">
+        <f t="shared" ref="O113:O148" si="6">O102+1</f>
+        <v>7</v>
+      </c>
+      <c r="P113" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q113">
         <v>2023</v>
       </c>
-      <c r="P113" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q113">
+      <c r="R113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S113">
         <v>80</v>
       </c>
-      <c r="R113" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S113">
-        <f>S109+1</f>
-        <v>4</v>
-      </c>
       <c r="T113" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U113" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('13',NULL,'2','7/11/2023','80','4');</v>
+        <f>_xlfn.CONCAT(B113:T113)</f>
+        <v>insert into  inventario values ('13',NULL,'2','4','11/7/2023','80');</v>
       </c>
       <c r="Y113">
-        <f t="shared" si="16"/>
+        <f>S113/10</f>
         <v>8</v>
       </c>
     </row>
@@ -8780,43 +8778,43 @@
         <v>6</v>
       </c>
       <c r="K114">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L114" t="s">
-        <v>215</v>
-      </c>
-      <c r="M114" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M114" s="1">
         <v>12</v>
       </c>
       <c r="N114" t="s">
         <v>215</v>
       </c>
       <c r="O114">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P114" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q114">
         <v>2023</v>
       </c>
-      <c r="P114" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q114">
+      <c r="R114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S114">
         <v>84</v>
       </c>
-      <c r="R114" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S114">
-        <f>S110+1</f>
-        <v>4</v>
-      </c>
       <c r="T114" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U114" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('14',NULL,'4','7/12/2023','84','4');</v>
+        <f>_xlfn.CONCAT(B114:T114)</f>
+        <v>insert into  inventario values ('14',NULL,'4','4','12/7/2023','84');</v>
       </c>
       <c r="Y114">
-        <f t="shared" si="16"/>
+        <f>S114/10</f>
         <v>8.4</v>
       </c>
     </row>
@@ -8849,11 +8847,11 @@
         <v>6</v>
       </c>
       <c r="K115">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L115" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M115">
         <v>13</v>
@@ -8862,30 +8860,30 @@
         <v>215</v>
       </c>
       <c r="O115">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P115" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q115">
         <v>2023</v>
       </c>
-      <c r="P115" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q115">
+      <c r="R115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S115">
         <v>82</v>
       </c>
-      <c r="R115" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S115">
-        <f>S111+1</f>
-        <v>4</v>
-      </c>
       <c r="T115" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U115" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('15',NULL,'5','7/13/2023','82','4');</v>
+        <f>_xlfn.CONCAT(B115:T115)</f>
+        <v>insert into  inventario values ('15',NULL,'5','4','13/7/2023','82');</v>
       </c>
       <c r="Y115">
-        <f t="shared" si="16"/>
+        <f>S115/10</f>
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -8918,43 +8916,43 @@
         <v>6</v>
       </c>
       <c r="K116">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L116" t="s">
-        <v>215</v>
-      </c>
-      <c r="M116" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M116" s="1">
         <v>14</v>
       </c>
       <c r="N116" t="s">
         <v>215</v>
       </c>
       <c r="O116">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P116" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q116">
         <v>2023</v>
       </c>
-      <c r="P116" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q116">
+      <c r="R116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S116">
         <v>80</v>
       </c>
-      <c r="R116" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S116">
-        <f>S112+1</f>
-        <v>4</v>
-      </c>
       <c r="T116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U116" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('16',NULL,'6','7/14/2023','80','4');</v>
+        <f>_xlfn.CONCAT(B116:T116)</f>
+        <v>insert into  inventario values ('16',NULL,'6','4','14/7/2023','80');</v>
       </c>
       <c r="Y116">
-        <f t="shared" si="16"/>
+        <f>S116/10</f>
         <v>8</v>
       </c>
     </row>
@@ -8987,11 +8985,11 @@
         <v>6</v>
       </c>
       <c r="K117">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L117" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M117">
         <v>15</v>
@@ -9000,30 +8998,30 @@
         <v>215</v>
       </c>
       <c r="O117">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P117" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q117">
         <v>2023</v>
       </c>
-      <c r="P117" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q117">
+      <c r="R117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S117">
         <v>70</v>
       </c>
-      <c r="R117" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S117">
-        <f>S113+1</f>
-        <v>5</v>
-      </c>
       <c r="T117" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U117" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('17',NULL,'1','7/15/2023','70','5');</v>
+        <f>_xlfn.CONCAT(B117:T117)</f>
+        <v>insert into  inventario values ('17',NULL,'1','5','15/7/2023','70');</v>
       </c>
       <c r="Y117">
-        <f t="shared" si="16"/>
+        <f>S117/10</f>
         <v>7</v>
       </c>
     </row>
@@ -9056,43 +9054,43 @@
         <v>6</v>
       </c>
       <c r="K118">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L118" t="s">
-        <v>215</v>
-      </c>
-      <c r="M118" s="6">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M118" s="1">
         <v>16</v>
       </c>
       <c r="N118" t="s">
         <v>215</v>
       </c>
       <c r="O118">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P118" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q118">
         <v>2023</v>
       </c>
-      <c r="P118" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q118">
+      <c r="R118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S118">
         <v>74</v>
       </c>
-      <c r="R118" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S118">
-        <f>S114+1</f>
-        <v>5</v>
-      </c>
       <c r="T118" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U118" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('18',NULL,'2','7/16/2023','74','5');</v>
+        <f>_xlfn.CONCAT(B118:T118)</f>
+        <v>insert into  inventario values ('18',NULL,'2','5','16/7/2023','74');</v>
       </c>
       <c r="Y118">
-        <f t="shared" si="16"/>
+        <f>S118/10</f>
         <v>7.4</v>
       </c>
     </row>
@@ -9125,11 +9123,11 @@
         <v>6</v>
       </c>
       <c r="K119">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L119" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M119">
         <v>17</v>
@@ -9138,30 +9136,30 @@
         <v>215</v>
       </c>
       <c r="O119">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P119" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q119">
         <v>2023</v>
       </c>
-      <c r="P119" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q119">
+      <c r="R119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S119">
         <v>72</v>
       </c>
-      <c r="R119" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S119">
-        <f>S115+1</f>
-        <v>5</v>
-      </c>
       <c r="T119" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U119" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('19',NULL,'4','7/17/2023','72','5');</v>
+        <f>_xlfn.CONCAT(B119:T119)</f>
+        <v>insert into  inventario values ('19',NULL,'4','5','17/7/2023','72');</v>
       </c>
       <c r="Y119">
-        <f t="shared" si="16"/>
+        <f>S119/10</f>
         <v>7.2</v>
       </c>
     </row>
@@ -9194,43 +9192,43 @@
         <v>6</v>
       </c>
       <c r="K120">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L120" t="s">
-        <v>215</v>
-      </c>
-      <c r="M120" s="6">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M120" s="1">
         <v>18</v>
       </c>
       <c r="N120" t="s">
         <v>215</v>
       </c>
       <c r="O120">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P120" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q120">
         <v>2023</v>
       </c>
-      <c r="P120" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q120">
+      <c r="R120" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S120">
         <v>70</v>
       </c>
-      <c r="R120" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S120">
-        <f>S116+1</f>
-        <v>5</v>
-      </c>
       <c r="T120" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U120" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('20',NULL,'5','7/18/2023','70','5');</v>
+        <f>_xlfn.CONCAT(B120:T120)</f>
+        <v>insert into  inventario values ('20',NULL,'5','5','18/7/2023','70');</v>
       </c>
       <c r="Y120">
-        <f t="shared" si="16"/>
+        <f>S120/10</f>
         <v>7</v>
       </c>
     </row>
@@ -9263,11 +9261,11 @@
         <v>6</v>
       </c>
       <c r="K121">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L121" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M121">
         <v>19</v>
@@ -9276,30 +9274,30 @@
         <v>215</v>
       </c>
       <c r="O121">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P121" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q121">
         <v>2023</v>
       </c>
-      <c r="P121" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q121">
+      <c r="R121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S121">
         <v>11</v>
       </c>
-      <c r="R121" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S121">
-        <f>S117+1</f>
-        <v>6</v>
-      </c>
       <c r="T121" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U121" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('21',NULL,'6','7/19/2023','11','6');</v>
+        <f>_xlfn.CONCAT(B121:T121)</f>
+        <v>insert into  inventario values ('21',NULL,'6','6','19/7/2023','11');</v>
       </c>
       <c r="Y121">
-        <f>Q121/100</f>
+        <f>S121/100</f>
         <v>0.11</v>
       </c>
     </row>
@@ -9332,40 +9330,40 @@
         <v>6</v>
       </c>
       <c r="K122">
-        <f t="shared" si="17"/>
-        <v>7</v>
-      </c>
-      <c r="L122" t="s">
-        <v>215</v>
-      </c>
-      <c r="M122" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M122" s="1">
         <v>20</v>
       </c>
       <c r="N122" t="s">
         <v>215</v>
       </c>
       <c r="O122">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="P122" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q122">
         <v>2023</v>
       </c>
-      <c r="P122" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q122">
+      <c r="R122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S122">
         <v>11</v>
       </c>
-      <c r="R122" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S122">
-        <f>S118+1</f>
-        <v>6</v>
-      </c>
       <c r="T122" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U122" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('22',NULL,'1','7/20/2023','11','6');</v>
+        <f>_xlfn.CONCAT(B122:T122)</f>
+        <v>insert into  inventario values ('22',NULL,'1','6','20/7/2023','11');</v>
       </c>
       <c r="Y122">
         <v>11</v>
@@ -9400,40 +9398,40 @@
         <v>6</v>
       </c>
       <c r="K123">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L123" t="s">
-        <v>215</v>
-      </c>
-      <c r="M123" s="6">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M123" s="1">
         <v>10</v>
       </c>
       <c r="N123" t="s">
         <v>215</v>
       </c>
       <c r="O123">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P123" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q123">
         <v>2023</v>
       </c>
-      <c r="P123" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q123">
+      <c r="R123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S123">
         <v>11</v>
       </c>
-      <c r="R123" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S123">
-        <f>S119+1</f>
-        <v>6</v>
-      </c>
       <c r="T123" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U123" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('23',NULL,'1','8/10/2023','11','6');</v>
+        <f>_xlfn.CONCAT(B123:T123)</f>
+        <v>insert into  inventario values ('23',NULL,'1','6','10/8/2023','11');</v>
       </c>
       <c r="Y123">
         <v>11</v>
@@ -9468,11 +9466,11 @@
         <v>6</v>
       </c>
       <c r="K124">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L124" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M124">
         <v>11</v>
@@ -9481,30 +9479,30 @@
         <v>215</v>
       </c>
       <c r="O124">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P124" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q124">
         <v>2023</v>
       </c>
-      <c r="P124" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q124">
+      <c r="R124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S124">
         <v>11</v>
       </c>
-      <c r="R124" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S124">
-        <f>S120+1</f>
-        <v>6</v>
-      </c>
       <c r="T124" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U124" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('24',NULL,'2','8/11/2023','11','6');</v>
+        <f>_xlfn.CONCAT(B124:T124)</f>
+        <v>insert into  inventario values ('24',NULL,'2','6','11/8/2023','11');</v>
       </c>
       <c r="Y124">
-        <f t="shared" ref="Y122:Y124" si="18">Q124/100</f>
+        <f>S124/100</f>
         <v>0.11</v>
       </c>
     </row>
@@ -9537,43 +9535,43 @@
         <v>6</v>
       </c>
       <c r="K125">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L125" t="s">
-        <v>215</v>
-      </c>
-      <c r="M125" s="6">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M125" s="1">
         <v>12</v>
       </c>
       <c r="N125" t="s">
         <v>215</v>
       </c>
       <c r="O125">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P125" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q125">
         <v>2023</v>
       </c>
-      <c r="P125" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q125">
+      <c r="R125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S125">
         <v>20</v>
       </c>
-      <c r="R125" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S125">
-        <f>S121+1</f>
-        <v>7</v>
-      </c>
       <c r="T125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U125" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('25',NULL,'4','8/12/2023','20','7');</v>
+        <f>_xlfn.CONCAT(B125:T125)</f>
+        <v>insert into  inventario values ('25',NULL,'4','7','12/8/2023','20');</v>
       </c>
       <c r="Y125">
-        <f t="shared" si="16"/>
+        <f>S125/10</f>
         <v>2</v>
       </c>
     </row>
@@ -9606,11 +9604,11 @@
         <v>6</v>
       </c>
       <c r="K126">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L126" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M126">
         <v>13</v>
@@ -9619,30 +9617,30 @@
         <v>215</v>
       </c>
       <c r="O126">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P126" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q126">
         <v>2023</v>
       </c>
-      <c r="P126" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q126">
+      <c r="R126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S126">
         <v>21</v>
       </c>
-      <c r="R126" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S126">
-        <f>S122+1</f>
-        <v>7</v>
-      </c>
       <c r="T126" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U126" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('26',NULL,'5','8/13/2023','21','7');</v>
+        <f>_xlfn.CONCAT(B126:T126)</f>
+        <v>insert into  inventario values ('26',NULL,'5','7','13/8/2023','21');</v>
       </c>
       <c r="Y126">
-        <f t="shared" si="16"/>
+        <f>S126/10</f>
         <v>2.1</v>
       </c>
     </row>
@@ -9675,40 +9673,40 @@
         <v>6</v>
       </c>
       <c r="K127">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L127" t="s">
-        <v>215</v>
-      </c>
-      <c r="M127" s="6">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M127" s="1">
         <v>14</v>
       </c>
       <c r="N127" t="s">
         <v>215</v>
       </c>
       <c r="O127">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P127" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q127">
         <v>2023</v>
       </c>
-      <c r="P127" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q127">
+      <c r="R127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S127">
         <v>20</v>
       </c>
-      <c r="R127" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S127">
-        <f>S123+1</f>
-        <v>7</v>
-      </c>
       <c r="T127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U127" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('27',NULL,'6','8/14/2023','20','7');</v>
+        <f>_xlfn.CONCAT(B127:T127)</f>
+        <v>insert into  inventario values ('27',NULL,'6','7','14/8/2023','20');</v>
       </c>
       <c r="Y127">
         <v>20</v>
@@ -9743,11 +9741,11 @@
         <v>6</v>
       </c>
       <c r="K128">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L128" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M128">
         <v>15</v>
@@ -9756,30 +9754,30 @@
         <v>215</v>
       </c>
       <c r="O128">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P128" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q128">
         <v>2023</v>
       </c>
-      <c r="P128" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q128">
+      <c r="R128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S128">
         <v>20</v>
       </c>
-      <c r="R128" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S128">
-        <f>S124+1</f>
-        <v>7</v>
-      </c>
       <c r="T128" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U128" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('28',NULL,'1','8/15/2023','20','7');</v>
+        <f>_xlfn.CONCAT(B128:T128)</f>
+        <v>insert into  inventario values ('28',NULL,'1','7','15/8/2023','20');</v>
       </c>
       <c r="Y128">
-        <f t="shared" si="16"/>
+        <f>S128/10</f>
         <v>2</v>
       </c>
     </row>
@@ -9812,40 +9810,40 @@
         <v>6</v>
       </c>
       <c r="K129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="L129" t="s">
-        <v>215</v>
-      </c>
-      <c r="M129" s="6">
+      <c r="L129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M129" s="1">
         <v>16</v>
       </c>
       <c r="N129" t="s">
         <v>215</v>
       </c>
       <c r="O129">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P129" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q129">
         <v>2023</v>
       </c>
-      <c r="P129" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q129">
+      <c r="R129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S129">
         <v>17</v>
       </c>
-      <c r="R129" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S129">
-        <f>S125+1</f>
-        <v>8</v>
-      </c>
       <c r="T129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U129" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('29',NULL,'2','8/16/2023','17','8');</v>
+        <f>_xlfn.CONCAT(B129:T129)</f>
+        <v>insert into  inventario values ('29',NULL,'2','8','16/8/2023','17');</v>
       </c>
       <c r="Y129">
         <v>17</v>
@@ -9880,11 +9878,11 @@
         <v>6</v>
       </c>
       <c r="K130">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="L130" t="s">
-        <v>215</v>
+      <c r="L130" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M130">
         <v>17</v>
@@ -9893,27 +9891,27 @@
         <v>215</v>
       </c>
       <c r="O130">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P130" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q130">
         <v>2023</v>
       </c>
-      <c r="P130" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q130">
+      <c r="R130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S130">
         <v>18</v>
       </c>
-      <c r="R130" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S130">
-        <f>S126+1</f>
-        <v>8</v>
-      </c>
       <c r="T130" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U130" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('30',NULL,'4','8/17/2023','18','8');</v>
+        <f>_xlfn.CONCAT(B130:T130)</f>
+        <v>insert into  inventario values ('30',NULL,'4','8','17/8/2023','18');</v>
       </c>
       <c r="Y130">
         <v>18</v>
@@ -9948,43 +9946,43 @@
         <v>6</v>
       </c>
       <c r="K131">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="L131" t="s">
-        <v>215</v>
-      </c>
-      <c r="M131" s="6">
+      <c r="L131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M131" s="1">
         <v>18</v>
       </c>
       <c r="N131" t="s">
         <v>215</v>
       </c>
       <c r="O131">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P131" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q131">
         <v>2023</v>
       </c>
-      <c r="P131" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q131">
+      <c r="R131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S131">
         <v>18</v>
       </c>
-      <c r="R131" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S131">
-        <f>S127+1</f>
-        <v>8</v>
-      </c>
       <c r="T131" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U131" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('31',NULL,'5','8/18/2023','18','8');</v>
+        <f>_xlfn.CONCAT(B131:T131)</f>
+        <v>insert into  inventario values ('31',NULL,'5','8','18/8/2023','18');</v>
       </c>
       <c r="Y131">
-        <f t="shared" si="16"/>
+        <f>S131/10</f>
         <v>1.8</v>
       </c>
     </row>
@@ -10017,11 +10015,11 @@
         <v>6</v>
       </c>
       <c r="K132">
-        <f t="shared" si="17"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="L132" t="s">
-        <v>215</v>
+      <c r="L132" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M132">
         <v>19</v>
@@ -10030,27 +10028,27 @@
         <v>215</v>
       </c>
       <c r="O132">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P132" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q132">
         <v>2023</v>
       </c>
-      <c r="P132" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q132">
+      <c r="R132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S132">
         <v>17</v>
       </c>
-      <c r="R132" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S132">
-        <f>S128+1</f>
-        <v>8</v>
-      </c>
       <c r="T132" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U132" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('32',NULL,'6','8/19/2023','17','8');</v>
+        <f>_xlfn.CONCAT(B132:T132)</f>
+        <v>insert into  inventario values ('32',NULL,'6','8','19/8/2023','17');</v>
       </c>
       <c r="Y132">
         <v>17</v>
@@ -10085,43 +10083,43 @@
         <v>6</v>
       </c>
       <c r="K133">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
-      <c r="L133" t="s">
-        <v>215</v>
-      </c>
-      <c r="M133" s="6">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M133" s="1">
         <v>20</v>
       </c>
       <c r="N133" t="s">
         <v>215</v>
       </c>
       <c r="O133">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="P133" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q133">
         <v>2023</v>
       </c>
-      <c r="P133" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q133">
+      <c r="R133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S133">
         <v>20</v>
       </c>
-      <c r="R133" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S133">
-        <f>S129+1</f>
-        <v>9</v>
-      </c>
       <c r="T133" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U133" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('33',NULL,'1','8/20/2023','20','9');</v>
+        <f>_xlfn.CONCAT(B133:T133)</f>
+        <v>insert into  inventario values ('33',NULL,'1','9','20/8/2023','20');</v>
       </c>
       <c r="Y133">
-        <f t="shared" si="16"/>
+        <f>S133/10</f>
         <v>2</v>
       </c>
     </row>
@@ -10154,43 +10152,43 @@
         <v>6</v>
       </c>
       <c r="K134">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L134" t="s">
-        <v>215</v>
-      </c>
-      <c r="M134" s="6">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M134" s="1">
         <v>10</v>
       </c>
       <c r="N134" t="s">
         <v>215</v>
       </c>
       <c r="O134">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P134" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q134">
         <v>2023</v>
       </c>
-      <c r="P134" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q134">
+      <c r="R134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S134">
         <v>21</v>
       </c>
-      <c r="R134" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S134">
-        <f>S130+1</f>
-        <v>9</v>
-      </c>
       <c r="T134" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U134" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('34',NULL,'1','9/10/2023','21','9');</v>
+        <f>_xlfn.CONCAT(B134:T134)</f>
+        <v>insert into  inventario values ('34',NULL,'1','9','10/9/2023','21');</v>
       </c>
       <c r="Y134">
-        <f t="shared" si="16"/>
+        <f>S134/10</f>
         <v>2.1</v>
       </c>
     </row>
@@ -10223,11 +10221,11 @@
         <v>6</v>
       </c>
       <c r="K135">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L135" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M135">
         <v>11</v>
@@ -10236,27 +10234,27 @@
         <v>215</v>
       </c>
       <c r="O135">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P135" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q135">
         <v>2023</v>
       </c>
-      <c r="P135" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q135">
+      <c r="R135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S135">
         <v>20</v>
       </c>
-      <c r="R135" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S135">
-        <f>S131+1</f>
-        <v>9</v>
-      </c>
       <c r="T135" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U135" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('35',NULL,'2','9/11/2023','20','9');</v>
+        <f>_xlfn.CONCAT(B135:T135)</f>
+        <v>insert into  inventario values ('35',NULL,'2','9','11/9/2023','20');</v>
       </c>
       <c r="Y135">
         <v>20</v>
@@ -10291,43 +10289,43 @@
         <v>6</v>
       </c>
       <c r="K136">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L136" t="s">
-        <v>215</v>
-      </c>
-      <c r="M136" s="6">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M136" s="1">
         <v>12</v>
       </c>
       <c r="N136" t="s">
         <v>215</v>
       </c>
       <c r="O136">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P136" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q136">
         <v>2023</v>
       </c>
-      <c r="P136" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q136">
+      <c r="R136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S136">
         <v>20</v>
       </c>
-      <c r="R136" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S136">
-        <f>S132+1</f>
-        <v>9</v>
-      </c>
       <c r="T136" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U136" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('36',NULL,'4','9/12/2023','20','9');</v>
+        <f>_xlfn.CONCAT(B136:T136)</f>
+        <v>insert into  inventario values ('36',NULL,'4','9','12/9/2023','20');</v>
       </c>
       <c r="Y136">
-        <f t="shared" si="16"/>
+        <f>S136/10</f>
         <v>2</v>
       </c>
     </row>
@@ -10360,11 +10358,11 @@
         <v>6</v>
       </c>
       <c r="K137">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L137" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M137">
         <v>13</v>
@@ -10373,27 +10371,27 @@
         <v>215</v>
       </c>
       <c r="O137">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P137" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q137">
         <v>2023</v>
       </c>
-      <c r="P137" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q137">
+      <c r="R137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S137">
         <v>17</v>
       </c>
-      <c r="R137" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S137">
-        <f>S133+1</f>
-        <v>10</v>
-      </c>
       <c r="T137" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U137" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('37',NULL,'5','9/13/2023','17','10');</v>
+        <f>_xlfn.CONCAT(B137:T137)</f>
+        <v>insert into  inventario values ('37',NULL,'5','10','13/9/2023','17');</v>
       </c>
       <c r="Y137">
         <v>17</v>
@@ -10428,40 +10426,40 @@
         <v>6</v>
       </c>
       <c r="K138">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L138" t="s">
-        <v>215</v>
-      </c>
-      <c r="M138" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M138" s="1">
         <v>14</v>
       </c>
       <c r="N138" t="s">
         <v>215</v>
       </c>
       <c r="O138">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P138" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q138">
         <v>2023</v>
       </c>
-      <c r="P138" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q138">
+      <c r="R138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S138">
         <v>18</v>
       </c>
-      <c r="R138" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S138">
-        <f>S134+1</f>
-        <v>10</v>
-      </c>
       <c r="T138" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U138" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('38',NULL,'6','9/14/2023','18','10');</v>
+        <f>_xlfn.CONCAT(B138:T138)</f>
+        <v>insert into  inventario values ('38',NULL,'6','10','14/9/2023','18');</v>
       </c>
       <c r="Y138">
         <v>18</v>
@@ -10496,11 +10494,11 @@
         <v>6</v>
       </c>
       <c r="K139">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L139" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M139">
         <v>15</v>
@@ -10509,27 +10507,27 @@
         <v>215</v>
       </c>
       <c r="O139">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P139" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q139">
         <v>2023</v>
       </c>
-      <c r="P139" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q139">
+      <c r="R139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S139">
         <v>18</v>
       </c>
-      <c r="R139" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S139">
-        <f>S135+1</f>
-        <v>10</v>
-      </c>
       <c r="T139" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U139" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('39',NULL,'1','9/15/2023','18','10');</v>
+        <f>_xlfn.CONCAT(B139:T139)</f>
+        <v>insert into  inventario values ('39',NULL,'1','10','15/9/2023','18');</v>
       </c>
       <c r="Y139">
         <v>18</v>
@@ -10564,40 +10562,40 @@
         <v>6</v>
       </c>
       <c r="K140">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L140" t="s">
-        <v>215</v>
-      </c>
-      <c r="M140" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M140" s="1">
         <v>16</v>
       </c>
       <c r="N140" t="s">
         <v>215</v>
       </c>
       <c r="O140">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P140" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q140">
         <v>2023</v>
       </c>
-      <c r="P140" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q140">
+      <c r="R140" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S140">
         <v>17</v>
       </c>
-      <c r="R140" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S140">
-        <f>S136+1</f>
-        <v>10</v>
-      </c>
       <c r="T140" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U140" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('40',NULL,'2','9/16/2023','17','10');</v>
+        <f>_xlfn.CONCAT(B140:T140)</f>
+        <v>insert into  inventario values ('40',NULL,'2','10','16/9/2023','17');</v>
       </c>
       <c r="Y140">
         <v>17</v>
@@ -10632,11 +10630,11 @@
         <v>6</v>
       </c>
       <c r="K141">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L141" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M141">
         <v>17</v>
@@ -10645,30 +10643,30 @@
         <v>215</v>
       </c>
       <c r="O141">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P141" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q141">
         <v>2023</v>
       </c>
-      <c r="P141" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q141">
+      <c r="R141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S141">
         <v>18</v>
       </c>
-      <c r="R141" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S141">
-        <f>S137+1</f>
-        <v>11</v>
-      </c>
       <c r="T141" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U141" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('41',NULL,'4','9/17/2023','18','11');</v>
+        <f>_xlfn.CONCAT(B141:T141)</f>
+        <v>insert into  inventario values ('41',NULL,'4','11','17/9/2023','18');</v>
       </c>
       <c r="Y141">
-        <f t="shared" si="16"/>
+        <f>S141/10</f>
         <v>1.8</v>
       </c>
     </row>
@@ -10701,43 +10699,43 @@
         <v>6</v>
       </c>
       <c r="K142">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L142" t="s">
-        <v>215</v>
-      </c>
-      <c r="M142" s="6">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M142" s="1">
         <v>18</v>
       </c>
       <c r="N142" t="s">
         <v>215</v>
       </c>
       <c r="O142">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P142" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q142">
         <v>2023</v>
       </c>
-      <c r="P142" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q142">
+      <c r="R142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S142">
         <v>23</v>
       </c>
-      <c r="R142" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S142">
-        <f>S138+1</f>
-        <v>11</v>
-      </c>
       <c r="T142" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U142" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('42',NULL,'5','9/18/2023','23','11');</v>
+        <f>_xlfn.CONCAT(B142:T142)</f>
+        <v>insert into  inventario values ('42',NULL,'5','11','18/9/2023','23');</v>
       </c>
       <c r="Y142">
-        <f t="shared" si="16"/>
+        <f>S142/10</f>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -10770,11 +10768,11 @@
         <v>6</v>
       </c>
       <c r="K143">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L143" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M143">
         <v>19</v>
@@ -10783,30 +10781,30 @@
         <v>215</v>
       </c>
       <c r="O143">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P143" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q143">
         <v>2023</v>
       </c>
-      <c r="P143" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q143">
+      <c r="R143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S143">
         <v>18</v>
       </c>
-      <c r="R143" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S143">
-        <f>S139+1</f>
-        <v>11</v>
-      </c>
       <c r="T143" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U143" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('43',NULL,'6','9/19/2023','18','11');</v>
+        <f>_xlfn.CONCAT(B143:T143)</f>
+        <v>insert into  inventario values ('43',NULL,'6','11','19/9/2023','18');</v>
       </c>
       <c r="Y143">
-        <f t="shared" si="16"/>
+        <f>S143/10</f>
         <v>1.8</v>
       </c>
     </row>
@@ -10839,43 +10837,43 @@
         <v>6</v>
       </c>
       <c r="K144">
-        <f t="shared" si="17"/>
-        <v>9</v>
-      </c>
-      <c r="L144" t="s">
-        <v>215</v>
-      </c>
-      <c r="M144" s="6">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M144" s="1">
         <v>20</v>
       </c>
       <c r="N144" t="s">
         <v>215</v>
       </c>
       <c r="O144">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="P144" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q144">
         <v>2023</v>
       </c>
-      <c r="P144" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q144">
+      <c r="R144" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S144">
         <v>17</v>
       </c>
-      <c r="R144" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S144">
-        <f>S140+1</f>
-        <v>11</v>
-      </c>
       <c r="T144" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U144" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('44',NULL,'1','9/20/2023','17','11');</v>
+        <f>_xlfn.CONCAT(B144:T144)</f>
+        <v>insert into  inventario values ('44',NULL,'1','11','20/9/2023','17');</v>
       </c>
       <c r="Y144">
-        <f t="shared" si="16"/>
+        <f>S144/10</f>
         <v>1.7</v>
       </c>
     </row>
@@ -10908,43 +10906,43 @@
         <v>6</v>
       </c>
       <c r="K145">
-        <f t="shared" si="17"/>
-        <v>10</v>
-      </c>
-      <c r="L145" t="s">
-        <v>215</v>
-      </c>
-      <c r="M145" s="6">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M145" s="1">
         <v>10</v>
       </c>
       <c r="N145" t="s">
         <v>215</v>
       </c>
       <c r="O145">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="P145" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q145">
         <v>2023</v>
       </c>
-      <c r="P145" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q145">
+      <c r="R145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S145">
         <v>25</v>
       </c>
-      <c r="R145" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S145">
-        <f>S141+1</f>
-        <v>12</v>
-      </c>
       <c r="T145" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U145" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('45',NULL,'1','10/10/2023','25','12');</v>
+        <f>_xlfn.CONCAT(B145:T145)</f>
+        <v>insert into  inventario values ('45',NULL,'1','12','10/10/2023','25');</v>
       </c>
       <c r="Y145">
-        <f t="shared" si="16"/>
+        <f>S145/10</f>
         <v>2.5</v>
       </c>
     </row>
@@ -10977,11 +10975,11 @@
         <v>6</v>
       </c>
       <c r="K146">
-        <f t="shared" si="17"/>
-        <v>10</v>
-      </c>
-      <c r="L146" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L146" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M146">
         <v>11</v>
@@ -10990,30 +10988,30 @@
         <v>215</v>
       </c>
       <c r="O146">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="P146" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q146">
         <v>2023</v>
       </c>
-      <c r="P146" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q146">
+      <c r="R146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S146">
         <v>18</v>
       </c>
-      <c r="R146" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S146">
-        <f>S142+1</f>
-        <v>12</v>
-      </c>
       <c r="T146" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U146" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('46',NULL,'2','10/11/2023','18','12');</v>
+        <f>_xlfn.CONCAT(B146:T146)</f>
+        <v>insert into  inventario values ('46',NULL,'2','12','11/10/2023','18');</v>
       </c>
       <c r="Y146">
-        <f t="shared" si="16"/>
+        <f>S146/10</f>
         <v>1.8</v>
       </c>
     </row>
@@ -11046,43 +11044,43 @@
         <v>6</v>
       </c>
       <c r="K147">
-        <f t="shared" si="17"/>
-        <v>10</v>
-      </c>
-      <c r="L147" t="s">
-        <v>215</v>
-      </c>
-      <c r="M147" s="6">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M147" s="1">
         <v>12</v>
       </c>
       <c r="N147" t="s">
         <v>215</v>
       </c>
       <c r="O147">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="P147" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q147">
         <v>2023</v>
       </c>
-      <c r="P147" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q147">
+      <c r="R147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S147">
         <v>15</v>
       </c>
-      <c r="R147" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S147">
-        <f>S143+1</f>
-        <v>12</v>
-      </c>
       <c r="T147" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U147" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('47',NULL,'4','10/12/2023','15','12');</v>
+        <f>_xlfn.CONCAT(B147:T147)</f>
+        <v>insert into  inventario values ('47',NULL,'4','12','12/10/2023','15');</v>
       </c>
       <c r="Y147">
-        <f t="shared" si="16"/>
+        <f>S147/10</f>
         <v>1.5</v>
       </c>
     </row>
@@ -11115,11 +11113,11 @@
         <v>6</v>
       </c>
       <c r="K148">
-        <f t="shared" si="17"/>
-        <v>10</v>
-      </c>
-      <c r="L148" t="s">
-        <v>215</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="M148">
         <v>13</v>
@@ -11128,30 +11126,30 @@
         <v>215</v>
       </c>
       <c r="O148">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="P148" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q148">
         <v>2023</v>
       </c>
-      <c r="P148" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q148">
+      <c r="R148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S148">
         <v>30</v>
       </c>
-      <c r="R148" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S148">
-        <f>S144+1</f>
-        <v>12</v>
-      </c>
       <c r="T148" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U148" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into  inventario values ('48',NULL,'5','10/13/2023','30','12');</v>
+        <f>_xlfn.CONCAT(B148:T148)</f>
+        <v>insert into  inventario values ('48',NULL,'5','12','13/10/2023','30');</v>
       </c>
       <c r="Y148">
-        <f t="shared" si="16"/>
+        <f>S148/10</f>
         <v>3</v>
       </c>
     </row>
@@ -11177,7 +11175,7 @@
         <v>6</v>
       </c>
       <c r="G151">
-        <f>K140+1</f>
+        <f>O140+1</f>
         <v>10</v>
       </c>
       <c r="H151" t="s">
@@ -11210,7 +11208,7 @@
         <v>7</v>
       </c>
       <c r="U151" t="str">
-        <f t="shared" ref="U151:U153" si="19">_xlfn.CONCAT(B151:T151)</f>
+        <f>_xlfn.CONCAT(B151:T151)</f>
         <v>insert into  ensamble values ('1','10/13/2023',true,'301');</v>
       </c>
     </row>
@@ -11231,7 +11229,7 @@
         <v>6</v>
       </c>
       <c r="G152">
-        <f t="shared" ref="G152:G153" si="20">K141+1</f>
+        <f>O141+1</f>
         <v>10</v>
       </c>
       <c r="H152" t="s">
@@ -11264,7 +11262,7 @@
         <v>121</v>
       </c>
       <c r="U152" t="str">
-        <f t="shared" si="19"/>
+        <f>_xlfn.CONCAT(B152:T152)</f>
         <v>insert into  ensamble values ('2','10/14/2023',false,NULL);</v>
       </c>
     </row>
@@ -11285,7 +11283,7 @@
         <v>6</v>
       </c>
       <c r="G153">
-        <f t="shared" si="20"/>
+        <f>O142+1</f>
         <v>10</v>
       </c>
       <c r="H153" t="s">
@@ -11318,7 +11316,7 @@
         <v>121</v>
       </c>
       <c r="U153" t="str">
-        <f t="shared" si="19"/>
+        <f>_xlfn.CONCAT(B153:T153)</f>
         <v>insert into  ensamble values ('3','10/15/2023',false,NULL);</v>
       </c>
     </row>
@@ -11382,7 +11380,7 @@
         <v>7</v>
       </c>
       <c r="U158" t="str">
-        <f t="shared" ref="U158:U163" si="21">_xlfn.CONCAT(B158:T158)</f>
+        <f>_xlfn.CONCAT(B158:T158)</f>
         <v>insert into  detalleensamble values ('1','1','1');</v>
       </c>
     </row>
@@ -11415,7 +11413,7 @@
         <v>7</v>
       </c>
       <c r="U159" t="str">
-        <f t="shared" si="21"/>
+        <f>_xlfn.CONCAT(B159:T159)</f>
         <v>insert into  detalleensamble values ('2','1','5');</v>
       </c>
     </row>
@@ -11448,7 +11446,7 @@
         <v>7</v>
       </c>
       <c r="U160" t="str">
-        <f t="shared" si="21"/>
+        <f>_xlfn.CONCAT(B160:T160)</f>
         <v>insert into  detalleensamble values ('3','1','9');</v>
       </c>
     </row>
@@ -11481,7 +11479,7 @@
         <v>7</v>
       </c>
       <c r="U161" t="str">
-        <f t="shared" si="21"/>
+        <f>_xlfn.CONCAT(B161:T161)</f>
         <v>insert into  detalleensamble values ('4','1','13');</v>
       </c>
     </row>
@@ -11514,7 +11512,7 @@
         <v>7</v>
       </c>
       <c r="U162" t="str">
-        <f t="shared" si="21"/>
+        <f>_xlfn.CONCAT(B162:T162)</f>
         <v>insert into  detalleensamble values ('5','1','17');</v>
       </c>
     </row>
@@ -11548,7 +11546,7 @@
         <v>7</v>
       </c>
       <c r="U163" t="str">
-        <f t="shared" si="21"/>
+        <f>_xlfn.CONCAT(B163:T163)</f>
         <v>insert into  detalleensamble values ('6','2','21');</v>
       </c>
     </row>
@@ -11569,7 +11567,7 @@
         <v>6</v>
       </c>
       <c r="G164">
-        <f t="shared" ref="G164:G172" si="22">G159+1</f>
+        <f t="shared" ref="G164:G172" si="7">G159+1</f>
         <v>2</v>
       </c>
       <c r="H164" s="1" t="s">
@@ -11582,7 +11580,7 @@
         <v>7</v>
       </c>
       <c r="U164" t="str">
-        <f t="shared" ref="U164:U171" si="23">_xlfn.CONCAT(B164:T164)</f>
+        <f>_xlfn.CONCAT(B164:T164)</f>
         <v>insert into  detalleensamble values ('7','2','25');</v>
       </c>
     </row>
@@ -11603,7 +11601,7 @@
         <v>6</v>
       </c>
       <c r="G165">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H165" s="1" t="s">
@@ -11616,7 +11614,7 @@
         <v>7</v>
       </c>
       <c r="U165" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B165:T165)</f>
         <v>insert into  detalleensamble values ('8','2','29');</v>
       </c>
     </row>
@@ -11637,7 +11635,7 @@
         <v>6</v>
       </c>
       <c r="G166">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H166" s="1" t="s">
@@ -11650,7 +11648,7 @@
         <v>7</v>
       </c>
       <c r="U166" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B166:T166)</f>
         <v>insert into  detalleensamble values ('9','2','33');</v>
       </c>
     </row>
@@ -11671,7 +11669,7 @@
         <v>6</v>
       </c>
       <c r="G167">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="H167" s="1" t="s">
@@ -11684,7 +11682,7 @@
         <v>7</v>
       </c>
       <c r="U167" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B167:T167)</f>
         <v>insert into  detalleensamble values ('10','2','37');</v>
       </c>
     </row>
@@ -11705,7 +11703,7 @@
         <v>6</v>
       </c>
       <c r="G168">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="H168" s="1" t="s">
@@ -11718,7 +11716,7 @@
         <v>7</v>
       </c>
       <c r="U168" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B168:T168)</f>
         <v>insert into  detalleensamble values ('11','3','41');</v>
       </c>
     </row>
@@ -11739,7 +11737,7 @@
         <v>6</v>
       </c>
       <c r="G169">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="H169" s="1" t="s">
@@ -11752,7 +11750,7 @@
         <v>7</v>
       </c>
       <c r="U169" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B169:T169)</f>
         <v>insert into  detalleensamble values ('12','3','45');</v>
       </c>
     </row>
@@ -11773,7 +11771,7 @@
         <v>6</v>
       </c>
       <c r="G170">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="H170" s="1" t="s">
@@ -11786,7 +11784,7 @@
         <v>7</v>
       </c>
       <c r="U170" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B170:T170)</f>
         <v>insert into  detalleensamble values ('13','3','2');</v>
       </c>
     </row>
@@ -11807,7 +11805,7 @@
         <v>6</v>
       </c>
       <c r="G171">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="H171" s="1" t="s">
@@ -11820,7 +11818,7 @@
         <v>7</v>
       </c>
       <c r="U171" t="str">
-        <f t="shared" si="23"/>
+        <f>_xlfn.CONCAT(B171:T171)</f>
         <v>insert into  detalleensamble values ('14','3','6');</v>
       </c>
     </row>
@@ -11841,7 +11839,7 @@
         <v>6</v>
       </c>
       <c r="G172">
-        <f t="shared" si="22"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="H172" s="1" t="s">
@@ -11854,7 +11852,7 @@
         <v>7</v>
       </c>
       <c r="U172" t="str">
-        <f t="shared" ref="U172" si="24">_xlfn.CONCAT(B172:T172)</f>
+        <f>_xlfn.CONCAT(B172:T172)</f>
         <v>insert into  detalleensamble values ('15','3','10');</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se actualizo estructura  y datos de la BD 3.0
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\OneDrive\Documentos\Trabajos Universidad\ModuloFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957CEBAA-CE03-4922-A8E0-FE9D88452452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B51F94-030F-40ED-BCE7-AA4052F10F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{D6C15466-4649-4A22-BCE7-3BF8AFBFC14E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="223">
   <si>
     <t>Telefono Casa</t>
   </si>
@@ -675,15 +675,6 @@
     <t>FCHEVE</t>
   </si>
   <si>
-    <t>VALOR</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>IDREF</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
@@ -709,6 +700,12 @@
   </si>
   <si>
     <t>NO INVEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,' </t>
+  </si>
+  <si>
+    <t>Id REF</t>
   </si>
 </sst>
 </file>
@@ -773,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -782,6 +779,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3650,8 +3648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530204FE-A160-4075-98A7-610FC6631479}">
   <dimension ref="B2:Y172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K114" workbookViewId="0">
-      <selection activeCell="U101" sqref="U101:U148"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="M168" sqref="M168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,7 +3725,7 @@
         <v>7</v>
       </c>
       <c r="T2" t="str">
-        <f>_xlfn.CONCAT(B2:R2)</f>
+        <f t="shared" ref="T2:T12" si="0">_xlfn.CONCAT(B2:R2)</f>
         <v>insert into empleado values ('101','1','Andrea','Andes','1023456789','1/06/2022','2/09/2000');</v>
       </c>
     </row>
@@ -3784,7 +3782,7 @@
         <v>7</v>
       </c>
       <c r="T3" t="str">
-        <f>_xlfn.CONCAT(B3:R3)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('102','1','Anuel','Ara','1234567899','2/06/2022','3/10/1984');</v>
       </c>
     </row>
@@ -3842,7 +3840,7 @@
         <v>7</v>
       </c>
       <c r="T4" t="str">
-        <f>_xlfn.CONCAT(B4:R4)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('103','4','Ana','Aguila','1234567900','3/06/2023','4/08/1985');</v>
       </c>
     </row>
@@ -3899,7 +3897,7 @@
         <v>7</v>
       </c>
       <c r="T5" t="str">
-        <f>_xlfn.CONCAT(B5:R5)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('201','1','Bruno','Baldomero','1234567900','1/06/2023','2/09/2000');</v>
       </c>
     </row>
@@ -3938,7 +3936,7 @@
         <v>6</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6" si="0">M5+1</f>
+        <f t="shared" ref="M6" si="1">M5+1</f>
         <v>1234567901</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -3957,7 +3955,7 @@
         <v>7</v>
       </c>
       <c r="T6" t="str">
-        <f>_xlfn.CONCAT(B6:R6)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('202','1','Benito','Baez','1234567901','2/06/2023','3/10/1995');</v>
       </c>
     </row>
@@ -4014,7 +4012,7 @@
         <v>7</v>
       </c>
       <c r="T7" t="str">
-        <f>_xlfn.CONCAT(B7:R7)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('203','1','Brenda','Basilio','1234567901','4/06/2022','3/10/1996');</v>
       </c>
     </row>
@@ -4053,7 +4051,7 @@
         <v>6</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8" si="1">M7+1</f>
+        <f t="shared" ref="M8" si="2">M7+1</f>
         <v>1234567902</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -4072,7 +4070,7 @@
         <v>7</v>
       </c>
       <c r="T8" t="str">
-        <f>_xlfn.CONCAT(B8:R8)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('301','4','Carla','Casto','1234567902','5/06/2022','3/10/1997');</v>
       </c>
     </row>
@@ -4129,7 +4127,7 @@
         <v>7</v>
       </c>
       <c r="T9" t="str">
-        <f>_xlfn.CONCAT(B9:R9)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('302','4','Carlo','Castro','1234567902','6/06/2022','3/10/1998');</v>
       </c>
     </row>
@@ -4168,7 +4166,7 @@
         <v>6</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10" si="2">M9+1</f>
+        <f t="shared" ref="M10" si="3">M9+1</f>
         <v>1234567903</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -4187,7 +4185,7 @@
         <v>7</v>
       </c>
       <c r="T10" t="str">
-        <f>_xlfn.CONCAT(B10:R10)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('303','1','Camilo','Ciel','1234567903','7/06/2022','3/10/1999');</v>
       </c>
     </row>
@@ -4244,7 +4242,7 @@
         <v>7</v>
       </c>
       <c r="T11" t="str">
-        <f>_xlfn.CONCAT(B11:R11)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('304','1','Caleb','Carmelo','1234567903','8/06/2022','3/10/2000');</v>
       </c>
     </row>
@@ -4283,7 +4281,7 @@
         <v>6</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12" si="3">M11+1</f>
+        <f t="shared" ref="M12" si="4">M11+1</f>
         <v>1234567904</v>
       </c>
       <c r="N12" s="1" t="s">
@@ -4302,7 +4300,7 @@
         <v>7</v>
       </c>
       <c r="T12" t="str">
-        <f>_xlfn.CONCAT(B12:R12)</f>
+        <f t="shared" si="0"/>
         <v>insert into empleado values ('305','4','Camilo','Ciro','1234567904','9/06/2022','3/10/2001');</v>
       </c>
     </row>
@@ -4396,7 +4394,7 @@
         <v>121</v>
       </c>
       <c r="P15" t="str">
-        <f>_xlfn.CONCAT(B15:N15)</f>
+        <f t="shared" ref="P15:P24" si="5">_xlfn.CONCAT(B15:N15)</f>
         <v>insert into historiacargo values ('2','1','102','2/06/2022','1/06/2024');</v>
       </c>
     </row>
@@ -4441,7 +4439,7 @@
         <v>121</v>
       </c>
       <c r="P16" t="str">
-        <f>_xlfn.CONCAT(B16:N16)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('3','1','103','3/06/2023','2/06/2025');</v>
       </c>
     </row>
@@ -4486,7 +4484,7 @@
         <v>121</v>
       </c>
       <c r="P17" t="str">
-        <f>_xlfn.CONCAT(B17:N17)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('4','2','201','1/06/2023','31/05/2025');</v>
       </c>
     </row>
@@ -4531,7 +4529,7 @@
         <v>121</v>
       </c>
       <c r="P18" t="str">
-        <f>_xlfn.CONCAT(B18:N18)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('5','2','202','2/06/2023','1/06/2025');</v>
       </c>
     </row>
@@ -4576,7 +4574,7 @@
         <v>121</v>
       </c>
       <c r="P19" t="str">
-        <f>_xlfn.CONCAT(B19:N19)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('6','2','203','4/06/2022','3/06/2024');</v>
       </c>
     </row>
@@ -4621,7 +4619,7 @@
         <v>121</v>
       </c>
       <c r="P20" t="str">
-        <f>_xlfn.CONCAT(B20:N20)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('7','3','301','5/06/2022','4/06/2024');</v>
       </c>
     </row>
@@ -4666,7 +4664,7 @@
         <v>121</v>
       </c>
       <c r="P21" t="str">
-        <f>_xlfn.CONCAT(B21:N21)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('8','3','302','6/06/2022','5/06/2024');</v>
       </c>
     </row>
@@ -4711,7 +4709,7 @@
         <v>121</v>
       </c>
       <c r="P22" t="str">
-        <f>_xlfn.CONCAT(B22:N22)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('9','3','303','7/06/2022','6/06/2024');</v>
       </c>
     </row>
@@ -4756,7 +4754,7 @@
         <v>121</v>
       </c>
       <c r="P23" t="str">
-        <f>_xlfn.CONCAT(B23:N23)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('10','3','304','8/06/2022','7/06/2024');</v>
       </c>
     </row>
@@ -4801,7 +4799,7 @@
         <v>121</v>
       </c>
       <c r="P24" t="str">
-        <f>_xlfn.CONCAT(B24:N24)</f>
+        <f t="shared" si="5"/>
         <v>insert into historiacargo values ('11','3','305','9/06/2022','8/06/2024');</v>
       </c>
     </row>
@@ -4967,7 +4965,7 @@
         <v>6</v>
       </c>
       <c r="Q28">
-        <f t="shared" ref="Q28:Q29" si="4">Q27+1</f>
+        <f t="shared" ref="Q28:Q29" si="6">Q27+1</f>
         <v>60000003</v>
       </c>
       <c r="R28" s="1" t="s">
@@ -5025,7 +5023,7 @@
         <v>6</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>60000004</v>
       </c>
       <c r="R29" s="1" t="s">
@@ -5077,7 +5075,7 @@
         <v>7</v>
       </c>
       <c r="N31" t="str">
-        <f>_xlfn.CONCAT(B31:L31)</f>
+        <f t="shared" ref="N31:N42" si="7">_xlfn.CONCAT(B31:L31)</f>
         <v>insert into referenciaelemento values ('1','1','Obs: Board A');</v>
       </c>
       <c r="O31" s="2"/>
@@ -5115,7 +5113,7 @@
         <v>7</v>
       </c>
       <c r="N32" t="str">
-        <f>_xlfn.CONCAT(B32:L32)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('2','1','Obs: Board B');</v>
       </c>
       <c r="O32" s="2"/>
@@ -5153,7 +5151,7 @@
         <v>7</v>
       </c>
       <c r="N33" t="str">
-        <f>_xlfn.CONCAT(B33:L33)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('3','1','Obs: Board C');</v>
       </c>
       <c r="O33" s="2"/>
@@ -5191,7 +5189,7 @@
         <v>7</v>
       </c>
       <c r="N34" t="str">
-        <f>_xlfn.CONCAT(B34:L34)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('4','2','Obs: Procesador A');</v>
       </c>
       <c r="O34" s="2"/>
@@ -5229,7 +5227,7 @@
         <v>7</v>
       </c>
       <c r="N35" t="str">
-        <f>_xlfn.CONCAT(B35:L35)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('5','2','Obs: Procesador B');</v>
       </c>
       <c r="O35" s="2"/>
@@ -5267,7 +5265,7 @@
         <v>7</v>
       </c>
       <c r="N36" t="str">
-        <f>_xlfn.CONCAT(B36:L36)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('6','2','Obs: Procesador C');</v>
       </c>
       <c r="O36" s="2"/>
@@ -5305,7 +5303,7 @@
         <v>7</v>
       </c>
       <c r="N37" t="str">
-        <f>_xlfn.CONCAT(B37:L37)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('7','3','Obs: Ram A');</v>
       </c>
       <c r="O37" s="2"/>
@@ -5343,7 +5341,7 @@
         <v>7</v>
       </c>
       <c r="N38" t="str">
-        <f>_xlfn.CONCAT(B38:L38)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('8','3','Obs: Ram B');</v>
       </c>
       <c r="O38" s="2"/>
@@ -5381,7 +5379,7 @@
         <v>7</v>
       </c>
       <c r="N39" t="str">
-        <f>_xlfn.CONCAT(B39:L39)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('9','4','Obs: Disco Duro A');</v>
       </c>
     </row>
@@ -5417,7 +5415,7 @@
         <v>7</v>
       </c>
       <c r="N40" t="str">
-        <f>_xlfn.CONCAT(B40:L40)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('10','4','Obs: Disco Duro B');</v>
       </c>
     </row>
@@ -5453,7 +5451,7 @@
         <v>7</v>
       </c>
       <c r="N41" t="str">
-        <f>_xlfn.CONCAT(B41:L41)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('11','5','Obs: Fuente de alimentación A');</v>
       </c>
     </row>
@@ -5489,7 +5487,7 @@
         <v>7</v>
       </c>
       <c r="N42" t="str">
-        <f>_xlfn.CONCAT(B42:L42)</f>
+        <f t="shared" si="7"/>
         <v>insert into referenciaelemento values ('12','5','Obs: Fuente de alimentación B');</v>
       </c>
     </row>
@@ -5653,7 +5651,7 @@
         <v>7</v>
       </c>
       <c r="P47" t="str">
-        <f>_xlfn.CONCAT(B47:N47)</f>
+        <f t="shared" ref="P47:P93" si="8">_xlfn.CONCAT(B47:N47)</f>
         <v>insert into refcarac values ('3','2',NULL,'2','AMD');</v>
       </c>
     </row>
@@ -5698,7 +5696,7 @@
         <v>7</v>
       </c>
       <c r="P48" t="str">
-        <f>_xlfn.CONCAT(B48:N48)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('4','2','14','9','3');</v>
       </c>
     </row>
@@ -5743,7 +5741,7 @@
         <v>7</v>
       </c>
       <c r="P49" t="str">
-        <f>_xlfn.CONCAT(B49:N49)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('5','3',NULL,'2','APPLE');</v>
       </c>
     </row>
@@ -5788,7 +5786,7 @@
         <v>7</v>
       </c>
       <c r="P50" t="str">
-        <f>_xlfn.CONCAT(B50:N50)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('6','3',14,'2','4');</v>
       </c>
     </row>
@@ -5833,7 +5831,7 @@
         <v>7</v>
       </c>
       <c r="P51" t="str">
-        <f>_xlfn.CONCAT(B51:N51)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('7','4',NULL,'2','INTEL');</v>
       </c>
     </row>
@@ -5878,7 +5876,7 @@
         <v>7</v>
       </c>
       <c r="P52" t="str">
-        <f>_xlfn.CONCAT(B52:N52)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('8','4','4','4','20');</v>
       </c>
     </row>
@@ -5923,7 +5921,7 @@
         <v>7</v>
       </c>
       <c r="P53" t="str">
-        <f>_xlfn.CONCAT(B53:N53)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('9','4','2','6','5,3');</v>
       </c>
     </row>
@@ -5968,7 +5966,7 @@
         <v>7</v>
       </c>
       <c r="P54" t="str">
-        <f>_xlfn.CONCAT(B54:N54)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('10','4','14','9','2');</v>
       </c>
     </row>
@@ -6013,7 +6011,7 @@
         <v>7</v>
       </c>
       <c r="P55" t="str">
-        <f>_xlfn.CONCAT(B55:N55)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('11','4','8','8','125');</v>
       </c>
     </row>
@@ -6058,7 +6056,7 @@
         <v>7</v>
       </c>
       <c r="P56" t="str">
-        <f>_xlfn.CONCAT(B56:N56)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('12','5',NULL,'2','AMD');</v>
       </c>
     </row>
@@ -6103,7 +6101,7 @@
         <v>7</v>
       </c>
       <c r="P57" t="str">
-        <f>_xlfn.CONCAT(B57:N57)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('13','5','4','4','32');</v>
       </c>
     </row>
@@ -6148,7 +6146,7 @@
         <v>7</v>
       </c>
       <c r="P58" t="str">
-        <f>_xlfn.CONCAT(B58:N58)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('14','5','2','6','3,8');</v>
       </c>
     </row>
@@ -6193,7 +6191,7 @@
         <v>7</v>
       </c>
       <c r="P59" t="str">
-        <f>_xlfn.CONCAT(B59:N59)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('15','5','14','9','3');</v>
       </c>
     </row>
@@ -6238,7 +6236,7 @@
         <v>7</v>
       </c>
       <c r="P60" t="str">
-        <f>_xlfn.CONCAT(B60:N60)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('16','5','8','8','105');</v>
       </c>
     </row>
@@ -6283,7 +6281,7 @@
         <v>7</v>
       </c>
       <c r="P61" t="str">
-        <f>_xlfn.CONCAT(B61:N61)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('17','6',NULL,'2','APPLE');</v>
       </c>
     </row>
@@ -6328,7 +6326,7 @@
         <v>7</v>
       </c>
       <c r="P62" t="str">
-        <f>_xlfn.CONCAT(B62:N62)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('18','6','4','4','12');</v>
       </c>
     </row>
@@ -6373,7 +6371,7 @@
         <v>7</v>
       </c>
       <c r="P63" t="str">
-        <f>_xlfn.CONCAT(B63:N63)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('19','6','2','6','4,5');</v>
       </c>
     </row>
@@ -6418,7 +6416,7 @@
         <v>7</v>
       </c>
       <c r="P64" t="str">
-        <f>_xlfn.CONCAT(B64:N64)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('20','6','14','9','4');</v>
       </c>
     </row>
@@ -6463,7 +6461,7 @@
         <v>7</v>
       </c>
       <c r="P65" t="str">
-        <f>_xlfn.CONCAT(B65:N65)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('21','6','8','8','110');</v>
       </c>
     </row>
@@ -6508,7 +6506,7 @@
         <v>7</v>
       </c>
       <c r="P66" t="str">
-        <f>_xlfn.CONCAT(B66:N66)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('22','7',NULL,'2','Corsair ');</v>
       </c>
     </row>
@@ -6553,7 +6551,7 @@
         <v>7</v>
       </c>
       <c r="P67" t="str">
-        <f>_xlfn.CONCAT(B67:N67)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('23','7',NULL,'1','DDR4');</v>
       </c>
     </row>
@@ -6598,7 +6596,7 @@
         <v>7</v>
       </c>
       <c r="P68" t="str">
-        <f>_xlfn.CONCAT(B68:N68)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('24','7','5','4','16');</v>
       </c>
     </row>
@@ -6643,7 +6641,7 @@
         <v>7</v>
       </c>
       <c r="P69" t="str">
-        <f>_xlfn.CONCAT(B69:N69)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('25','7','1','6','3200');</v>
       </c>
     </row>
@@ -6688,7 +6686,7 @@
         <v>7</v>
       </c>
       <c r="P70" t="str">
-        <f>_xlfn.CONCAT(B70:N70)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('26','7',NULL,'7','16-18-18-36');</v>
       </c>
     </row>
@@ -6733,7 +6731,7 @@
         <v>7</v>
       </c>
       <c r="P71" t="str">
-        <f>_xlfn.CONCAT(B71:N71)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('27','7','7','8','1,35');</v>
       </c>
     </row>
@@ -6778,7 +6776,7 @@
         <v>7</v>
       </c>
       <c r="P72" t="str">
-        <f>_xlfn.CONCAT(B72:N72)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('28','8',NULL,'2','Kingston ');</v>
       </c>
     </row>
@@ -6823,7 +6821,7 @@
         <v>7</v>
       </c>
       <c r="P73" t="str">
-        <f>_xlfn.CONCAT(B73:N73)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('29','8',NULL,'1','DDR4');</v>
       </c>
     </row>
@@ -6868,7 +6866,7 @@
         <v>7</v>
       </c>
       <c r="P74" t="str">
-        <f>_xlfn.CONCAT(B74:N74)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('30','8','5','4','32');</v>
       </c>
     </row>
@@ -6913,7 +6911,7 @@
         <v>7</v>
       </c>
       <c r="P75" t="str">
-        <f>_xlfn.CONCAT(B75:N75)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('31','8','1','6','3600');</v>
       </c>
     </row>
@@ -6958,7 +6956,7 @@
         <v>7</v>
       </c>
       <c r="P76" t="str">
-        <f>_xlfn.CONCAT(B76:N76)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('32','8',NULL,'7','16-17-17-35');</v>
       </c>
     </row>
@@ -7003,7 +7001,7 @@
         <v>7</v>
       </c>
       <c r="P77" t="str">
-        <f>_xlfn.CONCAT(B77:N77)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('33','8','7','8','1,2');</v>
       </c>
     </row>
@@ -7048,7 +7046,7 @@
         <v>7</v>
       </c>
       <c r="P78" t="str">
-        <f>_xlfn.CONCAT(B78:N78)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('34','9',NULL,'2','Toshiba ');</v>
       </c>
     </row>
@@ -7093,7 +7091,7 @@
         <v>7</v>
       </c>
       <c r="P79" t="str">
-        <f>_xlfn.CONCAT(B79:N79)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('35','9',NULL,'1','HDD');</v>
       </c>
     </row>
@@ -7138,7 +7136,7 @@
         <v>7</v>
       </c>
       <c r="P80" t="str">
-        <f>_xlfn.CONCAT(B80:N80)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('36','9','19','3','7200');</v>
       </c>
     </row>
@@ -7183,7 +7181,7 @@
         <v>7</v>
       </c>
       <c r="P81" t="str">
-        <f>_xlfn.CONCAT(B81:N81)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('37','9','6','4','3');</v>
       </c>
     </row>
@@ -7228,7 +7226,7 @@
         <v>7</v>
       </c>
       <c r="P82" t="str">
-        <f>_xlfn.CONCAT(B82:N82)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('38','9',NULL,'11','SATA 6 Gb/s');</v>
       </c>
     </row>
@@ -7273,7 +7271,7 @@
         <v>7</v>
       </c>
       <c r="P83" t="str">
-        <f>_xlfn.CONCAT(B83:N83)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('39','10',NULL,'2','Samsung ');</v>
       </c>
     </row>
@@ -7318,7 +7316,7 @@
         <v>7</v>
       </c>
       <c r="P84" t="str">
-        <f>_xlfn.CONCAT(B84:N84)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('40','10',NULL,'1','SDD');</v>
       </c>
     </row>
@@ -7363,7 +7361,7 @@
         <v>7</v>
       </c>
       <c r="P85" t="str">
-        <f>_xlfn.CONCAT(B85:N85)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('41','10','21','3','2500');</v>
       </c>
     </row>
@@ -7408,7 +7406,7 @@
         <v>7</v>
       </c>
       <c r="P86" t="str">
-        <f>_xlfn.CONCAT(B86:N86)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('42','10','5','4','250');</v>
       </c>
     </row>
@@ -7453,7 +7451,7 @@
         <v>7</v>
       </c>
       <c r="P87" t="str">
-        <f>_xlfn.CONCAT(B87:N87)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('43','10',NULL,'11','PCIe 3.0 x4');</v>
       </c>
     </row>
@@ -7498,7 +7496,7 @@
         <v>7</v>
       </c>
       <c r="P88" t="str">
-        <f>_xlfn.CONCAT(B88:N88)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('44','11',NULL,'2','EVGA ');</v>
       </c>
     </row>
@@ -7543,7 +7541,7 @@
         <v>7</v>
       </c>
       <c r="P89" t="str">
-        <f>_xlfn.CONCAT(B89:N89)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('45','11',NULL,'1','Modular');</v>
       </c>
     </row>
@@ -7588,7 +7586,7 @@
         <v>7</v>
       </c>
       <c r="P90" t="str">
-        <f>_xlfn.CONCAT(B90:N90)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('46','11',NULL,'5','1x 24-pin, 1x 8-pin (CPU)');</v>
       </c>
     </row>
@@ -7633,7 +7631,7 @@
         <v>7</v>
       </c>
       <c r="P91" t="str">
-        <f>_xlfn.CONCAT(B91:N91)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('47','12',NULL,'2','Seasonic  ');</v>
       </c>
     </row>
@@ -7678,7 +7676,7 @@
         <v>7</v>
       </c>
       <c r="P92" t="str">
-        <f>_xlfn.CONCAT(B92:N92)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('48','12',NULL,'1','Semi-Modular');</v>
       </c>
     </row>
@@ -7723,7 +7721,7 @@
         <v>7</v>
       </c>
       <c r="P93" t="str">
-        <f>_xlfn.CONCAT(B93:N93)</f>
+        <f t="shared" si="8"/>
         <v>insert into refcarac values ('49','12',NULL,'5','4x PCIe 8-pin');</v>
       </c>
     </row>
@@ -7864,15 +7862,15 @@
       </c>
       <c r="J100" s="1"/>
       <c r="K100" t="s">
+        <v>222</v>
+      </c>
+      <c r="M100" t="s">
         <v>211</v>
       </c>
       <c r="P100" s="1"/>
-      <c r="Q100" t="s">
-        <v>212</v>
-      </c>
       <c r="R100" s="1"/>
       <c r="S100" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" spans="2:25" x14ac:dyDescent="0.25">
@@ -7913,13 +7911,13 @@
         <v>10</v>
       </c>
       <c r="N101" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O101" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P101" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q101">
         <v>2023</v>
@@ -7934,11 +7932,11 @@
         <v>7</v>
       </c>
       <c r="U101" t="str">
-        <f>_xlfn.CONCAT(B101:T101)</f>
+        <f t="shared" ref="U101:U148" si="9">_xlfn.CONCAT(B101:T101)</f>
         <v>insert into  inventario values ('1',NULL,'1','1','10/06/2023','40');</v>
       </c>
       <c r="Y101">
-        <f>S101/10</f>
+        <f t="shared" ref="Y101:Y120" si="10">S101/10</f>
         <v>4</v>
       </c>
     </row>
@@ -7980,13 +7978,13 @@
         <v>11</v>
       </c>
       <c r="N102" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O102" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P102" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q102">
         <v>2023</v>
@@ -8001,11 +7999,11 @@
         <v>7</v>
       </c>
       <c r="U102" t="str">
-        <f>_xlfn.CONCAT(B102:T102)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('2',NULL,'2','1','11/06/2023','42');</v>
       </c>
       <c r="Y102">
-        <f>S102/10</f>
+        <f t="shared" si="10"/>
         <v>4.2</v>
       </c>
     </row>
@@ -8047,13 +8045,13 @@
         <v>12</v>
       </c>
       <c r="N103" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O103" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P103" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q103">
         <v>2023</v>
@@ -8068,11 +8066,11 @@
         <v>7</v>
       </c>
       <c r="U103" t="str">
-        <f>_xlfn.CONCAT(B103:T103)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('3',NULL,'4','1','12/06/2023','41');</v>
       </c>
       <c r="Y103">
-        <f>S103/10</f>
+        <f t="shared" si="10"/>
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -8114,13 +8112,13 @@
         <v>13</v>
       </c>
       <c r="N104" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O104" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P104" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q104">
         <v>2023</v>
@@ -8135,11 +8133,11 @@
         <v>7</v>
       </c>
       <c r="U104" t="str">
-        <f>_xlfn.CONCAT(B104:T104)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('4',NULL,'5','1','13/06/2023','40');</v>
       </c>
       <c r="Y104">
-        <f>S104/10</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
@@ -8181,13 +8179,13 @@
         <v>14</v>
       </c>
       <c r="N105" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O105" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P105" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q105">
         <v>2023</v>
@@ -8202,11 +8200,11 @@
         <v>7</v>
       </c>
       <c r="U105" t="str">
-        <f>_xlfn.CONCAT(B105:T105)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('5',NULL,'6','2','14/06/2023','35');</v>
       </c>
       <c r="Y105">
-        <f>S105/10</f>
+        <f t="shared" si="10"/>
         <v>3.5</v>
       </c>
     </row>
@@ -8248,13 +8246,13 @@
         <v>15</v>
       </c>
       <c r="N106" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O106" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P106" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q106">
         <v>2023</v>
@@ -8269,11 +8267,11 @@
         <v>7</v>
       </c>
       <c r="U106" t="str">
-        <f>_xlfn.CONCAT(B106:T106)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('6',NULL,'1','2','15/06/2023','37');</v>
       </c>
       <c r="Y106">
-        <f>S106/10</f>
+        <f t="shared" si="10"/>
         <v>3.7</v>
       </c>
     </row>
@@ -8315,13 +8313,13 @@
         <v>16</v>
       </c>
       <c r="N107" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O107" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P107" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q107">
         <v>2023</v>
@@ -8336,11 +8334,11 @@
         <v>7</v>
       </c>
       <c r="U107" t="str">
-        <f>_xlfn.CONCAT(B107:T107)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('7',NULL,'2','2','16/06/2023','36');</v>
       </c>
       <c r="Y107">
-        <f>S107/10</f>
+        <f t="shared" si="10"/>
         <v>3.6</v>
       </c>
     </row>
@@ -8382,13 +8380,13 @@
         <v>17</v>
       </c>
       <c r="N108" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O108" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P108" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q108">
         <v>2023</v>
@@ -8403,11 +8401,11 @@
         <v>7</v>
       </c>
       <c r="U108" t="str">
-        <f>_xlfn.CONCAT(B108:T108)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('8',NULL,'4','2','17/06/2023','35');</v>
       </c>
       <c r="Y108">
-        <f>S108/10</f>
+        <f t="shared" si="10"/>
         <v>3.5</v>
       </c>
     </row>
@@ -8449,13 +8447,13 @@
         <v>18</v>
       </c>
       <c r="N109" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O109" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P109" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q109">
         <v>2023</v>
@@ -8470,11 +8468,11 @@
         <v>7</v>
       </c>
       <c r="U109" t="str">
-        <f>_xlfn.CONCAT(B109:T109)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('9',NULL,'5','3','18/06/2023','55');</v>
       </c>
       <c r="Y109">
-        <f>S109/10</f>
+        <f t="shared" si="10"/>
         <v>5.5</v>
       </c>
     </row>
@@ -8516,13 +8514,13 @@
         <v>19</v>
       </c>
       <c r="N110" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O110" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P110" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q110">
         <v>2023</v>
@@ -8537,11 +8535,11 @@
         <v>7</v>
       </c>
       <c r="U110" t="str">
-        <f>_xlfn.CONCAT(B110:T110)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('10',NULL,'6','3','19/06/2023','57');</v>
       </c>
       <c r="Y110">
-        <f>S110/10</f>
+        <f t="shared" si="10"/>
         <v>5.7</v>
       </c>
     </row>
@@ -8583,13 +8581,13 @@
         <v>20</v>
       </c>
       <c r="N111" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O111" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P111" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q111">
         <v>2023</v>
@@ -8604,11 +8602,11 @@
         <v>7</v>
       </c>
       <c r="U111" t="str">
-        <f>_xlfn.CONCAT(B111:T111)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('11',NULL,'1','3','20/06/2023','56');</v>
       </c>
       <c r="Y111">
-        <f>S111/10</f>
+        <f t="shared" si="10"/>
         <v>5.6</v>
       </c>
     </row>
@@ -8650,14 +8648,14 @@
         <v>10</v>
       </c>
       <c r="N112" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O112">
         <f>O101+1</f>
         <v>7</v>
       </c>
       <c r="P112" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q112">
         <v>2023</v>
@@ -8672,11 +8670,11 @@
         <v>7</v>
       </c>
       <c r="U112" t="str">
-        <f>_xlfn.CONCAT(B112:T112)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('12',NULL,'1','3','10/7/2023','55');</v>
       </c>
       <c r="Y112">
-        <f>S112/10</f>
+        <f t="shared" si="10"/>
         <v>5.5</v>
       </c>
     </row>
@@ -8709,7 +8707,7 @@
         <v>6</v>
       </c>
       <c r="K113">
-        <f t="shared" ref="K113:K148" si="5">K109+1</f>
+        <f t="shared" ref="K113:K148" si="11">K109+1</f>
         <v>4</v>
       </c>
       <c r="L113" s="1" t="s">
@@ -8719,14 +8717,14 @@
         <v>11</v>
       </c>
       <c r="N113" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O113">
-        <f t="shared" ref="O113:O148" si="6">O102+1</f>
+        <f t="shared" ref="O113:O148" si="12">O102+1</f>
         <v>7</v>
       </c>
       <c r="P113" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q113">
         <v>2023</v>
@@ -8741,11 +8739,11 @@
         <v>7</v>
       </c>
       <c r="U113" t="str">
-        <f>_xlfn.CONCAT(B113:T113)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('13',NULL,'2','4','11/7/2023','80');</v>
       </c>
       <c r="Y113">
-        <f>S113/10</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
     </row>
@@ -8778,7 +8776,7 @@
         <v>6</v>
       </c>
       <c r="K114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="L114" s="1" t="s">
@@ -8788,14 +8786,14 @@
         <v>12</v>
       </c>
       <c r="N114" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P114" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q114">
         <v>2023</v>
@@ -8810,11 +8808,11 @@
         <v>7</v>
       </c>
       <c r="U114" t="str">
-        <f>_xlfn.CONCAT(B114:T114)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('14',NULL,'4','4','12/7/2023','84');</v>
       </c>
       <c r="Y114">
-        <f>S114/10</f>
+        <f t="shared" si="10"/>
         <v>8.4</v>
       </c>
     </row>
@@ -8847,7 +8845,7 @@
         <v>6</v>
       </c>
       <c r="K115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="L115" s="1" t="s">
@@ -8857,14 +8855,14 @@
         <v>13</v>
       </c>
       <c r="N115" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P115" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q115">
         <v>2023</v>
@@ -8879,11 +8877,11 @@
         <v>7</v>
       </c>
       <c r="U115" t="str">
-        <f>_xlfn.CONCAT(B115:T115)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('15',NULL,'5','4','13/7/2023','82');</v>
       </c>
       <c r="Y115">
-        <f>S115/10</f>
+        <f t="shared" si="10"/>
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -8916,7 +8914,7 @@
         <v>6</v>
       </c>
       <c r="K116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="L116" s="1" t="s">
@@ -8926,14 +8924,14 @@
         <v>14</v>
       </c>
       <c r="N116" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P116" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q116">
         <v>2023</v>
@@ -8948,11 +8946,11 @@
         <v>7</v>
       </c>
       <c r="U116" t="str">
-        <f>_xlfn.CONCAT(B116:T116)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('16',NULL,'6','4','14/7/2023','80');</v>
       </c>
       <c r="Y116">
-        <f>S116/10</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
     </row>
@@ -8985,7 +8983,7 @@
         <v>6</v>
       </c>
       <c r="K117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="L117" s="1" t="s">
@@ -8995,14 +8993,14 @@
         <v>15</v>
       </c>
       <c r="N117" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P117" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q117">
         <v>2023</v>
@@ -9017,11 +9015,11 @@
         <v>7</v>
       </c>
       <c r="U117" t="str">
-        <f>_xlfn.CONCAT(B117:T117)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('17',NULL,'1','5','15/7/2023','70');</v>
       </c>
       <c r="Y117">
-        <f>S117/10</f>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
     </row>
@@ -9054,7 +9052,7 @@
         <v>6</v>
       </c>
       <c r="K118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="L118" s="1" t="s">
@@ -9064,14 +9062,14 @@
         <v>16</v>
       </c>
       <c r="N118" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P118" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q118">
         <v>2023</v>
@@ -9086,11 +9084,11 @@
         <v>7</v>
       </c>
       <c r="U118" t="str">
-        <f>_xlfn.CONCAT(B118:T118)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('18',NULL,'2','5','16/7/2023','74');</v>
       </c>
       <c r="Y118">
-        <f>S118/10</f>
+        <f t="shared" si="10"/>
         <v>7.4</v>
       </c>
     </row>
@@ -9123,7 +9121,7 @@
         <v>6</v>
       </c>
       <c r="K119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="L119" s="1" t="s">
@@ -9133,14 +9131,14 @@
         <v>17</v>
       </c>
       <c r="N119" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P119" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q119">
         <v>2023</v>
@@ -9155,11 +9153,11 @@
         <v>7</v>
       </c>
       <c r="U119" t="str">
-        <f>_xlfn.CONCAT(B119:T119)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('19',NULL,'4','5','17/7/2023','72');</v>
       </c>
       <c r="Y119">
-        <f>S119/10</f>
+        <f t="shared" si="10"/>
         <v>7.2</v>
       </c>
     </row>
@@ -9192,7 +9190,7 @@
         <v>6</v>
       </c>
       <c r="K120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="L120" s="1" t="s">
@@ -9202,14 +9200,14 @@
         <v>18</v>
       </c>
       <c r="N120" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P120" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q120">
         <v>2023</v>
@@ -9224,11 +9222,11 @@
         <v>7</v>
       </c>
       <c r="U120" t="str">
-        <f>_xlfn.CONCAT(B120:T120)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('20',NULL,'5','5','18/7/2023','70');</v>
       </c>
       <c r="Y120">
-        <f>S120/10</f>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
     </row>
@@ -9261,7 +9259,7 @@
         <v>6</v>
       </c>
       <c r="K121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="L121" s="1" t="s">
@@ -9271,14 +9269,14 @@
         <v>19</v>
       </c>
       <c r="N121" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P121" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q121">
         <v>2023</v>
@@ -9293,7 +9291,7 @@
         <v>7</v>
       </c>
       <c r="U121" t="str">
-        <f>_xlfn.CONCAT(B121:T121)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('21',NULL,'6','6','19/7/2023','11');</v>
       </c>
       <c r="Y121">
@@ -9330,7 +9328,7 @@
         <v>6</v>
       </c>
       <c r="K122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="L122" s="1" t="s">
@@ -9340,14 +9338,14 @@
         <v>20</v>
       </c>
       <c r="N122" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="P122" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q122">
         <v>2023</v>
@@ -9362,7 +9360,7 @@
         <v>7</v>
       </c>
       <c r="U122" t="str">
-        <f>_xlfn.CONCAT(B122:T122)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('22',NULL,'1','6','20/7/2023','11');</v>
       </c>
       <c r="Y122">
@@ -9398,7 +9396,7 @@
         <v>6</v>
       </c>
       <c r="K123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="L123" s="1" t="s">
@@ -9408,14 +9406,14 @@
         <v>10</v>
       </c>
       <c r="N123" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P123" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q123">
         <v>2023</v>
@@ -9430,7 +9428,7 @@
         <v>7</v>
       </c>
       <c r="U123" t="str">
-        <f>_xlfn.CONCAT(B123:T123)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('23',NULL,'1','6','10/8/2023','11');</v>
       </c>
       <c r="Y123">
@@ -9466,7 +9464,7 @@
         <v>6</v>
       </c>
       <c r="K124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="L124" s="1" t="s">
@@ -9476,14 +9474,14 @@
         <v>11</v>
       </c>
       <c r="N124" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P124" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q124">
         <v>2023</v>
@@ -9498,7 +9496,7 @@
         <v>7</v>
       </c>
       <c r="U124" t="str">
-        <f>_xlfn.CONCAT(B124:T124)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('24',NULL,'2','6','11/8/2023','11');</v>
       </c>
       <c r="Y124">
@@ -9535,7 +9533,7 @@
         <v>6</v>
       </c>
       <c r="K125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="L125" s="1" t="s">
@@ -9545,14 +9543,14 @@
         <v>12</v>
       </c>
       <c r="N125" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P125" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q125">
         <v>2023</v>
@@ -9567,7 +9565,7 @@
         <v>7</v>
       </c>
       <c r="U125" t="str">
-        <f>_xlfn.CONCAT(B125:T125)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('25',NULL,'4','7','12/8/2023','20');</v>
       </c>
       <c r="Y125">
@@ -9604,7 +9602,7 @@
         <v>6</v>
       </c>
       <c r="K126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="L126" s="1" t="s">
@@ -9614,14 +9612,14 @@
         <v>13</v>
       </c>
       <c r="N126" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P126" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q126">
         <v>2023</v>
@@ -9636,7 +9634,7 @@
         <v>7</v>
       </c>
       <c r="U126" t="str">
-        <f>_xlfn.CONCAT(B126:T126)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('26',NULL,'5','7','13/8/2023','21');</v>
       </c>
       <c r="Y126">
@@ -9673,7 +9671,7 @@
         <v>6</v>
       </c>
       <c r="K127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="L127" s="1" t="s">
@@ -9683,14 +9681,14 @@
         <v>14</v>
       </c>
       <c r="N127" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P127" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q127">
         <v>2023</v>
@@ -9705,7 +9703,7 @@
         <v>7</v>
       </c>
       <c r="U127" t="str">
-        <f>_xlfn.CONCAT(B127:T127)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('27',NULL,'6','7','14/8/2023','20');</v>
       </c>
       <c r="Y127">
@@ -9741,7 +9739,7 @@
         <v>6</v>
       </c>
       <c r="K128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="L128" s="1" t="s">
@@ -9751,14 +9749,14 @@
         <v>15</v>
       </c>
       <c r="N128" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P128" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q128">
         <v>2023</v>
@@ -9773,7 +9771,7 @@
         <v>7</v>
       </c>
       <c r="U128" t="str">
-        <f>_xlfn.CONCAT(B128:T128)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('28',NULL,'1','7','15/8/2023','20');</v>
       </c>
       <c r="Y128">
@@ -9810,7 +9808,7 @@
         <v>6</v>
       </c>
       <c r="K129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="L129" s="1" t="s">
@@ -9820,14 +9818,14 @@
         <v>16</v>
       </c>
       <c r="N129" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P129" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q129">
         <v>2023</v>
@@ -9842,7 +9840,7 @@
         <v>7</v>
       </c>
       <c r="U129" t="str">
-        <f>_xlfn.CONCAT(B129:T129)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('29',NULL,'2','8','16/8/2023','17');</v>
       </c>
       <c r="Y129">
@@ -9878,7 +9876,7 @@
         <v>6</v>
       </c>
       <c r="K130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="L130" s="1" t="s">
@@ -9888,14 +9886,14 @@
         <v>17</v>
       </c>
       <c r="N130" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O130">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P130" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q130">
         <v>2023</v>
@@ -9910,7 +9908,7 @@
         <v>7</v>
       </c>
       <c r="U130" t="str">
-        <f>_xlfn.CONCAT(B130:T130)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('30',NULL,'4','8','17/8/2023','18');</v>
       </c>
       <c r="Y130">
@@ -9946,7 +9944,7 @@
         <v>6</v>
       </c>
       <c r="K131">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="L131" s="1" t="s">
@@ -9956,14 +9954,14 @@
         <v>18</v>
       </c>
       <c r="N131" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O131">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P131" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q131">
         <v>2023</v>
@@ -9978,7 +9976,7 @@
         <v>7</v>
       </c>
       <c r="U131" t="str">
-        <f>_xlfn.CONCAT(B131:T131)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('31',NULL,'5','8','18/8/2023','18');</v>
       </c>
       <c r="Y131">
@@ -10015,7 +10013,7 @@
         <v>6</v>
       </c>
       <c r="K132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="L132" s="1" t="s">
@@ -10025,14 +10023,14 @@
         <v>19</v>
       </c>
       <c r="N132" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O132">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P132" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q132">
         <v>2023</v>
@@ -10047,7 +10045,7 @@
         <v>7</v>
       </c>
       <c r="U132" t="str">
-        <f>_xlfn.CONCAT(B132:T132)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('32',NULL,'6','8','19/8/2023','17');</v>
       </c>
       <c r="Y132">
@@ -10083,7 +10081,7 @@
         <v>6</v>
       </c>
       <c r="K133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="L133" s="1" t="s">
@@ -10093,14 +10091,14 @@
         <v>20</v>
       </c>
       <c r="N133" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O133">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="P133" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q133">
         <v>2023</v>
@@ -10115,7 +10113,7 @@
         <v>7</v>
       </c>
       <c r="U133" t="str">
-        <f>_xlfn.CONCAT(B133:T133)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('33',NULL,'1','9','20/8/2023','20');</v>
       </c>
       <c r="Y133">
@@ -10152,7 +10150,7 @@
         <v>6</v>
       </c>
       <c r="K134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="L134" s="1" t="s">
@@ -10162,14 +10160,14 @@
         <v>10</v>
       </c>
       <c r="N134" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O134">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P134" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q134">
         <v>2023</v>
@@ -10184,7 +10182,7 @@
         <v>7</v>
       </c>
       <c r="U134" t="str">
-        <f>_xlfn.CONCAT(B134:T134)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('34',NULL,'1','9','10/9/2023','21');</v>
       </c>
       <c r="Y134">
@@ -10221,7 +10219,7 @@
         <v>6</v>
       </c>
       <c r="K135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="L135" s="1" t="s">
@@ -10231,14 +10229,14 @@
         <v>11</v>
       </c>
       <c r="N135" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O135">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P135" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q135">
         <v>2023</v>
@@ -10253,7 +10251,7 @@
         <v>7</v>
       </c>
       <c r="U135" t="str">
-        <f>_xlfn.CONCAT(B135:T135)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('35',NULL,'2','9','11/9/2023','20');</v>
       </c>
       <c r="Y135">
@@ -10289,7 +10287,7 @@
         <v>6</v>
       </c>
       <c r="K136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="L136" s="1" t="s">
@@ -10299,14 +10297,14 @@
         <v>12</v>
       </c>
       <c r="N136" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O136">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P136" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q136">
         <v>2023</v>
@@ -10321,7 +10319,7 @@
         <v>7</v>
       </c>
       <c r="U136" t="str">
-        <f>_xlfn.CONCAT(B136:T136)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('36',NULL,'4','9','12/9/2023','20');</v>
       </c>
       <c r="Y136">
@@ -10358,7 +10356,7 @@
         <v>6</v>
       </c>
       <c r="K137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="L137" s="1" t="s">
@@ -10368,14 +10366,14 @@
         <v>13</v>
       </c>
       <c r="N137" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O137">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P137" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q137">
         <v>2023</v>
@@ -10390,7 +10388,7 @@
         <v>7</v>
       </c>
       <c r="U137" t="str">
-        <f>_xlfn.CONCAT(B137:T137)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('37',NULL,'5','10','13/9/2023','17');</v>
       </c>
       <c r="Y137">
@@ -10426,7 +10424,7 @@
         <v>6</v>
       </c>
       <c r="K138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="L138" s="1" t="s">
@@ -10436,14 +10434,14 @@
         <v>14</v>
       </c>
       <c r="N138" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O138">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P138" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q138">
         <v>2023</v>
@@ -10458,7 +10456,7 @@
         <v>7</v>
       </c>
       <c r="U138" t="str">
-        <f>_xlfn.CONCAT(B138:T138)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('38',NULL,'6','10','14/9/2023','18');</v>
       </c>
       <c r="Y138">
@@ -10494,7 +10492,7 @@
         <v>6</v>
       </c>
       <c r="K139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="L139" s="1" t="s">
@@ -10504,14 +10502,14 @@
         <v>15</v>
       </c>
       <c r="N139" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O139">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P139" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q139">
         <v>2023</v>
@@ -10526,7 +10524,7 @@
         <v>7</v>
       </c>
       <c r="U139" t="str">
-        <f>_xlfn.CONCAT(B139:T139)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('39',NULL,'1','10','15/9/2023','18');</v>
       </c>
       <c r="Y139">
@@ -10562,7 +10560,7 @@
         <v>6</v>
       </c>
       <c r="K140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="L140" s="1" t="s">
@@ -10572,14 +10570,14 @@
         <v>16</v>
       </c>
       <c r="N140" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O140">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P140" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q140">
         <v>2023</v>
@@ -10594,7 +10592,7 @@
         <v>7</v>
       </c>
       <c r="U140" t="str">
-        <f>_xlfn.CONCAT(B140:T140)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('40',NULL,'2','10','16/9/2023','17');</v>
       </c>
       <c r="Y140">
@@ -10630,7 +10628,7 @@
         <v>6</v>
       </c>
       <c r="K141">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="L141" s="1" t="s">
@@ -10640,14 +10638,14 @@
         <v>17</v>
       </c>
       <c r="N141" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O141">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P141" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q141">
         <v>2023</v>
@@ -10662,11 +10660,11 @@
         <v>7</v>
       </c>
       <c r="U141" t="str">
-        <f>_xlfn.CONCAT(B141:T141)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('41',NULL,'4','11','17/9/2023','18');</v>
       </c>
       <c r="Y141">
-        <f>S141/10</f>
+        <f t="shared" ref="Y141:Y148" si="13">S141/10</f>
         <v>1.8</v>
       </c>
     </row>
@@ -10699,7 +10697,7 @@
         <v>6</v>
       </c>
       <c r="K142">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="L142" s="1" t="s">
@@ -10709,14 +10707,14 @@
         <v>18</v>
       </c>
       <c r="N142" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O142">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P142" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q142">
         <v>2023</v>
@@ -10731,11 +10729,11 @@
         <v>7</v>
       </c>
       <c r="U142" t="str">
-        <f>_xlfn.CONCAT(B142:T142)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('42',NULL,'5','11','18/9/2023','23');</v>
       </c>
       <c r="Y142">
-        <f>S142/10</f>
+        <f t="shared" si="13"/>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -10768,7 +10766,7 @@
         <v>6</v>
       </c>
       <c r="K143">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="L143" s="1" t="s">
@@ -10778,14 +10776,14 @@
         <v>19</v>
       </c>
       <c r="N143" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O143">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P143" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q143">
         <v>2023</v>
@@ -10800,11 +10798,11 @@
         <v>7</v>
       </c>
       <c r="U143" t="str">
-        <f>_xlfn.CONCAT(B143:T143)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('43',NULL,'6','11','19/9/2023','18');</v>
       </c>
       <c r="Y143">
-        <f>S143/10</f>
+        <f t="shared" si="13"/>
         <v>1.8</v>
       </c>
     </row>
@@ -10837,7 +10835,7 @@
         <v>6</v>
       </c>
       <c r="K144">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="L144" s="1" t="s">
@@ -10847,14 +10845,14 @@
         <v>20</v>
       </c>
       <c r="N144" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O144">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="P144" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q144">
         <v>2023</v>
@@ -10869,11 +10867,11 @@
         <v>7</v>
       </c>
       <c r="U144" t="str">
-        <f>_xlfn.CONCAT(B144:T144)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('44',NULL,'1','11','20/9/2023','17');</v>
       </c>
       <c r="Y144">
-        <f>S144/10</f>
+        <f t="shared" si="13"/>
         <v>1.7</v>
       </c>
     </row>
@@ -10906,7 +10904,7 @@
         <v>6</v>
       </c>
       <c r="K145">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="L145" s="1" t="s">
@@ -10916,14 +10914,14 @@
         <v>10</v>
       </c>
       <c r="N145" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O145">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="P145" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q145">
         <v>2023</v>
@@ -10938,11 +10936,11 @@
         <v>7</v>
       </c>
       <c r="U145" t="str">
-        <f>_xlfn.CONCAT(B145:T145)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('45',NULL,'1','12','10/10/2023','25');</v>
       </c>
       <c r="Y145">
-        <f>S145/10</f>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
     </row>
@@ -10975,7 +10973,7 @@
         <v>6</v>
       </c>
       <c r="K146">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="L146" s="1" t="s">
@@ -10985,14 +10983,14 @@
         <v>11</v>
       </c>
       <c r="N146" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O146">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="P146" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q146">
         <v>2023</v>
@@ -11007,11 +11005,11 @@
         <v>7</v>
       </c>
       <c r="U146" t="str">
-        <f>_xlfn.CONCAT(B146:T146)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('46',NULL,'2','12','11/10/2023','18');</v>
       </c>
       <c r="Y146">
-        <f>S146/10</f>
+        <f t="shared" si="13"/>
         <v>1.8</v>
       </c>
     </row>
@@ -11044,7 +11042,7 @@
         <v>6</v>
       </c>
       <c r="K147">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="L147" s="1" t="s">
@@ -11054,14 +11052,14 @@
         <v>12</v>
       </c>
       <c r="N147" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O147">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="P147" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q147">
         <v>2023</v>
@@ -11076,11 +11074,11 @@
         <v>7</v>
       </c>
       <c r="U147" t="str">
-        <f>_xlfn.CONCAT(B147:T147)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('47',NULL,'4','12','12/10/2023','15');</v>
       </c>
       <c r="Y147">
-        <f>S147/10</f>
+        <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
     </row>
@@ -11113,7 +11111,7 @@
         <v>6</v>
       </c>
       <c r="K148">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="L148" s="1" t="s">
@@ -11123,14 +11121,14 @@
         <v>13</v>
       </c>
       <c r="N148" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O148">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="P148" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="Q148">
         <v>2023</v>
@@ -11145,17 +11143,17 @@
         <v>7</v>
       </c>
       <c r="U148" t="str">
-        <f>_xlfn.CONCAT(B148:T148)</f>
+        <f t="shared" si="9"/>
         <v>insert into  inventario values ('48',NULL,'5','12','13/10/2023','30');</v>
       </c>
       <c r="Y148">
-        <f>S148/10</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
     </row>
     <row r="150" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="2:25" x14ac:dyDescent="0.25">
@@ -11163,7 +11161,7 @@
         <v>206</v>
       </c>
       <c r="C151" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D151" t="s">
         <v>9</v>
@@ -11175,41 +11173,39 @@
         <v>6</v>
       </c>
       <c r="G151">
+        <v>301</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M151">
+        <v>13</v>
+      </c>
+      <c r="N151" t="s">
+        <v>212</v>
+      </c>
+      <c r="O151">
         <f>O140+1</f>
         <v>10</v>
       </c>
-      <c r="H151" t="s">
-        <v>215</v>
-      </c>
-      <c r="I151">
-        <v>13</v>
-      </c>
-      <c r="J151" t="s">
-        <v>215</v>
-      </c>
-      <c r="K151">
+      <c r="P151" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q151">
         <v>2023</v>
       </c>
-      <c r="L151" s="1" t="s">
+      <c r="R151" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="M151" t="s">
-        <v>219</v>
-      </c>
-      <c r="N151" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="O151">
-        <v>301</v>
-      </c>
-      <c r="P151" s="1"/>
-      <c r="R151" s="1"/>
+      <c r="S151" t="s">
+        <v>216</v>
+      </c>
       <c r="T151" s="1" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="U151" t="str">
         <f>_xlfn.CONCAT(B151:T151)</f>
-        <v>insert into  ensamble values ('1','10/13/2023',true,'301');</v>
+        <v>insert into  ensamble values ('1','301','13/10/2023',true);</v>
       </c>
     </row>
     <row r="152" spans="2:25" x14ac:dyDescent="0.25">
@@ -11217,7 +11213,7 @@
         <v>206</v>
       </c>
       <c r="C152" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D152" t="s">
         <v>9</v>
@@ -11226,44 +11222,42 @@
         <v>2</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G152">
+        <v>96</v>
+      </c>
+      <c r="G152" t="s">
+        <v>163</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M152">
+        <v>14</v>
+      </c>
+      <c r="N152" t="s">
+        <v>212</v>
+      </c>
+      <c r="O152">
         <f>O141+1</f>
         <v>10</v>
       </c>
-      <c r="H152" t="s">
+      <c r="P152" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q152">
+        <v>2023</v>
+      </c>
+      <c r="R152" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S152" t="s">
         <v>215</v>
       </c>
-      <c r="I152">
-        <v>14</v>
-      </c>
-      <c r="J152" t="s">
-        <v>215</v>
-      </c>
-      <c r="K152">
-        <v>2023</v>
-      </c>
-      <c r="L152" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M152" t="s">
-        <v>218</v>
-      </c>
-      <c r="N152" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="O152" t="s">
-        <v>163</v>
-      </c>
-      <c r="P152" s="1"/>
-      <c r="R152" s="1"/>
       <c r="T152" s="1" t="s">
         <v>121</v>
       </c>
       <c r="U152" t="str">
         <f>_xlfn.CONCAT(B152:T152)</f>
-        <v>insert into  ensamble values ('2','10/14/2023',false,NULL);</v>
+        <v>insert into  ensamble values ('2',NULL,' 14/10/2023',false);</v>
       </c>
     </row>
     <row r="153" spans="2:25" x14ac:dyDescent="0.25">
@@ -11271,7 +11265,7 @@
         <v>206</v>
       </c>
       <c r="C153" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D153" t="s">
         <v>9</v>
@@ -11280,44 +11274,42 @@
         <v>3</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G153">
+        <v>96</v>
+      </c>
+      <c r="G153" t="s">
+        <v>163</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M153">
+        <v>15</v>
+      </c>
+      <c r="N153" t="s">
+        <v>212</v>
+      </c>
+      <c r="O153">
         <f>O142+1</f>
         <v>10</v>
       </c>
-      <c r="H153" t="s">
+      <c r="P153" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q153">
+        <v>2023</v>
+      </c>
+      <c r="R153" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S153" t="s">
         <v>215</v>
       </c>
-      <c r="I153">
-        <v>15</v>
-      </c>
-      <c r="J153" t="s">
-        <v>215</v>
-      </c>
-      <c r="K153">
-        <v>2023</v>
-      </c>
-      <c r="L153" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M153" t="s">
-        <v>218</v>
-      </c>
-      <c r="N153" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="O153" t="s">
-        <v>163</v>
-      </c>
-      <c r="P153" s="1"/>
-      <c r="R153" s="1"/>
       <c r="T153" s="1" t="s">
         <v>121</v>
       </c>
       <c r="U153" t="str">
         <f>_xlfn.CONCAT(B153:T153)</f>
-        <v>insert into  ensamble values ('3','10/15/2023',false,NULL);</v>
+        <v>insert into  ensamble values ('3',NULL,'15/10/2023',false);</v>
       </c>
     </row>
     <row r="154" spans="2:25" x14ac:dyDescent="0.25">
@@ -11331,7 +11323,6 @@
     <row r="155" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F155" s="1"/>
       <c r="L155" s="1"/>
-      <c r="N155" s="1"/>
       <c r="P155" s="1"/>
       <c r="R155" s="1"/>
       <c r="T155" s="1"/>
@@ -11341,13 +11332,13 @@
     </row>
     <row r="157" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E157" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G157" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I157" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="T157" s="1"/>
     </row>
@@ -11356,7 +11347,7 @@
         <v>206</v>
       </c>
       <c r="C158" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D158" t="s">
         <v>9</v>
@@ -11376,12 +11367,20 @@
       <c r="I158">
         <v>1</v>
       </c>
+      <c r="J158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K158">
+        <f>K101</f>
+        <v>1</v>
+      </c>
+      <c r="O158" s="6"/>
       <c r="T158" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U158" t="str">
-        <f>_xlfn.CONCAT(B158:T158)</f>
-        <v>insert into  detalleensamble values ('1','1','1');</v>
+        <f t="shared" ref="U158:U172" si="14">_xlfn.CONCAT(B158:T158)</f>
+        <v>insert into  detalleensamble values ('1','1','1','1');</v>
       </c>
     </row>
     <row r="159" spans="2:25" x14ac:dyDescent="0.25">
@@ -11389,7 +11388,7 @@
         <v>206</v>
       </c>
       <c r="C159" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D159" t="s">
         <v>9</v>
@@ -11409,12 +11408,19 @@
       <c r="I159">
         <v>5</v>
       </c>
+      <c r="J159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K159">
+        <f>K105</f>
+        <v>2</v>
+      </c>
       <c r="T159" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U159" t="str">
-        <f>_xlfn.CONCAT(B159:T159)</f>
-        <v>insert into  detalleensamble values ('2','1','5');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('2','1','5','2');</v>
       </c>
     </row>
     <row r="160" spans="2:25" x14ac:dyDescent="0.25">
@@ -11422,7 +11428,7 @@
         <v>206</v>
       </c>
       <c r="C160" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D160" t="s">
         <v>9</v>
@@ -11442,12 +11448,19 @@
       <c r="I160">
         <v>9</v>
       </c>
+      <c r="J160" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K160">
+        <f>K109</f>
+        <v>3</v>
+      </c>
       <c r="T160" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U160" t="str">
-        <f>_xlfn.CONCAT(B160:T160)</f>
-        <v>insert into  detalleensamble values ('3','1','9');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('3','1','9','3');</v>
       </c>
     </row>
     <row r="161" spans="2:21" x14ac:dyDescent="0.25">
@@ -11455,7 +11468,7 @@
         <v>206</v>
       </c>
       <c r="C161" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D161" t="s">
         <v>9</v>
@@ -11475,12 +11488,19 @@
       <c r="I161">
         <v>13</v>
       </c>
+      <c r="J161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K161">
+        <f>K113</f>
+        <v>4</v>
+      </c>
       <c r="T161" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U161" t="str">
-        <f>_xlfn.CONCAT(B161:T161)</f>
-        <v>insert into  detalleensamble values ('4','1','13');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('4','1','13','4');</v>
       </c>
     </row>
     <row r="162" spans="2:21" x14ac:dyDescent="0.25">
@@ -11488,7 +11508,7 @@
         <v>206</v>
       </c>
       <c r="C162" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D162" t="s">
         <v>9</v>
@@ -11508,12 +11528,19 @@
       <c r="I162">
         <v>17</v>
       </c>
+      <c r="J162" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K162">
+        <f>K117</f>
+        <v>5</v>
+      </c>
       <c r="T162" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U162" t="str">
-        <f>_xlfn.CONCAT(B162:T162)</f>
-        <v>insert into  detalleensamble values ('5','1','17');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('5','1','17','5');</v>
       </c>
     </row>
     <row r="163" spans="2:21" x14ac:dyDescent="0.25">
@@ -11521,7 +11548,7 @@
         <v>206</v>
       </c>
       <c r="C163" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D163" t="s">
         <v>9</v>
@@ -11542,12 +11569,19 @@
       <c r="I163">
         <v>21</v>
       </c>
+      <c r="J163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K163">
+        <f>K121</f>
+        <v>6</v>
+      </c>
       <c r="T163" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U163" t="str">
-        <f>_xlfn.CONCAT(B163:T163)</f>
-        <v>insert into  detalleensamble values ('6','2','21');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('6','2','21','6');</v>
       </c>
     </row>
     <row r="164" spans="2:21" x14ac:dyDescent="0.25">
@@ -11555,7 +11589,7 @@
         <v>206</v>
       </c>
       <c r="C164" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D164" t="s">
         <v>9</v>
@@ -11567,7 +11601,7 @@
         <v>6</v>
       </c>
       <c r="G164">
-        <f t="shared" ref="G164:G172" si="7">G159+1</f>
+        <f t="shared" ref="G164:G172" si="15">G159+1</f>
         <v>2</v>
       </c>
       <c r="H164" s="1" t="s">
@@ -11576,12 +11610,19 @@
       <c r="I164">
         <v>25</v>
       </c>
+      <c r="J164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K164">
+        <f>K125</f>
+        <v>7</v>
+      </c>
       <c r="T164" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U164" t="str">
-        <f>_xlfn.CONCAT(B164:T164)</f>
-        <v>insert into  detalleensamble values ('7','2','25');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('7','2','25','7');</v>
       </c>
     </row>
     <row r="165" spans="2:21" x14ac:dyDescent="0.25">
@@ -11589,7 +11630,7 @@
         <v>206</v>
       </c>
       <c r="C165" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D165" t="s">
         <v>9</v>
@@ -11601,7 +11642,7 @@
         <v>6</v>
       </c>
       <c r="G165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="H165" s="1" t="s">
@@ -11610,12 +11651,19 @@
       <c r="I165">
         <v>29</v>
       </c>
+      <c r="J165" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K165">
+        <f>K129</f>
+        <v>8</v>
+      </c>
       <c r="T165" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U165" t="str">
-        <f>_xlfn.CONCAT(B165:T165)</f>
-        <v>insert into  detalleensamble values ('8','2','29');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('8','2','29','8');</v>
       </c>
     </row>
     <row r="166" spans="2:21" x14ac:dyDescent="0.25">
@@ -11623,7 +11671,7 @@
         <v>206</v>
       </c>
       <c r="C166" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D166" t="s">
         <v>9</v>
@@ -11635,7 +11683,7 @@
         <v>6</v>
       </c>
       <c r="G166">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="H166" s="1" t="s">
@@ -11644,12 +11692,19 @@
       <c r="I166">
         <v>33</v>
       </c>
+      <c r="J166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K166">
+        <f>K133</f>
+        <v>9</v>
+      </c>
       <c r="T166" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U166" t="str">
-        <f>_xlfn.CONCAT(B166:T166)</f>
-        <v>insert into  detalleensamble values ('9','2','33');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('9','2','33','9');</v>
       </c>
     </row>
     <row r="167" spans="2:21" x14ac:dyDescent="0.25">
@@ -11657,7 +11712,7 @@
         <v>206</v>
       </c>
       <c r="C167" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D167" t="s">
         <v>9</v>
@@ -11669,7 +11724,7 @@
         <v>6</v>
       </c>
       <c r="G167">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="H167" s="1" t="s">
@@ -11678,12 +11733,19 @@
       <c r="I167">
         <v>37</v>
       </c>
+      <c r="J167" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K167">
+        <f>K137</f>
+        <v>10</v>
+      </c>
       <c r="T167" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U167" t="str">
-        <f>_xlfn.CONCAT(B167:T167)</f>
-        <v>insert into  detalleensamble values ('10','2','37');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('10','2','37','10');</v>
       </c>
     </row>
     <row r="168" spans="2:21" x14ac:dyDescent="0.25">
@@ -11691,7 +11753,7 @@
         <v>206</v>
       </c>
       <c r="C168" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D168" t="s">
         <v>9</v>
@@ -11703,7 +11765,7 @@
         <v>6</v>
       </c>
       <c r="G168">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="H168" s="1" t="s">
@@ -11712,12 +11774,19 @@
       <c r="I168">
         <v>41</v>
       </c>
+      <c r="J168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K168">
+        <f>K141</f>
+        <v>11</v>
+      </c>
       <c r="T168" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U168" t="str">
-        <f>_xlfn.CONCAT(B168:T168)</f>
-        <v>insert into  detalleensamble values ('11','3','41');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('11','3','41','11');</v>
       </c>
     </row>
     <row r="169" spans="2:21" x14ac:dyDescent="0.25">
@@ -11725,7 +11794,7 @@
         <v>206</v>
       </c>
       <c r="C169" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D169" t="s">
         <v>9</v>
@@ -11737,7 +11806,7 @@
         <v>6</v>
       </c>
       <c r="G169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="H169" s="1" t="s">
@@ -11746,12 +11815,19 @@
       <c r="I169">
         <v>45</v>
       </c>
+      <c r="J169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K169">
+        <f>K145</f>
+        <v>12</v>
+      </c>
       <c r="T169" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U169" t="str">
-        <f>_xlfn.CONCAT(B169:T169)</f>
-        <v>insert into  detalleensamble values ('12','3','45');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('12','3','45','12');</v>
       </c>
     </row>
     <row r="170" spans="2:21" x14ac:dyDescent="0.25">
@@ -11759,7 +11835,7 @@
         <v>206</v>
       </c>
       <c r="C170" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D170" t="s">
         <v>9</v>
@@ -11771,7 +11847,7 @@
         <v>6</v>
       </c>
       <c r="G170">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="H170" s="1" t="s">
@@ -11780,12 +11856,19 @@
       <c r="I170">
         <v>2</v>
       </c>
+      <c r="J170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K170">
+        <f>K102</f>
+        <v>1</v>
+      </c>
       <c r="T170" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U170" t="str">
-        <f>_xlfn.CONCAT(B170:T170)</f>
-        <v>insert into  detalleensamble values ('13','3','2');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('13','3','2','1');</v>
       </c>
     </row>
     <row r="171" spans="2:21" x14ac:dyDescent="0.25">
@@ -11793,7 +11876,7 @@
         <v>206</v>
       </c>
       <c r="C171" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D171" t="s">
         <v>9</v>
@@ -11805,7 +11888,7 @@
         <v>6</v>
       </c>
       <c r="G171">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="H171" s="1" t="s">
@@ -11814,12 +11897,19 @@
       <c r="I171">
         <v>6</v>
       </c>
+      <c r="J171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K171">
+        <f>K105</f>
+        <v>2</v>
+      </c>
       <c r="T171" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U171" t="str">
-        <f>_xlfn.CONCAT(B171:T171)</f>
-        <v>insert into  detalleensamble values ('14','3','6');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('14','3','6','2');</v>
       </c>
     </row>
     <row r="172" spans="2:21" x14ac:dyDescent="0.25">
@@ -11827,7 +11917,7 @@
         <v>206</v>
       </c>
       <c r="C172" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D172" t="s">
         <v>9</v>
@@ -11839,7 +11929,7 @@
         <v>6</v>
       </c>
       <c r="G172">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="H172" s="1" t="s">
@@ -11848,12 +11938,19 @@
       <c r="I172">
         <v>10</v>
       </c>
+      <c r="J172" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K172">
+        <f>K110</f>
+        <v>3</v>
+      </c>
       <c r="T172" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U172" t="str">
-        <f>_xlfn.CONCAT(B172:T172)</f>
-        <v>insert into  detalleensamble values ('15','3','10');</v>
+        <f t="shared" si="14"/>
+        <v>insert into  detalleensamble values ('15','3','10','3');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>